<commit_message>
changed comparison sheet and snapshots
</commit_message>
<xml_diff>
--- a/TechWatchJSFrameworkComparison.xlsx
+++ b/TechWatchJSFrameworkComparison.xlsx
@@ -1209,28 +1209,55 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1238,33 +1265,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1561,22 +1561,22 @@
                   <c:v>4.14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.18</c:v>
+                  <c:v>4.21</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.6</c:v>
+                  <c:v>3.42</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.85</c:v>
+                  <c:v>3.7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.63</c:v>
+                  <c:v>3.23</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.24</c:v>
+                  <c:v>2.54</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1596,11 +1596,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2127443496"/>
-        <c:axId val="2127434072"/>
+        <c:axId val="-2138445240"/>
+        <c:axId val="-2138441736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2127443496"/>
+        <c:axId val="-2138445240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1610,12 +1610,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127434072"/>
+        <c:crossAx val="-2138441736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2127434072"/>
+        <c:axId val="-2138441736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1626,7 +1626,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127443496"/>
+        <c:crossAx val="-2138445240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1668,7 +1668,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1980,7 +1980,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1990,9 +1990,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H58" sqref="H58"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N59" sqref="N59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2671,31 +2671,31 @@
       <c r="E22" s="16"/>
       <c r="F22" s="65"/>
       <c r="G22" s="21">
-        <f>AVERAGE(G4:G21)</f>
+        <f t="shared" ref="G22:M22" si="0">AVERAGE(G4:G21)</f>
         <v>4.2777777777777777</v>
       </c>
       <c r="H22" s="21">
-        <f>AVERAGE(H4:H21)</f>
+        <f t="shared" si="0"/>
         <v>4.4444444444444446</v>
       </c>
       <c r="I22" s="21">
-        <f>AVERAGE(I4:I21)</f>
+        <f t="shared" si="0"/>
         <v>4.2222222222222223</v>
       </c>
       <c r="J22" s="21">
-        <f>AVERAGE(J4:J21)</f>
+        <f t="shared" si="0"/>
         <v>4.5555555555555554</v>
       </c>
       <c r="K22" s="21">
-        <f>AVERAGE(K4:K21)</f>
+        <f t="shared" si="0"/>
         <v>3.3333333333333335</v>
       </c>
       <c r="L22" s="21">
-        <f>AVERAGE(L4:L21)</f>
+        <f t="shared" si="0"/>
         <v>3.6666666666666665</v>
       </c>
       <c r="M22" s="22">
-        <f>AVERAGE(M4:M21)</f>
+        <f t="shared" si="0"/>
         <v>2.2777777777777777</v>
       </c>
     </row>
@@ -2895,124 +2895,124 @@
       <c r="M29" s="86"/>
     </row>
     <row r="30" spans="1:13" ht="30">
-      <c r="A30" s="122">
+      <c r="A30" s="110">
         <v>5</v>
       </c>
       <c r="B30" s="119" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="109" t="s">
+      <c r="C30" s="114" t="s">
         <v>50</v>
       </c>
       <c r="D30" s="67" t="s">
         <v>51</v>
       </c>
-      <c r="E30" s="109" t="s">
+      <c r="E30" s="114" t="s">
         <v>52</v>
       </c>
-      <c r="F30" s="112"/>
-      <c r="G30" s="114">
+      <c r="F30" s="116"/>
+      <c r="G30" s="108">
         <v>4</v>
       </c>
       <c r="H30" s="103"/>
-      <c r="I30" s="114">
+      <c r="I30" s="108">
         <v>2</v>
       </c>
-      <c r="J30" s="114">
+      <c r="J30" s="108">
         <v>0</v>
       </c>
-      <c r="K30" s="114">
-        <v>3</v>
-      </c>
-      <c r="L30" s="114">
-        <v>4</v>
-      </c>
-      <c r="M30" s="114">
+      <c r="K30" s="108">
+        <v>3</v>
+      </c>
+      <c r="L30" s="108">
+        <v>4</v>
+      </c>
+      <c r="M30" s="108">
         <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:13">
-      <c r="A31" s="122"/>
+      <c r="A31" s="110"/>
       <c r="B31" s="119"/>
-      <c r="C31" s="109"/>
+      <c r="C31" s="114"/>
       <c r="D31" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E31" s="109"/>
-      <c r="F31" s="112"/>
-      <c r="G31" s="114"/>
+      <c r="E31" s="114"/>
+      <c r="F31" s="116"/>
+      <c r="G31" s="108"/>
       <c r="H31" s="103"/>
-      <c r="I31" s="114"/>
-      <c r="J31" s="114"/>
-      <c r="K31" s="114"/>
-      <c r="L31" s="114"/>
-      <c r="M31" s="114"/>
+      <c r="I31" s="108"/>
+      <c r="J31" s="108"/>
+      <c r="K31" s="108"/>
+      <c r="L31" s="108"/>
+      <c r="M31" s="108"/>
     </row>
     <row r="32" spans="1:13">
-      <c r="A32" s="122"/>
+      <c r="A32" s="110"/>
       <c r="B32" s="119"/>
-      <c r="C32" s="109"/>
+      <c r="C32" s="114"/>
       <c r="D32" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E32" s="109"/>
-      <c r="F32" s="112"/>
-      <c r="G32" s="114"/>
+      <c r="E32" s="114"/>
+      <c r="F32" s="116"/>
+      <c r="G32" s="108"/>
       <c r="H32" s="103"/>
-      <c r="I32" s="114"/>
-      <c r="J32" s="114"/>
-      <c r="K32" s="114"/>
-      <c r="L32" s="114"/>
-      <c r="M32" s="114"/>
+      <c r="I32" s="108"/>
+      <c r="J32" s="108"/>
+      <c r="K32" s="108"/>
+      <c r="L32" s="108"/>
+      <c r="M32" s="108"/>
     </row>
     <row r="33" spans="1:13" ht="30">
-      <c r="A33" s="122"/>
+      <c r="A33" s="110"/>
       <c r="B33" s="119"/>
-      <c r="C33" s="109"/>
+      <c r="C33" s="114"/>
       <c r="D33" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E33" s="109"/>
-      <c r="F33" s="112"/>
-      <c r="G33" s="114"/>
+      <c r="E33" s="114"/>
+      <c r="F33" s="116"/>
+      <c r="G33" s="108"/>
       <c r="H33" s="103"/>
-      <c r="I33" s="114"/>
-      <c r="J33" s="114"/>
-      <c r="K33" s="114"/>
-      <c r="L33" s="114"/>
-      <c r="M33" s="114"/>
+      <c r="I33" s="108"/>
+      <c r="J33" s="108"/>
+      <c r="K33" s="108"/>
+      <c r="L33" s="108"/>
+      <c r="M33" s="108"/>
     </row>
     <row r="34" spans="1:13" s="4" customFormat="1" ht="18">
-      <c r="A34" s="122"/>
+      <c r="A34" s="110"/>
       <c r="B34" s="119"/>
-      <c r="C34" s="109"/>
+      <c r="C34" s="114"/>
       <c r="D34" s="9"/>
-      <c r="E34" s="109"/>
-      <c r="F34" s="112"/>
-      <c r="G34" s="114"/>
+      <c r="E34" s="114"/>
+      <c r="F34" s="116"/>
+      <c r="G34" s="108"/>
       <c r="H34" s="103"/>
-      <c r="I34" s="114"/>
-      <c r="J34" s="114"/>
-      <c r="K34" s="114"/>
-      <c r="L34" s="114"/>
-      <c r="M34" s="114"/>
+      <c r="I34" s="108"/>
+      <c r="J34" s="108"/>
+      <c r="K34" s="108"/>
+      <c r="L34" s="108"/>
+      <c r="M34" s="108"/>
     </row>
     <row r="35" spans="1:13" ht="45">
-      <c r="A35" s="122"/>
+      <c r="A35" s="110"/>
       <c r="B35" s="119"/>
-      <c r="C35" s="109"/>
+      <c r="C35" s="114"/>
       <c r="D35" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="E35" s="110"/>
-      <c r="F35" s="113"/>
-      <c r="G35" s="115"/>
+      <c r="E35" s="115"/>
+      <c r="F35" s="117"/>
+      <c r="G35" s="109"/>
       <c r="H35" s="104"/>
-      <c r="I35" s="115"/>
-      <c r="J35" s="115"/>
-      <c r="K35" s="115"/>
-      <c r="L35" s="115"/>
-      <c r="M35" s="115"/>
+      <c r="I35" s="109"/>
+      <c r="J35" s="109"/>
+      <c r="K35" s="109"/>
+      <c r="L35" s="109"/>
+      <c r="M35" s="109"/>
     </row>
     <row r="36" spans="1:13" ht="30">
       <c r="A36" s="59"/>
@@ -3027,13 +3027,13 @@
         <v>4</v>
       </c>
       <c r="H36" s="105">
-        <v>4</v>
+        <v>4.2</v>
       </c>
       <c r="I36" s="65">
         <v>2</v>
       </c>
       <c r="J36" s="105">
-        <v>2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="K36" s="65">
         <v>5</v>
@@ -3058,13 +3058,13 @@
         <v>4</v>
       </c>
       <c r="H37" s="105">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I37" s="65">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J37" s="105">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K37" s="65">
         <v>2</v>
@@ -3089,26 +3089,26 @@
       </c>
       <c r="H38" s="21">
         <f>AVERAGE(H35:H37)</f>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I38" s="21">
+        <f t="shared" ref="I38:M38" si="1">AVERAGE(I35:I37)</f>
+        <v>3</v>
+      </c>
+      <c r="J38" s="21">
+        <f t="shared" si="1"/>
+        <v>3.1</v>
+      </c>
+      <c r="K38" s="21">
+        <f t="shared" si="1"/>
         <v>3.5</v>
       </c>
-      <c r="I38" s="21">
-        <f t="shared" ref="I38:M38" si="0">AVERAGE(I35:I37)</f>
-        <v>2.5</v>
-      </c>
-      <c r="J38" s="21">
-        <f t="shared" si="0"/>
-        <v>2.5</v>
-      </c>
-      <c r="K38" s="21">
-        <f t="shared" si="0"/>
-        <v>3.5</v>
-      </c>
       <c r="L38" s="21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="M38" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -3127,15 +3127,15 @@
       </c>
       <c r="H39" s="26">
         <f>H38 * F39 / 100</f>
-        <v>0.875</v>
+        <v>1.0249999999999999</v>
       </c>
       <c r="I39" s="26">
         <f>I38 * F39 / 100</f>
-        <v>0.625</v>
+        <v>0.75</v>
       </c>
       <c r="J39" s="26">
         <f>J38 * F39 / 100</f>
-        <v>0.625</v>
+        <v>0.77500000000000002</v>
       </c>
       <c r="K39" s="26">
         <f>K38 * F39 / 100</f>
@@ -3308,13 +3308,13 @@
       <c r="M45" s="13"/>
     </row>
     <row r="46" spans="1:13" s="4" customFormat="1" ht="76">
-      <c r="A46" s="122">
+      <c r="A46" s="110">
         <v>9</v>
       </c>
-      <c r="B46" s="125" t="s">
+      <c r="B46" s="112" t="s">
         <v>71</v>
       </c>
-      <c r="C46" s="109" t="s">
+      <c r="C46" s="114" t="s">
         <v>72</v>
       </c>
       <c r="D46" s="67" t="s">
@@ -3323,147 +3323,147 @@
       <c r="E46" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="F46" s="112"/>
-      <c r="G46" s="114">
+      <c r="F46" s="116"/>
+      <c r="G46" s="108">
         <v>4</v>
       </c>
       <c r="H46" s="103"/>
-      <c r="I46" s="114">
+      <c r="I46" s="108">
         <v>5</v>
       </c>
       <c r="J46" s="103"/>
-      <c r="K46" s="114">
+      <c r="K46" s="108">
         <v>2</v>
       </c>
-      <c r="L46" s="114">
-        <v>3</v>
-      </c>
-      <c r="M46" s="114">
+      <c r="L46" s="108">
+        <v>3</v>
+      </c>
+      <c r="M46" s="108">
         <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="135">
-      <c r="A47" s="122"/>
-      <c r="B47" s="125"/>
-      <c r="C47" s="109"/>
+      <c r="A47" s="110"/>
+      <c r="B47" s="112"/>
+      <c r="C47" s="114"/>
       <c r="D47" s="9" t="s">
         <v>75</v>
       </c>
       <c r="E47" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="F47" s="112"/>
-      <c r="G47" s="114"/>
+      <c r="F47" s="116"/>
+      <c r="G47" s="108"/>
       <c r="H47" s="103"/>
-      <c r="I47" s="114"/>
+      <c r="I47" s="108"/>
       <c r="J47" s="103"/>
-      <c r="K47" s="114"/>
-      <c r="L47" s="114"/>
-      <c r="M47" s="114"/>
+      <c r="K47" s="108"/>
+      <c r="L47" s="108"/>
+      <c r="M47" s="108"/>
     </row>
     <row r="48" spans="1:13" s="4" customFormat="1" ht="18">
-      <c r="A48" s="122"/>
-      <c r="B48" s="125"/>
-      <c r="C48" s="109"/>
+      <c r="A48" s="110"/>
+      <c r="B48" s="112"/>
+      <c r="C48" s="114"/>
       <c r="D48" s="9" t="s">
         <v>77</v>
       </c>
       <c r="E48" s="17"/>
-      <c r="F48" s="112"/>
-      <c r="G48" s="114"/>
+      <c r="F48" s="116"/>
+      <c r="G48" s="108"/>
       <c r="H48" s="103"/>
-      <c r="I48" s="114"/>
+      <c r="I48" s="108"/>
       <c r="J48" s="103"/>
-      <c r="K48" s="114"/>
-      <c r="L48" s="114"/>
-      <c r="M48" s="114"/>
+      <c r="K48" s="108"/>
+      <c r="L48" s="108"/>
+      <c r="M48" s="108"/>
     </row>
     <row r="49" spans="1:13">
-      <c r="A49" s="122"/>
-      <c r="B49" s="125"/>
-      <c r="C49" s="109"/>
+      <c r="A49" s="110"/>
+      <c r="B49" s="112"/>
+      <c r="C49" s="114"/>
       <c r="D49" s="10"/>
       <c r="E49" s="17"/>
-      <c r="F49" s="112"/>
-      <c r="G49" s="114"/>
+      <c r="F49" s="116"/>
+      <c r="G49" s="108"/>
       <c r="H49" s="103"/>
-      <c r="I49" s="114"/>
+      <c r="I49" s="108"/>
       <c r="J49" s="103"/>
-      <c r="K49" s="114"/>
-      <c r="L49" s="114"/>
-      <c r="M49" s="114"/>
+      <c r="K49" s="108"/>
+      <c r="L49" s="108"/>
+      <c r="M49" s="108"/>
     </row>
     <row r="50" spans="1:13" s="4" customFormat="1" ht="18">
-      <c r="A50" s="122"/>
-      <c r="B50" s="125"/>
-      <c r="C50" s="109"/>
+      <c r="A50" s="110"/>
+      <c r="B50" s="112"/>
+      <c r="C50" s="114"/>
       <c r="D50" s="9" t="s">
         <v>78</v>
       </c>
       <c r="E50" s="17"/>
-      <c r="F50" s="112"/>
-      <c r="G50" s="114"/>
+      <c r="F50" s="116"/>
+      <c r="G50" s="108"/>
       <c r="H50" s="103"/>
-      <c r="I50" s="114"/>
+      <c r="I50" s="108"/>
       <c r="J50" s="103"/>
-      <c r="K50" s="114"/>
-      <c r="L50" s="114"/>
-      <c r="M50" s="114"/>
+      <c r="K50" s="108"/>
+      <c r="L50" s="108"/>
+      <c r="M50" s="108"/>
     </row>
     <row r="51" spans="1:13" ht="30">
-      <c r="A51" s="122"/>
-      <c r="B51" s="125"/>
-      <c r="C51" s="109"/>
+      <c r="A51" s="110"/>
+      <c r="B51" s="112"/>
+      <c r="C51" s="114"/>
       <c r="D51" s="9" t="s">
         <v>79</v>
       </c>
       <c r="E51" s="17"/>
-      <c r="F51" s="112"/>
-      <c r="G51" s="114"/>
+      <c r="F51" s="116"/>
+      <c r="G51" s="108"/>
       <c r="H51" s="103"/>
-      <c r="I51" s="114"/>
+      <c r="I51" s="108"/>
       <c r="J51" s="103"/>
-      <c r="K51" s="114"/>
-      <c r="L51" s="114"/>
-      <c r="M51" s="114"/>
+      <c r="K51" s="108"/>
+      <c r="L51" s="108"/>
+      <c r="M51" s="108"/>
     </row>
     <row r="52" spans="1:13" s="6" customFormat="1" ht="45">
-      <c r="A52" s="122"/>
-      <c r="B52" s="125"/>
-      <c r="C52" s="109"/>
+      <c r="A52" s="110"/>
+      <c r="B52" s="112"/>
+      <c r="C52" s="114"/>
       <c r="D52" s="9" t="s">
         <v>80</v>
       </c>
       <c r="E52" s="17"/>
-      <c r="F52" s="112"/>
-      <c r="G52" s="114"/>
+      <c r="F52" s="116"/>
+      <c r="G52" s="108"/>
       <c r="H52" s="103"/>
-      <c r="I52" s="114"/>
+      <c r="I52" s="108"/>
       <c r="J52" s="103"/>
-      <c r="K52" s="114"/>
-      <c r="L52" s="114"/>
-      <c r="M52" s="114"/>
+      <c r="K52" s="108"/>
+      <c r="L52" s="108"/>
+      <c r="M52" s="108"/>
     </row>
     <row r="53" spans="1:13" ht="75">
-      <c r="A53" s="123"/>
-      <c r="B53" s="126"/>
-      <c r="C53" s="110"/>
+      <c r="A53" s="111"/>
+      <c r="B53" s="113"/>
+      <c r="C53" s="115"/>
       <c r="D53" s="67" t="s">
         <v>81</v>
       </c>
       <c r="E53" s="17"/>
-      <c r="F53" s="113"/>
-      <c r="G53" s="115"/>
+      <c r="F53" s="117"/>
+      <c r="G53" s="109"/>
       <c r="H53" s="104">
         <v>4</v>
       </c>
-      <c r="I53" s="115"/>
+      <c r="I53" s="109"/>
       <c r="J53" s="104">
         <v>5</v>
       </c>
-      <c r="K53" s="115"/>
-      <c r="L53" s="115"/>
-      <c r="M53" s="115"/>
+      <c r="K53" s="109"/>
+      <c r="L53" s="109"/>
+      <c r="M53" s="109"/>
     </row>
     <row r="54" spans="1:13" ht="18">
       <c r="A54" s="47"/>
@@ -3507,91 +3507,91 @@
       <c r="A55" s="121">
         <v>10</v>
       </c>
-      <c r="B55" s="124" t="s">
+      <c r="B55" s="122" t="s">
         <v>82</v>
       </c>
-      <c r="C55" s="108" t="s">
+      <c r="C55" s="123" t="s">
         <v>83</v>
       </c>
       <c r="D55" s="67" t="s">
         <v>84</v>
       </c>
-      <c r="E55" s="108" t="s">
+      <c r="E55" s="123" t="s">
         <v>85</v>
       </c>
-      <c r="F55" s="111"/>
+      <c r="F55" s="124"/>
       <c r="G55" s="118">
         <v>4</v>
       </c>
       <c r="H55" s="106"/>
       <c r="I55" s="118">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J55" s="106"/>
       <c r="K55" s="118">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L55" s="118">
         <v>5</v>
       </c>
       <c r="M55" s="118">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:13">
-      <c r="A56" s="122"/>
-      <c r="B56" s="125"/>
-      <c r="C56" s="109"/>
+      <c r="A56" s="110"/>
+      <c r="B56" s="112"/>
+      <c r="C56" s="114"/>
       <c r="D56" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="E56" s="109"/>
-      <c r="F56" s="112"/>
-      <c r="G56" s="114"/>
+      <c r="E56" s="114"/>
+      <c r="F56" s="116"/>
+      <c r="G56" s="108"/>
       <c r="H56" s="103"/>
-      <c r="I56" s="114"/>
+      <c r="I56" s="108"/>
       <c r="J56" s="103"/>
-      <c r="K56" s="114"/>
-      <c r="L56" s="114"/>
-      <c r="M56" s="114"/>
+      <c r="K56" s="108"/>
+      <c r="L56" s="108"/>
+      <c r="M56" s="108"/>
     </row>
     <row r="57" spans="1:13" ht="30">
-      <c r="A57" s="122"/>
-      <c r="B57" s="125"/>
-      <c r="C57" s="109"/>
+      <c r="A57" s="110"/>
+      <c r="B57" s="112"/>
+      <c r="C57" s="114"/>
       <c r="D57" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="E57" s="109"/>
-      <c r="F57" s="112"/>
-      <c r="G57" s="114"/>
+      <c r="E57" s="114"/>
+      <c r="F57" s="116"/>
+      <c r="G57" s="108"/>
       <c r="H57" s="103"/>
-      <c r="I57" s="114"/>
+      <c r="I57" s="108"/>
       <c r="J57" s="103"/>
-      <c r="K57" s="114"/>
-      <c r="L57" s="114"/>
-      <c r="M57" s="114"/>
+      <c r="K57" s="108"/>
+      <c r="L57" s="108"/>
+      <c r="M57" s="108"/>
     </row>
     <row r="58" spans="1:13" ht="30">
-      <c r="A58" s="123"/>
-      <c r="B58" s="126"/>
-      <c r="C58" s="110"/>
+      <c r="A58" s="111"/>
+      <c r="B58" s="113"/>
+      <c r="C58" s="115"/>
       <c r="D58" s="44" t="s">
         <v>88</v>
       </c>
-      <c r="E58" s="110"/>
-      <c r="F58" s="113"/>
-      <c r="G58" s="115"/>
+      <c r="E58" s="115"/>
+      <c r="F58" s="117"/>
+      <c r="G58" s="109"/>
       <c r="H58" s="104">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="I58" s="115"/>
+        <v>4</v>
+      </c>
+      <c r="I58" s="109"/>
       <c r="J58" s="104">
-        <v>4</v>
-      </c>
-      <c r="K58" s="115"/>
-      <c r="L58" s="115"/>
-      <c r="M58" s="115"/>
+        <v>3</v>
+      </c>
+      <c r="K58" s="109"/>
+      <c r="L58" s="109"/>
+      <c r="M58" s="109"/>
     </row>
     <row r="59" spans="1:13" ht="18">
       <c r="A59" s="75"/>
@@ -3608,19 +3608,19 @@
       </c>
       <c r="H59" s="79">
         <f>H58 * F59 / 100</f>
-        <v>1.32</v>
+        <v>1.2</v>
       </c>
       <c r="I59" s="79">
         <f>I55 * F59 / 100</f>
-        <v>1.2</v>
+        <v>0.9</v>
       </c>
       <c r="J59" s="79">
         <f>J58 * F59 / 100</f>
-        <v>1.2</v>
+        <v>0.9</v>
       </c>
       <c r="K59" s="79">
         <f>K55 * F59 / 100</f>
-        <v>0.3</v>
+        <v>0.9</v>
       </c>
       <c r="L59" s="79">
         <f>L55 * F59 / 100</f>
@@ -3628,7 +3628,7 @@
       </c>
       <c r="M59" s="80">
         <f>M55 * F59 / 100</f>
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="60" spans="1:13">
@@ -3647,13 +3647,13 @@
       <c r="M60" s="13"/>
     </row>
     <row r="61" spans="1:13" ht="20">
-      <c r="A61" s="116" t="s">
+      <c r="A61" s="125" t="s">
         <v>89</v>
       </c>
-      <c r="B61" s="117"/>
-      <c r="C61" s="117"/>
-      <c r="D61" s="117"/>
-      <c r="E61" s="117"/>
+      <c r="B61" s="126"/>
+      <c r="C61" s="126"/>
+      <c r="D61" s="126"/>
+      <c r="E61" s="126"/>
       <c r="F61" s="81">
         <f>SUM(F59,F54,F43,F39,F25,F23)</f>
         <v>100</v>
@@ -3664,31 +3664,49 @@
       </c>
       <c r="H61" s="82">
         <f>ROUNDUP(SUM(H59,H54,H43,H39,H25,H23), 2)</f>
-        <v>4.18</v>
+        <v>4.21</v>
       </c>
       <c r="I61" s="82">
-        <f t="shared" ref="I61:M61" si="1">ROUNDUP(SUM(I59,I54,I43,I39,I25,I23), 2)</f>
-        <v>3.5999999999999996</v>
+        <f t="shared" ref="I61:M61" si="2">ROUNDUP(SUM(I59,I54,I43,I39,I25,I23), 2)</f>
+        <v>3.42</v>
       </c>
       <c r="J61" s="82">
-        <f t="shared" si="1"/>
-        <v>3.8499999999999996</v>
+        <f t="shared" si="2"/>
+        <v>3.6999999999999997</v>
       </c>
       <c r="K61" s="82">
-        <f t="shared" si="1"/>
-        <v>2.63</v>
+        <f t="shared" si="2"/>
+        <v>3.23</v>
       </c>
       <c r="L61" s="82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="M61" s="82">
-        <f t="shared" si="1"/>
-        <v>2.2399999999999998</v>
+        <f t="shared" si="2"/>
+        <v>2.5399999999999996</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="E55:E58"/>
+    <mergeCell ref="F55:F58"/>
+    <mergeCell ref="I30:I35"/>
+    <mergeCell ref="A61:E61"/>
+    <mergeCell ref="G55:G58"/>
+    <mergeCell ref="B3:B22"/>
+    <mergeCell ref="B30:B37"/>
+    <mergeCell ref="A55:A58"/>
+    <mergeCell ref="B55:B58"/>
+    <mergeCell ref="C55:C58"/>
+    <mergeCell ref="M55:M58"/>
+    <mergeCell ref="I46:I53"/>
+    <mergeCell ref="K46:K53"/>
+    <mergeCell ref="L46:L53"/>
+    <mergeCell ref="M46:M53"/>
+    <mergeCell ref="K55:K58"/>
+    <mergeCell ref="L55:L58"/>
+    <mergeCell ref="I55:I58"/>
     <mergeCell ref="K30:K35"/>
     <mergeCell ref="L30:L35"/>
     <mergeCell ref="M30:M35"/>
@@ -3703,24 +3721,6 @@
     <mergeCell ref="E30:E35"/>
     <mergeCell ref="F30:F35"/>
     <mergeCell ref="J30:J35"/>
-    <mergeCell ref="M55:M58"/>
-    <mergeCell ref="I46:I53"/>
-    <mergeCell ref="K46:K53"/>
-    <mergeCell ref="L46:L53"/>
-    <mergeCell ref="M46:M53"/>
-    <mergeCell ref="K55:K58"/>
-    <mergeCell ref="L55:L58"/>
-    <mergeCell ref="I55:I58"/>
-    <mergeCell ref="B3:B22"/>
-    <mergeCell ref="B30:B37"/>
-    <mergeCell ref="A55:A58"/>
-    <mergeCell ref="B55:B58"/>
-    <mergeCell ref="C55:C58"/>
-    <mergeCell ref="E55:E58"/>
-    <mergeCell ref="F55:F58"/>
-    <mergeCell ref="I30:I35"/>
-    <mergeCell ref="A61:E61"/>
-    <mergeCell ref="G55:G58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3736,8 +3736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3818,7 +3818,7 @@
       <c r="N2" s="69"/>
     </row>
     <row r="3" spans="1:14" ht="45" customHeight="1">
-      <c r="A3" s="122">
+      <c r="A3" s="110">
         <v>1</v>
       </c>
       <c r="B3" s="119" t="s">
@@ -3854,7 +3854,7 @@
       <c r="N3" s="58"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="122"/>
+      <c r="A4" s="110"/>
       <c r="B4" s="119"/>
       <c r="C4" s="8"/>
       <c r="D4" s="98" t="s">
@@ -3886,7 +3886,7 @@
       <c r="N4" s="58"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="122"/>
+      <c r="A5" s="110"/>
       <c r="B5" s="119"/>
       <c r="C5" s="8"/>
       <c r="D5" s="98" t="s">
@@ -3918,38 +3918,38 @@
       <c r="N5" s="58"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="122"/>
+      <c r="A6" s="110"/>
       <c r="B6" s="119"/>
       <c r="C6" s="62"/>
       <c r="D6" s="100"/>
       <c r="E6" s="97"/>
       <c r="F6" s="64"/>
       <c r="G6" s="21">
-        <f>AVERAGE(G4:G5)</f>
+        <f t="shared" ref="G6:M6" si="0">AVERAGE(G4:G5)</f>
         <v>3.5</v>
       </c>
       <c r="H6" s="21">
-        <f>AVERAGE(H4:H5)</f>
+        <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
       <c r="I6" s="21">
-        <f>AVERAGE(I4:I5)</f>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
       <c r="J6" s="21">
-        <f>AVERAGE(J4:J5)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="K6" s="21">
-        <f>AVERAGE(K4:K5)</f>
+        <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
       <c r="L6" s="21">
-        <f>AVERAGE(L4:L5)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="M6" s="22">
-        <f>AVERAGE(M4:M5)</f>
+        <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
       <c r="N6" s="58"/>
@@ -3994,7 +3994,7 @@
       <c r="N7" s="51"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="122">
+      <c r="A8" s="110">
         <v>2</v>
       </c>
       <c r="B8" s="119" t="s">
@@ -4030,7 +4030,7 @@
       <c r="N8" s="58"/>
     </row>
     <row r="9" spans="1:14" s="4" customFormat="1" ht="45">
-      <c r="A9" s="122"/>
+      <c r="A9" s="110"/>
       <c r="B9" s="119"/>
       <c r="C9" s="8"/>
       <c r="D9" s="98" t="s">
@@ -4062,7 +4062,7 @@
       <c r="N9" s="31"/>
     </row>
     <row r="10" spans="1:14" ht="30">
-      <c r="A10" s="122"/>
+      <c r="A10" s="110"/>
       <c r="B10" s="119"/>
       <c r="C10" s="8"/>
       <c r="D10" s="102" t="s">
@@ -4094,7 +4094,7 @@
       <c r="N10" s="58"/>
     </row>
     <row r="11" spans="1:14" s="5" customFormat="1">
-      <c r="A11" s="122"/>
+      <c r="A11" s="110"/>
       <c r="B11" s="119"/>
       <c r="C11" s="62"/>
       <c r="D11" s="56"/>
@@ -4264,31 +4264,31 @@
         <v>100</v>
       </c>
       <c r="G16" s="29">
-        <f>ROUNDUP(SUM(G7,G12,G14), 2)</f>
+        <f t="shared" ref="G16:M16" si="1">ROUNDUP(SUM(G7,G12,G14), 2)</f>
         <v>3.8</v>
       </c>
       <c r="H16" s="29">
-        <f>ROUNDUP(SUM(H7,H12,H14), 2)</f>
+        <f t="shared" si="1"/>
         <v>3.95</v>
       </c>
       <c r="I16" s="29">
-        <f>ROUNDUP(SUM(I7,I12,I14), 2)</f>
+        <f t="shared" si="1"/>
         <v>2.85</v>
       </c>
       <c r="J16" s="29">
-        <f>ROUNDUP(SUM(J7,J12,J14), 2)</f>
+        <f t="shared" si="1"/>
         <v>3.9</v>
       </c>
       <c r="K16" s="29">
-        <f>ROUNDUP(SUM(K7,K12,K14), 2)</f>
+        <f t="shared" si="1"/>
         <v>4.0999999999999996</v>
       </c>
       <c r="L16" s="29">
-        <f>ROUNDUP(SUM(L7,L12,L14), 2)</f>
+        <f t="shared" si="1"/>
         <v>1.95</v>
       </c>
       <c r="M16" s="29">
-        <f>ROUNDUP(SUM(M7,M12,M14), 2)</f>
+        <f t="shared" si="1"/>
         <v>4.25</v>
       </c>
       <c r="N16" s="33"/>
@@ -4316,7 +4316,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4360,7 +4360,7 @@
         <v>3.95</v>
       </c>
       <c r="C3" s="41">
-        <v>4.18</v>
+        <v>4.21</v>
       </c>
       <c r="D3" s="38"/>
       <c r="E3" s="38"/>
@@ -4375,7 +4375,7 @@
       </c>
       <c r="C4" s="41">
         <f>Capabilities!I61</f>
-        <v>3.5999999999999996</v>
+        <v>3.42</v>
       </c>
       <c r="D4" s="38"/>
       <c r="E4" s="38"/>
@@ -4388,7 +4388,7 @@
         <v>3.9</v>
       </c>
       <c r="C5" s="41">
-        <v>3.85</v>
+        <v>3.7</v>
       </c>
       <c r="D5" s="38"/>
       <c r="E5" s="38"/>
@@ -4403,7 +4403,7 @@
       </c>
       <c r="C6" s="41">
         <f>Capabilities!K61</f>
-        <v>2.63</v>
+        <v>3.23</v>
       </c>
       <c r="D6" s="38"/>
       <c r="E6" s="38"/>
@@ -4433,7 +4433,7 @@
       </c>
       <c r="C8" s="41">
         <f>Capabilities!M61</f>
-        <v>2.2399999999999998</v>
+        <v>2.5399999999999996</v>
       </c>
       <c r="D8" s="38"/>
       <c r="E8" s="38"/>

</xml_diff>

<commit_message>
Added benchmark result for vuejs
</commit_message>
<xml_diff>
--- a/TechWatchJSFrameworkComparison.xlsx
+++ b/TechWatchJSFrameworkComparison.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24709"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\githubs\TechWatchJS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14180"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14175" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Capabilities" sheetId="1" r:id="rId1"/>
     <sheet name="Adoption" sheetId="7" r:id="rId2"/>
     <sheet name="Adoption Vs Capabilities" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="105">
   <si>
     <t>S.N.</t>
   </si>
@@ -333,6 +341,9 @@
   </si>
   <si>
     <t xml:space="preserve">Number of projects in each JS </t>
+  </si>
+  <si>
+    <t>Vue.js</t>
   </si>
 </sst>
 </file>
@@ -911,7 +922,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -998,18 +1009,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1055,13 +1054,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1074,9 +1067,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1107,9 +1097,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1221,11 +1208,54 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1233,61 +1263,21 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="215">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1563,10 +1553,10 @@
                   <c:v>2.85</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.1</c:v>
+                  <c:v>4.0999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1.95</c:v>
@@ -1584,13 +1574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>4.1</c:v>
+                  <c:v>4.0999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4.18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.47</c:v>
+                  <c:v>3.4699999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>3.75</c:v>
@@ -1599,10 +1589,10 @@
                   <c:v>3.23</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.54</c:v>
+                  <c:v>2.5399999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1622,11 +1612,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2124889688"/>
-        <c:axId val="2124890056"/>
+        <c:axId val="295179456"/>
+        <c:axId val="295181024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2124889688"/>
+        <c:axId val="295179456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1636,12 +1626,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2124890056"/>
+        <c:crossAx val="295181024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2124890056"/>
+        <c:axId val="295181024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1652,7 +1642,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2124889688"/>
+        <c:crossAx val="295179456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1668,7 +1658,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1694,7 +1684,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1715,6 +1705,35 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Capabilities"/>
+      <sheetName val="Adoption"/>
+      <sheetName val="Adoption Vs Capabilities"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="61">
+          <cell r="N61">
+            <v>3.3699999999999997</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1">
+        <row r="16">
+          <cell r="N16">
+            <v>4.1500000000000004</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2006,7 +2025,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2014,74 +2033,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M61"/>
+  <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E42" sqref="E42"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5" style="37" customWidth="1"/>
-    <col min="2" max="2" width="21.1640625" style="20" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" style="33" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" style="3" customWidth="1"/>
     <col min="4" max="4" width="32" style="7" customWidth="1"/>
-    <col min="5" max="5" width="25.1640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" style="3" customWidth="1"/>
-    <col min="9" max="9" width="17.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.83203125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="13.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" style="3" customWidth="1"/>
-    <col min="13" max="13" width="17.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="10.83203125" style="3"/>
+    <col min="13" max="13" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" style="99"/>
+    <col min="15" max="16384" width="10.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="20">
-      <c r="A1" s="89" t="s">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+      <c r="A1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="90" t="s">
+      <c r="B1" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="91" t="s">
+      <c r="C1" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="92" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="91" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="91" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="93" t="s">
+      <c r="D1" s="84" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="83" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="83" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="94" t="s">
+      <c r="H1" s="86" t="s">
         <v>102</v>
       </c>
-      <c r="I1" s="94" t="s">
+      <c r="I1" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="94" t="s">
+      <c r="J1" s="86" t="s">
         <v>101</v>
       </c>
-      <c r="K1" s="94" t="s">
+      <c r="K1" s="86" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="94" t="s">
+      <c r="L1" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="95" t="s">
+      <c r="M1" s="87" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" s="35"/>
+      <c r="N1" s="87" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="31"/>
       <c r="B2" s="19"/>
       <c r="C2" s="11"/>
       <c r="D2" s="12"/>
@@ -2095,34 +2118,34 @@
       <c r="L2" s="11"/>
       <c r="M2" s="13"/>
     </row>
-    <row r="3" spans="1:13" ht="45" customHeight="1">
-      <c r="A3" s="59">
+    <row r="3" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="52">
         <v>1</v>
       </c>
-      <c r="B3" s="118" t="s">
+      <c r="B3" s="113" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="62" t="s">
+      <c r="C3" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="96" t="s">
+      <c r="D3" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="97" t="s">
+      <c r="E3" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="64"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="65"/>
-      <c r="M3" s="63"/>
-    </row>
-    <row r="4" spans="1:13" ht="30">
-      <c r="A4" s="59"/>
-      <c r="B4" s="118"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="56"/>
+    </row>
+    <row r="4" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="52"/>
+      <c r="B4" s="113"/>
       <c r="C4" s="8"/>
       <c r="D4" s="14" t="s">
         <v>15</v>
@@ -2130,32 +2153,35 @@
       <c r="E4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="64"/>
-      <c r="G4" s="65">
-        <v>5</v>
-      </c>
-      <c r="H4" s="104">
-        <v>5</v>
-      </c>
-      <c r="I4" s="65">
-        <v>5</v>
-      </c>
-      <c r="J4" s="104">
-        <v>5</v>
-      </c>
-      <c r="K4" s="65">
-        <v>5</v>
-      </c>
-      <c r="L4" s="65">
-        <v>5</v>
-      </c>
-      <c r="M4" s="63">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="59"/>
-      <c r="B5" s="118"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="58">
+        <v>5</v>
+      </c>
+      <c r="H4" s="96">
+        <v>5</v>
+      </c>
+      <c r="I4" s="58">
+        <v>5</v>
+      </c>
+      <c r="J4" s="96">
+        <v>5</v>
+      </c>
+      <c r="K4" s="58">
+        <v>5</v>
+      </c>
+      <c r="L4" s="58">
+        <v>5</v>
+      </c>
+      <c r="M4" s="56">
+        <v>3</v>
+      </c>
+      <c r="N4" s="99">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="52"/>
+      <c r="B5" s="113"/>
       <c r="C5" s="8"/>
       <c r="D5" s="14" t="s">
         <v>17</v>
@@ -2163,32 +2189,35 @@
       <c r="E5" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="64"/>
-      <c r="G5" s="65">
-        <v>5</v>
-      </c>
-      <c r="H5" s="104">
-        <v>5</v>
-      </c>
-      <c r="I5" s="65">
-        <v>5</v>
-      </c>
-      <c r="J5" s="104">
-        <v>5</v>
-      </c>
-      <c r="K5" s="65">
-        <v>4</v>
-      </c>
-      <c r="L5" s="65">
-        <v>4</v>
-      </c>
-      <c r="M5" s="63">
+      <c r="F5" s="57"/>
+      <c r="G5" s="58">
+        <v>5</v>
+      </c>
+      <c r="H5" s="96">
+        <v>5</v>
+      </c>
+      <c r="I5" s="58">
+        <v>5</v>
+      </c>
+      <c r="J5" s="96">
+        <v>5</v>
+      </c>
+      <c r="K5" s="58">
+        <v>4</v>
+      </c>
+      <c r="L5" s="58">
+        <v>4</v>
+      </c>
+      <c r="M5" s="56">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="30" customHeight="1">
-      <c r="A6" s="59"/>
-      <c r="B6" s="118"/>
+      <c r="N5" s="99">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="52"/>
+      <c r="B6" s="113"/>
       <c r="C6" s="8"/>
       <c r="D6" s="14" t="s">
         <v>19</v>
@@ -2196,32 +2225,35 @@
       <c r="E6" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="64"/>
-      <c r="G6" s="65">
-        <v>3</v>
-      </c>
-      <c r="H6" s="104">
-        <v>3</v>
-      </c>
-      <c r="I6" s="65">
-        <v>5</v>
-      </c>
-      <c r="J6" s="104">
-        <v>5</v>
-      </c>
-      <c r="K6" s="65">
-        <v>3</v>
-      </c>
-      <c r="L6" s="65">
-        <v>3</v>
-      </c>
-      <c r="M6" s="63">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="30" customHeight="1">
-      <c r="A7" s="59"/>
-      <c r="B7" s="118"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="58">
+        <v>3</v>
+      </c>
+      <c r="H6" s="96">
+        <v>3</v>
+      </c>
+      <c r="I6" s="58">
+        <v>5</v>
+      </c>
+      <c r="J6" s="96">
+        <v>5</v>
+      </c>
+      <c r="K6" s="58">
+        <v>3</v>
+      </c>
+      <c r="L6" s="58">
+        <v>3</v>
+      </c>
+      <c r="M6" s="56">
+        <v>3</v>
+      </c>
+      <c r="N6" s="99">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="52"/>
+      <c r="B7" s="113"/>
       <c r="C7" s="8"/>
       <c r="D7" s="14" t="s">
         <v>21</v>
@@ -2229,94 +2261,103 @@
       <c r="E7" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="64"/>
-      <c r="G7" s="65">
-        <v>4</v>
-      </c>
-      <c r="H7" s="104">
-        <v>4</v>
-      </c>
-      <c r="I7" s="65">
-        <v>5</v>
-      </c>
-      <c r="J7" s="104">
-        <v>5</v>
-      </c>
-      <c r="K7" s="65">
-        <v>4</v>
-      </c>
-      <c r="L7" s="65">
-        <v>4</v>
-      </c>
-      <c r="M7" s="63">
+      <c r="F7" s="57"/>
+      <c r="G7" s="58">
+        <v>4</v>
+      </c>
+      <c r="H7" s="96">
+        <v>4</v>
+      </c>
+      <c r="I7" s="58">
+        <v>5</v>
+      </c>
+      <c r="J7" s="96">
+        <v>5</v>
+      </c>
+      <c r="K7" s="58">
+        <v>4</v>
+      </c>
+      <c r="L7" s="58">
+        <v>4</v>
+      </c>
+      <c r="M7" s="56">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="59"/>
-      <c r="B8" s="118"/>
+      <c r="N7" s="99">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="52"/>
+      <c r="B8" s="113"/>
       <c r="C8" s="8"/>
       <c r="D8" s="14" t="s">
         <v>23</v>
       </c>
       <c r="E8" s="15"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="65">
-        <v>5</v>
-      </c>
-      <c r="H8" s="104">
-        <v>5</v>
-      </c>
-      <c r="I8" s="65">
-        <v>5</v>
-      </c>
-      <c r="J8" s="104">
-        <v>5</v>
-      </c>
-      <c r="K8" s="65">
-        <v>3</v>
-      </c>
-      <c r="L8" s="65">
-        <v>3</v>
-      </c>
-      <c r="M8" s="63">
+      <c r="F8" s="57"/>
+      <c r="G8" s="58">
+        <v>5</v>
+      </c>
+      <c r="H8" s="96">
+        <v>5</v>
+      </c>
+      <c r="I8" s="58">
+        <v>5</v>
+      </c>
+      <c r="J8" s="96">
+        <v>5</v>
+      </c>
+      <c r="K8" s="58">
+        <v>3</v>
+      </c>
+      <c r="L8" s="58">
+        <v>3</v>
+      </c>
+      <c r="M8" s="56">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="59"/>
-      <c r="B9" s="118"/>
+      <c r="N8" s="99">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="52"/>
+      <c r="B9" s="113"/>
       <c r="C9" s="8"/>
       <c r="D9" s="14" t="s">
         <v>24</v>
       </c>
       <c r="E9" s="15"/>
-      <c r="F9" s="64"/>
-      <c r="G9" s="65">
-        <v>5</v>
-      </c>
-      <c r="H9" s="104">
-        <v>5</v>
-      </c>
-      <c r="I9" s="65">
-        <v>5</v>
-      </c>
-      <c r="J9" s="104">
-        <v>5</v>
-      </c>
-      <c r="K9" s="65">
-        <v>5</v>
-      </c>
-      <c r="L9" s="65">
-        <v>5</v>
-      </c>
-      <c r="M9" s="63">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="30" customHeight="1">
-      <c r="A10" s="59"/>
-      <c r="B10" s="118"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="58">
+        <v>5</v>
+      </c>
+      <c r="H9" s="96">
+        <v>5</v>
+      </c>
+      <c r="I9" s="58">
+        <v>5</v>
+      </c>
+      <c r="J9" s="96">
+        <v>5</v>
+      </c>
+      <c r="K9" s="58">
+        <v>5</v>
+      </c>
+      <c r="L9" s="58">
+        <v>5</v>
+      </c>
+      <c r="M9" s="56">
+        <v>5</v>
+      </c>
+      <c r="N9" s="99">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="52"/>
+      <c r="B10" s="113"/>
       <c r="C10" s="8"/>
       <c r="D10" s="14" t="s">
         <v>25</v>
@@ -2324,32 +2365,35 @@
       <c r="E10" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="64"/>
-      <c r="G10" s="65">
-        <v>3</v>
-      </c>
-      <c r="H10" s="104">
-        <v>4</v>
-      </c>
-      <c r="I10" s="65">
-        <v>3</v>
-      </c>
-      <c r="J10" s="104">
-        <v>4</v>
-      </c>
-      <c r="K10" s="65">
+      <c r="F10" s="57"/>
+      <c r="G10" s="58">
+        <v>3</v>
+      </c>
+      <c r="H10" s="96">
+        <v>4</v>
+      </c>
+      <c r="I10" s="58">
+        <v>3</v>
+      </c>
+      <c r="J10" s="96">
+        <v>4</v>
+      </c>
+      <c r="K10" s="58">
         <v>1</v>
       </c>
-      <c r="L10" s="65">
-        <v>3</v>
-      </c>
-      <c r="M10" s="63">
+      <c r="L10" s="58">
+        <v>3</v>
+      </c>
+      <c r="M10" s="56">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" ht="45" customHeight="1">
-      <c r="A11" s="59"/>
-      <c r="B11" s="118"/>
+      <c r="N10" s="99">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="52"/>
+      <c r="B11" s="113"/>
       <c r="C11" s="8"/>
       <c r="D11" s="14" t="s">
         <v>27</v>
@@ -2357,347 +2401,380 @@
       <c r="E11" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="64"/>
-      <c r="G11" s="65">
-        <v>5</v>
-      </c>
-      <c r="H11" s="104">
-        <v>5</v>
-      </c>
-      <c r="I11" s="65">
-        <v>4</v>
-      </c>
-      <c r="J11" s="104">
-        <v>5</v>
-      </c>
-      <c r="K11" s="65">
-        <v>5</v>
-      </c>
-      <c r="L11" s="65">
-        <v>4</v>
-      </c>
-      <c r="M11" s="63">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="59"/>
-      <c r="B12" s="118"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="58">
+        <v>5</v>
+      </c>
+      <c r="H11" s="96">
+        <v>5</v>
+      </c>
+      <c r="I11" s="58">
+        <v>4</v>
+      </c>
+      <c r="J11" s="96">
+        <v>5</v>
+      </c>
+      <c r="K11" s="58">
+        <v>5</v>
+      </c>
+      <c r="L11" s="58">
+        <v>4</v>
+      </c>
+      <c r="M11" s="56">
+        <v>3</v>
+      </c>
+      <c r="N11" s="99">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="52"/>
+      <c r="B12" s="113"/>
       <c r="C12" s="8"/>
       <c r="D12" s="14" t="s">
         <v>29</v>
       </c>
       <c r="E12" s="15"/>
-      <c r="F12" s="64"/>
-      <c r="G12" s="65">
-        <v>3</v>
-      </c>
-      <c r="H12" s="104">
-        <v>4</v>
-      </c>
-      <c r="I12" s="65">
-        <v>3</v>
-      </c>
-      <c r="J12" s="104">
-        <v>5</v>
-      </c>
-      <c r="K12" s="65">
-        <v>3</v>
-      </c>
-      <c r="L12" s="65">
-        <v>3</v>
-      </c>
-      <c r="M12" s="63">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="59"/>
-      <c r="B13" s="118"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="58">
+        <v>3</v>
+      </c>
+      <c r="H12" s="96">
+        <v>4</v>
+      </c>
+      <c r="I12" s="58">
+        <v>3</v>
+      </c>
+      <c r="J12" s="96">
+        <v>5</v>
+      </c>
+      <c r="K12" s="58">
+        <v>3</v>
+      </c>
+      <c r="L12" s="58">
+        <v>3</v>
+      </c>
+      <c r="M12" s="56">
+        <v>3</v>
+      </c>
+      <c r="N12" s="99">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="52"/>
+      <c r="B13" s="113"/>
       <c r="C13" s="8"/>
       <c r="D13" s="14" t="s">
         <v>30</v>
       </c>
       <c r="E13" s="15"/>
-      <c r="F13" s="64"/>
-      <c r="G13" s="65">
-        <v>5</v>
-      </c>
-      <c r="H13" s="104">
-        <v>5</v>
-      </c>
-      <c r="I13" s="65">
-        <v>3</v>
-      </c>
-      <c r="J13" s="104">
-        <v>5</v>
-      </c>
-      <c r="K13" s="65">
-        <v>3</v>
-      </c>
-      <c r="L13" s="65">
-        <v>5</v>
-      </c>
-      <c r="M13" s="63">
+      <c r="F13" s="57"/>
+      <c r="G13" s="58">
+        <v>5</v>
+      </c>
+      <c r="H13" s="96">
+        <v>5</v>
+      </c>
+      <c r="I13" s="58">
+        <v>3</v>
+      </c>
+      <c r="J13" s="96">
+        <v>5</v>
+      </c>
+      <c r="K13" s="58">
+        <v>3</v>
+      </c>
+      <c r="L13" s="58">
+        <v>5</v>
+      </c>
+      <c r="M13" s="56">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="59"/>
-      <c r="B14" s="118"/>
+      <c r="N13" s="99">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="52"/>
+      <c r="B14" s="113"/>
       <c r="C14" s="8"/>
       <c r="D14" s="14" t="s">
         <v>31</v>
       </c>
       <c r="E14" s="15"/>
-      <c r="F14" s="64"/>
-      <c r="G14" s="65">
-        <v>5</v>
-      </c>
-      <c r="H14" s="104">
-        <v>5</v>
-      </c>
-      <c r="I14" s="65">
-        <v>5</v>
-      </c>
-      <c r="J14" s="104">
-        <v>5</v>
-      </c>
-      <c r="K14" s="65">
-        <v>3</v>
-      </c>
-      <c r="L14" s="65">
-        <v>3</v>
-      </c>
-      <c r="M14" s="63">
+      <c r="F14" s="57"/>
+      <c r="G14" s="58">
+        <v>5</v>
+      </c>
+      <c r="H14" s="96">
+        <v>5</v>
+      </c>
+      <c r="I14" s="58">
+        <v>5</v>
+      </c>
+      <c r="J14" s="96">
+        <v>5</v>
+      </c>
+      <c r="K14" s="58">
+        <v>3</v>
+      </c>
+      <c r="L14" s="58">
+        <v>3</v>
+      </c>
+      <c r="M14" s="56">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="59"/>
-      <c r="B15" s="118"/>
+      <c r="N14" s="99">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="52"/>
+      <c r="B15" s="113"/>
       <c r="C15" s="8"/>
       <c r="D15" s="14" t="s">
         <v>32</v>
       </c>
       <c r="E15" s="15"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="65">
-        <v>3</v>
-      </c>
-      <c r="H15" s="104">
-        <v>3</v>
-      </c>
-      <c r="I15" s="65">
-        <v>4</v>
-      </c>
-      <c r="J15" s="104">
-        <v>4</v>
-      </c>
-      <c r="K15" s="65">
-        <v>3</v>
-      </c>
-      <c r="L15" s="65">
-        <v>4</v>
-      </c>
-      <c r="M15" s="63">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" s="59"/>
-      <c r="B16" s="118"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="58">
+        <v>3</v>
+      </c>
+      <c r="H15" s="96">
+        <v>3</v>
+      </c>
+      <c r="I15" s="58">
+        <v>4</v>
+      </c>
+      <c r="J15" s="96">
+        <v>4</v>
+      </c>
+      <c r="K15" s="58">
+        <v>3</v>
+      </c>
+      <c r="L15" s="58">
+        <v>4</v>
+      </c>
+      <c r="M15" s="56">
+        <v>3</v>
+      </c>
+      <c r="N15" s="99">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="52"/>
+      <c r="B16" s="113"/>
       <c r="C16" s="8"/>
       <c r="D16" s="14" t="s">
         <v>33</v>
       </c>
       <c r="E16" s="15"/>
-      <c r="F16" s="64"/>
-      <c r="G16" s="65">
-        <v>5</v>
-      </c>
-      <c r="H16" s="104">
-        <v>5</v>
-      </c>
-      <c r="I16" s="65">
-        <v>5</v>
-      </c>
-      <c r="J16" s="104">
-        <v>5</v>
-      </c>
-      <c r="K16" s="65">
+      <c r="F16" s="57"/>
+      <c r="G16" s="58">
+        <v>5</v>
+      </c>
+      <c r="H16" s="96">
+        <v>5</v>
+      </c>
+      <c r="I16" s="58">
+        <v>5</v>
+      </c>
+      <c r="J16" s="96">
+        <v>5</v>
+      </c>
+      <c r="K16" s="58">
         <v>1</v>
       </c>
-      <c r="L16" s="65">
+      <c r="L16" s="58">
         <v>1</v>
       </c>
-      <c r="M16" s="63">
+      <c r="M16" s="56">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:13">
-      <c r="A17" s="59"/>
-      <c r="B17" s="118"/>
+      <c r="N16" s="99">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="52"/>
+      <c r="B17" s="113"/>
       <c r="C17" s="8"/>
       <c r="D17" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F17" s="64"/>
-      <c r="G17" s="65">
-        <v>3</v>
-      </c>
-      <c r="H17" s="104">
-        <v>4</v>
-      </c>
-      <c r="I17" s="65">
-        <v>4</v>
-      </c>
-      <c r="J17" s="104">
-        <v>4</v>
-      </c>
-      <c r="K17" s="65">
-        <v>3</v>
-      </c>
-      <c r="L17" s="65">
-        <v>5</v>
-      </c>
-      <c r="M17" s="63">
+      <c r="F17" s="57"/>
+      <c r="G17" s="58">
+        <v>3</v>
+      </c>
+      <c r="H17" s="96">
+        <v>4</v>
+      </c>
+      <c r="I17" s="58">
+        <v>4</v>
+      </c>
+      <c r="J17" s="96">
+        <v>4</v>
+      </c>
+      <c r="K17" s="58">
+        <v>3</v>
+      </c>
+      <c r="L17" s="58">
+        <v>5</v>
+      </c>
+      <c r="M17" s="56">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:13">
-      <c r="A18" s="59"/>
-      <c r="B18" s="118"/>
+      <c r="N17" s="99">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="52"/>
+      <c r="B18" s="113"/>
       <c r="C18" s="8"/>
       <c r="D18" s="14" t="s">
         <v>35</v>
       </c>
       <c r="E18" s="15"/>
-      <c r="F18" s="64"/>
-      <c r="G18" s="65">
-        <v>3</v>
-      </c>
-      <c r="H18" s="104">
-        <v>3</v>
-      </c>
-      <c r="I18" s="65">
-        <v>5</v>
-      </c>
-      <c r="J18" s="104">
-        <v>5</v>
-      </c>
-      <c r="K18" s="65">
-        <v>3</v>
-      </c>
-      <c r="L18" s="65">
-        <v>5</v>
-      </c>
-      <c r="M18" s="63">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="A19" s="59"/>
-      <c r="B19" s="118"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="58">
+        <v>3</v>
+      </c>
+      <c r="H18" s="96">
+        <v>3</v>
+      </c>
+      <c r="I18" s="58">
+        <v>5</v>
+      </c>
+      <c r="J18" s="96">
+        <v>5</v>
+      </c>
+      <c r="K18" s="58">
+        <v>3</v>
+      </c>
+      <c r="L18" s="58">
+        <v>5</v>
+      </c>
+      <c r="M18" s="56">
+        <v>3</v>
+      </c>
+      <c r="N18" s="99">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="52"/>
+      <c r="B19" s="113"/>
       <c r="C19" s="8"/>
       <c r="D19" s="14" t="s">
         <v>36</v>
       </c>
       <c r="E19" s="15"/>
-      <c r="F19" s="64"/>
-      <c r="G19" s="65">
-        <v>5</v>
-      </c>
-      <c r="H19" s="104">
-        <v>5</v>
-      </c>
-      <c r="I19" s="65">
-        <v>5</v>
-      </c>
-      <c r="J19" s="104">
-        <v>5</v>
-      </c>
-      <c r="K19" s="65">
-        <v>5</v>
-      </c>
-      <c r="L19" s="65">
+      <c r="F19" s="57"/>
+      <c r="G19" s="58">
+        <v>5</v>
+      </c>
+      <c r="H19" s="96">
+        <v>5</v>
+      </c>
+      <c r="I19" s="58">
+        <v>5</v>
+      </c>
+      <c r="J19" s="96">
+        <v>5</v>
+      </c>
+      <c r="K19" s="58">
+        <v>5</v>
+      </c>
+      <c r="L19" s="58">
         <v>1</v>
       </c>
-      <c r="M19" s="63">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
-      <c r="A20" s="59"/>
-      <c r="B20" s="118"/>
+      <c r="M19" s="56">
+        <v>5</v>
+      </c>
+      <c r="N19" s="99">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="52"/>
+      <c r="B20" s="113"/>
       <c r="C20" s="8"/>
       <c r="D20" s="14" t="s">
         <v>37</v>
       </c>
       <c r="E20" s="15"/>
-      <c r="F20" s="64"/>
-      <c r="G20" s="65">
-        <v>3</v>
-      </c>
-      <c r="H20" s="104">
-        <v>3</v>
-      </c>
-      <c r="I20" s="65">
-        <v>3</v>
-      </c>
-      <c r="J20" s="104">
-        <v>3</v>
-      </c>
-      <c r="K20" s="65">
-        <v>3</v>
-      </c>
-      <c r="L20" s="65">
-        <v>5</v>
-      </c>
-      <c r="M20" s="63">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
-      <c r="A21" s="59"/>
-      <c r="B21" s="118"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="58">
+        <v>3</v>
+      </c>
+      <c r="H20" s="96">
+        <v>3</v>
+      </c>
+      <c r="I20" s="58">
+        <v>3</v>
+      </c>
+      <c r="J20" s="96">
+        <v>3</v>
+      </c>
+      <c r="K20" s="58">
+        <v>3</v>
+      </c>
+      <c r="L20" s="58">
+        <v>5</v>
+      </c>
+      <c r="M20" s="56">
+        <v>3</v>
+      </c>
+      <c r="N20" s="99">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="52"/>
+      <c r="B21" s="113"/>
       <c r="C21" s="8"/>
       <c r="D21" s="14" t="s">
         <v>38</v>
       </c>
       <c r="E21" s="15"/>
-      <c r="F21" s="64"/>
-      <c r="G21" s="65">
-        <v>5</v>
-      </c>
-      <c r="H21" s="104">
-        <v>5</v>
-      </c>
-      <c r="I21" s="65">
-        <v>5</v>
-      </c>
-      <c r="J21" s="104">
-        <v>5</v>
-      </c>
-      <c r="K21" s="65">
-        <v>3</v>
-      </c>
-      <c r="L21" s="65">
-        <v>3</v>
-      </c>
-      <c r="M21" s="63">
+      <c r="F21" s="57"/>
+      <c r="G21" s="58">
+        <v>5</v>
+      </c>
+      <c r="H21" s="96">
+        <v>5</v>
+      </c>
+      <c r="I21" s="58">
+        <v>5</v>
+      </c>
+      <c r="J21" s="96">
+        <v>5</v>
+      </c>
+      <c r="K21" s="58">
+        <v>3</v>
+      </c>
+      <c r="L21" s="58">
+        <v>3</v>
+      </c>
+      <c r="M21" s="56">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:13">
-      <c r="A22" s="60"/>
-      <c r="B22" s="119"/>
-      <c r="C22" s="63"/>
+      <c r="N21" s="99">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="53"/>
+      <c r="B22" s="114"/>
+      <c r="C22" s="56"/>
       <c r="D22" s="14"/>
       <c r="E22" s="16"/>
-      <c r="F22" s="65"/>
+      <c r="F22" s="58"/>
       <c r="G22" s="21">
-        <f t="shared" ref="G22:M22" si="0">AVERAGE(G4:G21)</f>
+        <f t="shared" ref="G22:N22" si="0">AVERAGE(G4:G21)</f>
         <v>4.166666666666667</v>
       </c>
       <c r="H22" s="21">
@@ -2724,9 +2801,13 @@
         <f t="shared" si="0"/>
         <v>2.2777777777777777</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" s="4" customFormat="1" ht="18">
-      <c r="A23" s="34"/>
+      <c r="N22" s="21">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="30"/>
       <c r="B23" s="23"/>
       <c r="C23" s="24"/>
       <c r="D23" s="24"/>
@@ -2762,9 +2843,13 @@
         <f>M22 * F23 / 100</f>
         <v>0.68333333333333324</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" ht="30">
-      <c r="A24" s="35">
+      <c r="N23" s="27">
+        <f>N22 * F23 / 100</f>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="31">
         <v>2</v>
       </c>
       <c r="B24" s="19" t="s">
@@ -2780,30 +2865,33 @@
         <v>41</v>
       </c>
       <c r="F24" s="13"/>
-      <c r="G24" s="65">
-        <v>4</v>
-      </c>
-      <c r="H24" s="104">
-        <v>4</v>
-      </c>
-      <c r="I24" s="65">
+      <c r="G24" s="58">
+        <v>4</v>
+      </c>
+      <c r="H24" s="96">
+        <v>4</v>
+      </c>
+      <c r="I24" s="58">
         <v>2</v>
       </c>
-      <c r="J24" s="104">
-        <v>4</v>
-      </c>
-      <c r="K24" s="65">
-        <v>5</v>
-      </c>
-      <c r="L24" s="65">
+      <c r="J24" s="96">
+        <v>4</v>
+      </c>
+      <c r="K24" s="58">
+        <v>5</v>
+      </c>
+      <c r="L24" s="58">
         <v>1</v>
       </c>
-      <c r="M24" s="63">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" s="4" customFormat="1" ht="18">
-      <c r="A25" s="34"/>
+      <c r="M24" s="56">
+        <v>5</v>
+      </c>
+      <c r="N24" s="99">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A25" s="30"/>
       <c r="B25" s="23"/>
       <c r="C25" s="24"/>
       <c r="D25" s="24"/>
@@ -2839,276 +2927,298 @@
         <f>M24 * F25 / 100</f>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" ht="105">
-      <c r="A26" s="70">
-        <v>3</v>
-      </c>
-      <c r="B26" s="71" t="s">
+      <c r="N25" s="27">
+        <f>N24 * F25 / 100</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="126" x14ac:dyDescent="0.25">
+      <c r="A26" s="62">
+        <v>3</v>
+      </c>
+      <c r="B26" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="68" t="s">
+      <c r="C26" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="D26" s="43" t="s">
+      <c r="D26" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="E26" s="68" t="s">
+      <c r="E26" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="F26" s="72"/>
-      <c r="G26" s="73"/>
-      <c r="H26" s="73"/>
-      <c r="I26" s="73"/>
-      <c r="J26" s="73"/>
-      <c r="K26" s="73"/>
-      <c r="L26" s="73"/>
-      <c r="M26" s="74"/>
-    </row>
-    <row r="27" spans="1:13" s="5" customFormat="1">
-      <c r="A27" s="83"/>
-      <c r="B27" s="84"/>
-      <c r="C27" s="85"/>
-      <c r="D27" s="85"/>
-      <c r="E27" s="85"/>
-      <c r="F27" s="85"/>
-      <c r="G27" s="85"/>
-      <c r="H27" s="85"/>
-      <c r="I27" s="85"/>
-      <c r="J27" s="85"/>
-      <c r="K27" s="85"/>
-      <c r="L27" s="85"/>
-      <c r="M27" s="86"/>
-    </row>
-    <row r="28" spans="1:13" ht="180">
-      <c r="A28" s="87">
-        <v>4</v>
-      </c>
-      <c r="B28" s="88" t="s">
+      <c r="F26" s="64"/>
+      <c r="G26" s="65"/>
+      <c r="H26" s="65"/>
+      <c r="I26" s="65"/>
+      <c r="J26" s="65"/>
+      <c r="K26" s="65"/>
+      <c r="L26" s="65"/>
+      <c r="M26" s="66"/>
+      <c r="N26" s="66"/>
+    </row>
+    <row r="27" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="75"/>
+      <c r="B27" s="76"/>
+      <c r="C27" s="77"/>
+      <c r="D27" s="77"/>
+      <c r="E27" s="77"/>
+      <c r="F27" s="77"/>
+      <c r="G27" s="77"/>
+      <c r="H27" s="77"/>
+      <c r="I27" s="77"/>
+      <c r="J27" s="77"/>
+      <c r="K27" s="77"/>
+      <c r="L27" s="77"/>
+      <c r="M27" s="78"/>
+      <c r="N27" s="78"/>
+    </row>
+    <row r="28" spans="1:14" ht="204.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="79">
+        <v>4</v>
+      </c>
+      <c r="B28" s="80" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="74" t="s">
+      <c r="C28" s="66" t="s">
         <v>47</v>
       </c>
-      <c r="D28" s="67" t="s">
+      <c r="D28" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="E28" s="74" t="s">
+      <c r="E28" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="F28" s="73"/>
-      <c r="G28" s="73"/>
-      <c r="H28" s="73"/>
-      <c r="I28" s="73"/>
-      <c r="J28" s="73"/>
-      <c r="K28" s="73"/>
-      <c r="L28" s="73"/>
-      <c r="M28" s="74"/>
-    </row>
-    <row r="29" spans="1:13" s="5" customFormat="1">
-      <c r="A29" s="83"/>
-      <c r="B29" s="84"/>
-      <c r="C29" s="85"/>
-      <c r="D29" s="85"/>
-      <c r="E29" s="85"/>
-      <c r="F29" s="85"/>
-      <c r="G29" s="85"/>
-      <c r="H29" s="85"/>
-      <c r="I29" s="85"/>
-      <c r="J29" s="85"/>
-      <c r="K29" s="85"/>
-      <c r="L29" s="85"/>
-      <c r="M29" s="86"/>
-    </row>
-    <row r="30" spans="1:13" ht="30">
-      <c r="A30" s="109">
-        <v>5</v>
-      </c>
-      <c r="B30" s="118" t="s">
+      <c r="F28" s="65"/>
+      <c r="G28" s="65"/>
+      <c r="H28" s="65"/>
+      <c r="I28" s="65"/>
+      <c r="J28" s="65"/>
+      <c r="K28" s="65"/>
+      <c r="L28" s="65"/>
+      <c r="M28" s="66"/>
+      <c r="N28" s="66"/>
+    </row>
+    <row r="29" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="75"/>
+      <c r="B29" s="76"/>
+      <c r="C29" s="77"/>
+      <c r="D29" s="77"/>
+      <c r="E29" s="77"/>
+      <c r="F29" s="77"/>
+      <c r="G29" s="77"/>
+      <c r="H29" s="77"/>
+      <c r="I29" s="77"/>
+      <c r="J29" s="77"/>
+      <c r="K29" s="77"/>
+      <c r="L29" s="77"/>
+      <c r="M29" s="78"/>
+      <c r="N29" s="99"/>
+    </row>
+    <row r="30" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A30" s="116">
+        <v>5</v>
+      </c>
+      <c r="B30" s="113" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="113" t="s">
+      <c r="C30" s="103" t="s">
         <v>50</v>
       </c>
-      <c r="D30" s="67" t="s">
+      <c r="D30" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="E30" s="113" t="s">
+      <c r="E30" s="103" t="s">
         <v>52</v>
       </c>
-      <c r="F30" s="115"/>
-      <c r="G30" s="107">
-        <v>4</v>
-      </c>
-      <c r="H30" s="102"/>
-      <c r="I30" s="107">
+      <c r="F30" s="106"/>
+      <c r="G30" s="108">
+        <v>4</v>
+      </c>
+      <c r="H30" s="94"/>
+      <c r="I30" s="108">
         <v>2</v>
       </c>
-      <c r="J30" s="107">
+      <c r="J30" s="108">
         <v>0</v>
       </c>
-      <c r="K30" s="107">
-        <v>3</v>
-      </c>
-      <c r="L30" s="107">
-        <v>4</v>
-      </c>
-      <c r="M30" s="107">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13">
-      <c r="A31" s="109"/>
-      <c r="B31" s="118"/>
-      <c r="C31" s="113"/>
+      <c r="K30" s="108">
+        <v>3</v>
+      </c>
+      <c r="L30" s="108">
+        <v>4</v>
+      </c>
+      <c r="M30" s="108">
+        <v>3</v>
+      </c>
+      <c r="N30" s="108">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="116"/>
+      <c r="B31" s="113"/>
+      <c r="C31" s="103"/>
       <c r="D31" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E31" s="113"/>
-      <c r="F31" s="115"/>
-      <c r="G31" s="107"/>
-      <c r="H31" s="102"/>
-      <c r="I31" s="107"/>
-      <c r="J31" s="107"/>
-      <c r="K31" s="107"/>
-      <c r="L31" s="107"/>
-      <c r="M31" s="107"/>
-    </row>
-    <row r="32" spans="1:13">
-      <c r="A32" s="109"/>
-      <c r="B32" s="118"/>
-      <c r="C32" s="113"/>
+      <c r="E31" s="103"/>
+      <c r="F31" s="106"/>
+      <c r="G31" s="108"/>
+      <c r="H31" s="94"/>
+      <c r="I31" s="108"/>
+      <c r="J31" s="108"/>
+      <c r="K31" s="108"/>
+      <c r="L31" s="108"/>
+      <c r="M31" s="108"/>
+      <c r="N31" s="108"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="116"/>
+      <c r="B32" s="113"/>
+      <c r="C32" s="103"/>
       <c r="D32" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E32" s="113"/>
-      <c r="F32" s="115"/>
-      <c r="G32" s="107"/>
-      <c r="H32" s="102"/>
-      <c r="I32" s="107"/>
-      <c r="J32" s="107"/>
-      <c r="K32" s="107"/>
-      <c r="L32" s="107"/>
-      <c r="M32" s="107"/>
-    </row>
-    <row r="33" spans="1:13" ht="30">
-      <c r="A33" s="109"/>
-      <c r="B33" s="118"/>
-      <c r="C33" s="113"/>
+      <c r="E32" s="103"/>
+      <c r="F32" s="106"/>
+      <c r="G32" s="108"/>
+      <c r="H32" s="94"/>
+      <c r="I32" s="108"/>
+      <c r="J32" s="108"/>
+      <c r="K32" s="108"/>
+      <c r="L32" s="108"/>
+      <c r="M32" s="108"/>
+      <c r="N32" s="108"/>
+    </row>
+    <row r="33" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="116"/>
+      <c r="B33" s="113"/>
+      <c r="C33" s="103"/>
       <c r="D33" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E33" s="113"/>
-      <c r="F33" s="115"/>
-      <c r="G33" s="107"/>
-      <c r="H33" s="102"/>
-      <c r="I33" s="107"/>
-      <c r="J33" s="107"/>
-      <c r="K33" s="107"/>
-      <c r="L33" s="107"/>
-      <c r="M33" s="107"/>
-    </row>
-    <row r="34" spans="1:13" s="4" customFormat="1" ht="18">
-      <c r="A34" s="109"/>
-      <c r="B34" s="118"/>
-      <c r="C34" s="113"/>
+      <c r="E33" s="103"/>
+      <c r="F33" s="106"/>
+      <c r="G33" s="108"/>
+      <c r="H33" s="94"/>
+      <c r="I33" s="108"/>
+      <c r="J33" s="108"/>
+      <c r="K33" s="108"/>
+      <c r="L33" s="108"/>
+      <c r="M33" s="108"/>
+      <c r="N33" s="108"/>
+    </row>
+    <row r="34" spans="1:14" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A34" s="116"/>
+      <c r="B34" s="113"/>
+      <c r="C34" s="103"/>
       <c r="D34" s="9"/>
-      <c r="E34" s="113"/>
-      <c r="F34" s="115"/>
-      <c r="G34" s="107"/>
-      <c r="H34" s="102"/>
-      <c r="I34" s="107"/>
-      <c r="J34" s="107"/>
-      <c r="K34" s="107"/>
-      <c r="L34" s="107"/>
-      <c r="M34" s="107"/>
-    </row>
-    <row r="35" spans="1:13" ht="45">
-      <c r="A35" s="109"/>
-      <c r="B35" s="118"/>
-      <c r="C35" s="113"/>
+      <c r="E34" s="103"/>
+      <c r="F34" s="106"/>
+      <c r="G34" s="108"/>
+      <c r="H34" s="94"/>
+      <c r="I34" s="108"/>
+      <c r="J34" s="108"/>
+      <c r="K34" s="108"/>
+      <c r="L34" s="108"/>
+      <c r="M34" s="108"/>
+      <c r="N34" s="108"/>
+    </row>
+    <row r="35" spans="1:14" ht="63" x14ac:dyDescent="0.25">
+      <c r="A35" s="116"/>
+      <c r="B35" s="113"/>
+      <c r="C35" s="103"/>
       <c r="D35" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="E35" s="114"/>
-      <c r="F35" s="116"/>
-      <c r="G35" s="108"/>
-      <c r="H35" s="103"/>
-      <c r="I35" s="108"/>
-      <c r="J35" s="108"/>
-      <c r="K35" s="108"/>
-      <c r="L35" s="108"/>
-      <c r="M35" s="108"/>
-    </row>
-    <row r="36" spans="1:13" ht="30">
-      <c r="A36" s="59"/>
-      <c r="B36" s="118"/>
+      <c r="E35" s="104"/>
+      <c r="F35" s="107"/>
+      <c r="G35" s="109"/>
+      <c r="H35" s="95"/>
+      <c r="I35" s="109"/>
+      <c r="J35" s="109"/>
+      <c r="K35" s="109"/>
+      <c r="L35" s="109"/>
+      <c r="M35" s="109"/>
+      <c r="N35" s="109"/>
+    </row>
+    <row r="36" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A36" s="52"/>
+      <c r="B36" s="113"/>
       <c r="C36" s="8"/>
       <c r="D36" s="12" t="s">
         <v>57</v>
       </c>
       <c r="E36" s="11"/>
       <c r="F36" s="13"/>
-      <c r="G36" s="65">
-        <v>4</v>
-      </c>
-      <c r="H36" s="104">
+      <c r="G36" s="58">
+        <v>4</v>
+      </c>
+      <c r="H36" s="96">
         <v>4.2</v>
       </c>
-      <c r="I36" s="65">
+      <c r="I36" s="58">
         <v>2</v>
       </c>
-      <c r="J36" s="104">
+      <c r="J36" s="96">
         <v>2.2000000000000002</v>
       </c>
-      <c r="K36" s="65">
-        <v>5</v>
-      </c>
-      <c r="L36" s="65">
-        <v>3</v>
-      </c>
-      <c r="M36" s="63">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" ht="45">
-      <c r="A37" s="60"/>
-      <c r="B37" s="119"/>
-      <c r="C37" s="63"/>
-      <c r="D37" s="44" t="s">
+      <c r="K36" s="58">
+        <v>5</v>
+      </c>
+      <c r="L36" s="58">
+        <v>3</v>
+      </c>
+      <c r="M36" s="56">
+        <v>5</v>
+      </c>
+      <c r="N36" s="99">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="63" x14ac:dyDescent="0.25">
+      <c r="A37" s="53"/>
+      <c r="B37" s="114"/>
+      <c r="C37" s="56"/>
+      <c r="D37" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="E37" s="63"/>
-      <c r="F37" s="65"/>
-      <c r="G37" s="65">
-        <v>4</v>
-      </c>
-      <c r="H37" s="104">
-        <v>4</v>
-      </c>
-      <c r="I37" s="65">
-        <v>4</v>
-      </c>
-      <c r="J37" s="104">
-        <v>4</v>
-      </c>
-      <c r="K37" s="65">
+      <c r="E37" s="56"/>
+      <c r="F37" s="58"/>
+      <c r="G37" s="58">
+        <v>4</v>
+      </c>
+      <c r="H37" s="96">
+        <v>4</v>
+      </c>
+      <c r="I37" s="58">
+        <v>4</v>
+      </c>
+      <c r="J37" s="96">
+        <v>4</v>
+      </c>
+      <c r="K37" s="58">
         <v>2</v>
       </c>
-      <c r="L37" s="65">
-        <v>5</v>
-      </c>
-      <c r="M37" s="63">
+      <c r="L37" s="58">
+        <v>5</v>
+      </c>
+      <c r="M37" s="56">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" s="4" customFormat="1" ht="18">
-      <c r="A38" s="60"/>
-      <c r="B38" s="61"/>
-      <c r="C38" s="63"/>
-      <c r="D38" s="44"/>
-      <c r="E38" s="63"/>
-      <c r="F38" s="65"/>
+      <c r="N37" s="99">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A38" s="53"/>
+      <c r="B38" s="54"/>
+      <c r="C38" s="56"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="56"/>
+      <c r="F38" s="58"/>
       <c r="G38" s="21">
         <f>AVERAGE(G35:G37)</f>
         <v>4</v>
@@ -3118,7 +3228,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="I38" s="21">
-        <f t="shared" ref="I38:M38" si="1">AVERAGE(I35:I37)</f>
+        <f t="shared" ref="I38:N38" si="1">AVERAGE(I35:I37)</f>
         <v>3</v>
       </c>
       <c r="J38" s="21">
@@ -3137,9 +3247,13 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" ht="18">
-      <c r="A39" s="34"/>
+      <c r="N38" s="22">
+        <f t="shared" si="1"/>
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A39" s="30"/>
       <c r="B39" s="23"/>
       <c r="C39" s="24"/>
       <c r="D39" s="24"/>
@@ -3175,34 +3289,39 @@
         <f>M38 * F39 / 100</f>
         <v>0.75</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" ht="90">
-      <c r="A40" s="70">
+      <c r="N39" s="27">
+        <f>N38 * F39 / 100</f>
+        <v>0.8125</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A40" s="62">
         <v>6</v>
       </c>
-      <c r="B40" s="71" t="s">
+      <c r="B40" s="63" t="s">
         <v>59</v>
       </c>
-      <c r="C40" s="68" t="s">
+      <c r="C40" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="D40" s="43" t="s">
+      <c r="D40" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="E40" s="68" t="s">
+      <c r="E40" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="F40" s="72"/>
-      <c r="G40" s="73"/>
-      <c r="H40" s="73"/>
-      <c r="I40" s="73"/>
-      <c r="J40" s="73"/>
-      <c r="K40" s="73"/>
-      <c r="L40" s="73"/>
-      <c r="M40" s="74"/>
-    </row>
-    <row r="41" spans="1:13">
-      <c r="A41" s="35"/>
+      <c r="F40" s="64"/>
+      <c r="G40" s="65"/>
+      <c r="H40" s="65"/>
+      <c r="I40" s="65"/>
+      <c r="J40" s="65"/>
+      <c r="K40" s="65"/>
+      <c r="L40" s="65"/>
+      <c r="M40" s="66"/>
+      <c r="N40" s="66"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" s="31"/>
       <c r="B41" s="19"/>
       <c r="C41" s="11"/>
       <c r="D41" s="12"/>
@@ -3216,47 +3335,50 @@
       <c r="L41" s="11"/>
       <c r="M41" s="13"/>
     </row>
-    <row r="42" spans="1:13" s="4" customFormat="1" ht="128.25" customHeight="1">
-      <c r="A42" s="60">
+    <row r="42" spans="1:14" s="4" customFormat="1" ht="128.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="53">
         <v>7</v>
       </c>
-      <c r="B42" s="61" t="s">
+      <c r="B42" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="C42" s="63" t="s">
+      <c r="C42" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="44" t="s">
+      <c r="D42" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="E42" s="63" t="s">
+      <c r="E42" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="F42" s="65"/>
-      <c r="G42" s="65">
-        <v>5</v>
-      </c>
-      <c r="H42" s="104">
-        <v>5</v>
-      </c>
-      <c r="I42" s="65">
-        <v>3</v>
-      </c>
-      <c r="J42" s="104">
-        <v>4</v>
-      </c>
-      <c r="K42" s="65">
+      <c r="F42" s="58"/>
+      <c r="G42" s="58">
+        <v>5</v>
+      </c>
+      <c r="H42" s="96">
+        <v>5</v>
+      </c>
+      <c r="I42" s="58">
+        <v>3</v>
+      </c>
+      <c r="J42" s="96">
+        <v>4</v>
+      </c>
+      <c r="K42" s="58">
         <v>2</v>
       </c>
-      <c r="L42" s="65">
-        <v>4</v>
-      </c>
-      <c r="M42" s="63">
+      <c r="L42" s="58">
+        <v>4</v>
+      </c>
+      <c r="M42" s="56">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" ht="18">
-      <c r="A43" s="34"/>
+      <c r="N42" s="99">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A43" s="30"/>
       <c r="B43" s="23"/>
       <c r="C43" s="24"/>
       <c r="D43" s="24"/>
@@ -3292,34 +3414,39 @@
         <f>M42 * F43 / 100</f>
         <v>0.05</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" s="4" customFormat="1" ht="76">
-      <c r="A44" s="70">
+      <c r="N43" s="27">
+        <f>N42 * F43 / 100</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" s="4" customFormat="1" ht="95.25" x14ac:dyDescent="0.3">
+      <c r="A44" s="62">
         <v>8</v>
       </c>
-      <c r="B44" s="71" t="s">
+      <c r="B44" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="C44" s="68" t="s">
+      <c r="C44" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="D44" s="43" t="s">
+      <c r="D44" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="E44" s="68" t="s">
+      <c r="E44" s="61" t="s">
         <v>70</v>
       </c>
-      <c r="F44" s="72"/>
-      <c r="G44" s="73"/>
-      <c r="H44" s="73"/>
-      <c r="I44" s="73"/>
-      <c r="J44" s="73"/>
-      <c r="K44" s="73"/>
-      <c r="L44" s="73"/>
-      <c r="M44" s="74"/>
-    </row>
-    <row r="45" spans="1:13">
-      <c r="A45" s="35"/>
+      <c r="F44" s="64"/>
+      <c r="G44" s="65"/>
+      <c r="H44" s="65"/>
+      <c r="I44" s="65"/>
+      <c r="J44" s="65"/>
+      <c r="K44" s="65"/>
+      <c r="L44" s="65"/>
+      <c r="M44" s="66"/>
+      <c r="N44" s="66"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" s="31"/>
       <c r="B45" s="19"/>
       <c r="C45" s="11"/>
       <c r="D45" s="12"/>
@@ -3333,171 +3460,181 @@
       <c r="L45" s="11"/>
       <c r="M45" s="13"/>
     </row>
-    <row r="46" spans="1:13" s="4" customFormat="1" ht="76">
-      <c r="A46" s="109">
+    <row r="46" spans="1:14" s="4" customFormat="1" ht="95.25" x14ac:dyDescent="0.3">
+      <c r="A46" s="116">
         <v>9</v>
       </c>
-      <c r="B46" s="111" t="s">
+      <c r="B46" s="119" t="s">
         <v>71</v>
       </c>
-      <c r="C46" s="113" t="s">
+      <c r="C46" s="103" t="s">
         <v>72</v>
       </c>
-      <c r="D46" s="67" t="s">
+      <c r="D46" s="60" t="s">
         <v>73</v>
       </c>
       <c r="E46" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="F46" s="115"/>
-      <c r="G46" s="107">
-        <v>4</v>
-      </c>
-      <c r="H46" s="102"/>
-      <c r="I46" s="107">
-        <v>5</v>
-      </c>
-      <c r="J46" s="102"/>
-      <c r="K46" s="107">
+      <c r="F46" s="106"/>
+      <c r="G46" s="108">
+        <v>4</v>
+      </c>
+      <c r="H46" s="94"/>
+      <c r="I46" s="108">
+        <v>5</v>
+      </c>
+      <c r="J46" s="94"/>
+      <c r="K46" s="108">
         <v>2</v>
       </c>
-      <c r="L46" s="107">
-        <v>3</v>
-      </c>
-      <c r="M46" s="107">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" ht="135">
-      <c r="A47" s="109"/>
-      <c r="B47" s="111"/>
-      <c r="C47" s="113"/>
+      <c r="L46" s="108">
+        <v>3</v>
+      </c>
+      <c r="M46" s="108">
+        <v>4</v>
+      </c>
+      <c r="N46" s="108">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A47" s="116"/>
+      <c r="B47" s="119"/>
+      <c r="C47" s="103"/>
       <c r="D47" s="9" t="s">
         <v>75</v>
       </c>
       <c r="E47" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="F47" s="115"/>
-      <c r="G47" s="107"/>
-      <c r="H47" s="102"/>
-      <c r="I47" s="107"/>
-      <c r="J47" s="102"/>
-      <c r="K47" s="107"/>
-      <c r="L47" s="107"/>
-      <c r="M47" s="107"/>
-    </row>
-    <row r="48" spans="1:13" s="4" customFormat="1" ht="18">
-      <c r="A48" s="109"/>
-      <c r="B48" s="111"/>
-      <c r="C48" s="113"/>
+      <c r="F47" s="106"/>
+      <c r="G47" s="108"/>
+      <c r="H47" s="94"/>
+      <c r="I47" s="108"/>
+      <c r="J47" s="94"/>
+      <c r="K47" s="108"/>
+      <c r="L47" s="108"/>
+      <c r="M47" s="108"/>
+      <c r="N47" s="108"/>
+    </row>
+    <row r="48" spans="1:14" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A48" s="116"/>
+      <c r="B48" s="119"/>
+      <c r="C48" s="103"/>
       <c r="D48" s="9" t="s">
         <v>77</v>
       </c>
       <c r="E48" s="17"/>
-      <c r="F48" s="115"/>
-      <c r="G48" s="107"/>
-      <c r="H48" s="102"/>
-      <c r="I48" s="107"/>
-      <c r="J48" s="102"/>
-      <c r="K48" s="107"/>
-      <c r="L48" s="107"/>
-      <c r="M48" s="107"/>
-    </row>
-    <row r="49" spans="1:13">
-      <c r="A49" s="109"/>
-      <c r="B49" s="111"/>
-      <c r="C49" s="113"/>
+      <c r="F48" s="106"/>
+      <c r="G48" s="108"/>
+      <c r="H48" s="94"/>
+      <c r="I48" s="108"/>
+      <c r="J48" s="94"/>
+      <c r="K48" s="108"/>
+      <c r="L48" s="108"/>
+      <c r="M48" s="108"/>
+      <c r="N48" s="108"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A49" s="116"/>
+      <c r="B49" s="119"/>
+      <c r="C49" s="103"/>
       <c r="D49" s="10"/>
       <c r="E49" s="17"/>
-      <c r="F49" s="115"/>
-      <c r="G49" s="107"/>
-      <c r="H49" s="102"/>
-      <c r="I49" s="107"/>
-      <c r="J49" s="102"/>
-      <c r="K49" s="107"/>
-      <c r="L49" s="107"/>
-      <c r="M49" s="107"/>
-    </row>
-    <row r="50" spans="1:13" s="4" customFormat="1" ht="18">
-      <c r="A50" s="109"/>
-      <c r="B50" s="111"/>
-      <c r="C50" s="113"/>
+      <c r="F49" s="106"/>
+      <c r="G49" s="108"/>
+      <c r="H49" s="94"/>
+      <c r="I49" s="108"/>
+      <c r="J49" s="94"/>
+      <c r="K49" s="108"/>
+      <c r="L49" s="108"/>
+      <c r="M49" s="108"/>
+      <c r="N49" s="108"/>
+    </row>
+    <row r="50" spans="1:14" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A50" s="116"/>
+      <c r="B50" s="119"/>
+      <c r="C50" s="103"/>
       <c r="D50" s="9" t="s">
         <v>78</v>
       </c>
       <c r="E50" s="17"/>
-      <c r="F50" s="115"/>
-      <c r="G50" s="107"/>
-      <c r="H50" s="102"/>
-      <c r="I50" s="107"/>
-      <c r="J50" s="102"/>
-      <c r="K50" s="107"/>
-      <c r="L50" s="107"/>
-      <c r="M50" s="107"/>
-    </row>
-    <row r="51" spans="1:13" ht="30">
-      <c r="A51" s="109"/>
-      <c r="B51" s="111"/>
-      <c r="C51" s="113"/>
+      <c r="F50" s="106"/>
+      <c r="G50" s="108"/>
+      <c r="H50" s="94"/>
+      <c r="I50" s="108"/>
+      <c r="J50" s="94"/>
+      <c r="K50" s="108"/>
+      <c r="L50" s="108"/>
+      <c r="M50" s="108"/>
+      <c r="N50" s="108"/>
+    </row>
+    <row r="51" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A51" s="116"/>
+      <c r="B51" s="119"/>
+      <c r="C51" s="103"/>
       <c r="D51" s="9" t="s">
         <v>79</v>
       </c>
       <c r="E51" s="17"/>
-      <c r="F51" s="115"/>
-      <c r="G51" s="107"/>
-      <c r="H51" s="102"/>
-      <c r="I51" s="107"/>
-      <c r="J51" s="102"/>
-      <c r="K51" s="107"/>
-      <c r="L51" s="107"/>
-      <c r="M51" s="107"/>
-    </row>
-    <row r="52" spans="1:13" s="6" customFormat="1" ht="45">
-      <c r="A52" s="109"/>
-      <c r="B52" s="111"/>
-      <c r="C52" s="113"/>
+      <c r="F51" s="106"/>
+      <c r="G51" s="108"/>
+      <c r="H51" s="94"/>
+      <c r="I51" s="108"/>
+      <c r="J51" s="94"/>
+      <c r="K51" s="108"/>
+      <c r="L51" s="108"/>
+      <c r="M51" s="108"/>
+      <c r="N51" s="108"/>
+    </row>
+    <row r="52" spans="1:14" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A52" s="116"/>
+      <c r="B52" s="119"/>
+      <c r="C52" s="103"/>
       <c r="D52" s="9" t="s">
         <v>80</v>
       </c>
       <c r="E52" s="17"/>
-      <c r="F52" s="115"/>
-      <c r="G52" s="107"/>
-      <c r="H52" s="102"/>
-      <c r="I52" s="107"/>
-      <c r="J52" s="102"/>
-      <c r="K52" s="107"/>
-      <c r="L52" s="107"/>
-      <c r="M52" s="107"/>
-    </row>
-    <row r="53" spans="1:13" ht="75">
-      <c r="A53" s="110"/>
-      <c r="B53" s="112"/>
-      <c r="C53" s="114"/>
-      <c r="D53" s="67" t="s">
+      <c r="F52" s="106"/>
+      <c r="G52" s="108"/>
+      <c r="H52" s="94"/>
+      <c r="I52" s="108"/>
+      <c r="J52" s="94"/>
+      <c r="K52" s="108"/>
+      <c r="L52" s="108"/>
+      <c r="M52" s="108"/>
+      <c r="N52" s="108"/>
+    </row>
+    <row r="53" spans="1:14" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="117"/>
+      <c r="B53" s="120"/>
+      <c r="C53" s="104"/>
+      <c r="D53" s="60" t="s">
         <v>81</v>
       </c>
       <c r="E53" s="17"/>
-      <c r="F53" s="116"/>
-      <c r="G53" s="108"/>
-      <c r="H53" s="103">
-        <v>4</v>
-      </c>
-      <c r="I53" s="108"/>
-      <c r="J53" s="103">
-        <v>5</v>
-      </c>
-      <c r="K53" s="108"/>
-      <c r="L53" s="108"/>
-      <c r="M53" s="108"/>
-    </row>
-    <row r="54" spans="1:13" ht="18">
-      <c r="A54" s="47"/>
-      <c r="B54" s="48"/>
-      <c r="C54" s="49"/>
-      <c r="D54" s="49"/>
-      <c r="E54" s="49"/>
-      <c r="F54" s="50">
+      <c r="F53" s="107"/>
+      <c r="G53" s="109"/>
+      <c r="H53" s="95">
+        <v>4</v>
+      </c>
+      <c r="I53" s="109"/>
+      <c r="J53" s="95">
+        <v>5</v>
+      </c>
+      <c r="K53" s="109"/>
+      <c r="L53" s="109"/>
+      <c r="M53" s="109"/>
+      <c r="N53" s="109"/>
+    </row>
+    <row r="54" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A54" s="43"/>
+      <c r="B54" s="44"/>
+      <c r="C54" s="45"/>
+      <c r="D54" s="45"/>
+      <c r="E54" s="45"/>
+      <c r="F54" s="46">
         <v>5</v>
       </c>
       <c r="G54" s="26">
@@ -3528,137 +3665,151 @@
         <f>M46 * F54 / 100</f>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="55" spans="1:13">
-      <c r="A55" s="120">
+      <c r="N54" s="26">
+        <f>N46 * F54 / 100</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A55" s="115">
         <v>10</v>
       </c>
-      <c r="B55" s="121" t="s">
+      <c r="B55" s="118" t="s">
         <v>82</v>
       </c>
-      <c r="C55" s="122" t="s">
+      <c r="C55" s="102" t="s">
         <v>83</v>
       </c>
-      <c r="D55" s="67" t="s">
+      <c r="D55" s="60" t="s">
         <v>84</v>
       </c>
-      <c r="E55" s="122" t="s">
+      <c r="E55" s="102" t="s">
         <v>85</v>
       </c>
-      <c r="F55" s="123"/>
-      <c r="G55" s="117">
-        <v>4</v>
-      </c>
-      <c r="H55" s="105"/>
-      <c r="I55" s="117">
-        <v>3</v>
-      </c>
-      <c r="J55" s="105"/>
-      <c r="K55" s="117">
-        <v>3</v>
-      </c>
-      <c r="L55" s="117">
-        <v>5</v>
-      </c>
-      <c r="M55" s="117">
+      <c r="F55" s="105"/>
+      <c r="G55" s="112">
+        <v>4</v>
+      </c>
+      <c r="H55" s="97"/>
+      <c r="I55" s="112">
+        <v>3</v>
+      </c>
+      <c r="J55" s="97"/>
+      <c r="K55" s="112">
+        <v>3</v>
+      </c>
+      <c r="L55" s="112">
+        <v>5</v>
+      </c>
+      <c r="M55" s="112">
         <v>2</v>
       </c>
-    </row>
-    <row r="56" spans="1:13">
-      <c r="A56" s="109"/>
-      <c r="B56" s="111"/>
-      <c r="C56" s="113"/>
+      <c r="N55" s="112">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56" s="116"/>
+      <c r="B56" s="119"/>
+      <c r="C56" s="103"/>
       <c r="D56" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="E56" s="113"/>
-      <c r="F56" s="115"/>
-      <c r="G56" s="107"/>
-      <c r="H56" s="102"/>
-      <c r="I56" s="107"/>
-      <c r="J56" s="102"/>
-      <c r="K56" s="107"/>
-      <c r="L56" s="107"/>
-      <c r="M56" s="107"/>
-    </row>
-    <row r="57" spans="1:13" ht="30">
-      <c r="A57" s="109"/>
-      <c r="B57" s="111"/>
-      <c r="C57" s="113"/>
+      <c r="E56" s="103"/>
+      <c r="F56" s="106"/>
+      <c r="G56" s="108"/>
+      <c r="H56" s="94"/>
+      <c r="I56" s="108"/>
+      <c r="J56" s="94"/>
+      <c r="K56" s="108"/>
+      <c r="L56" s="108"/>
+      <c r="M56" s="108"/>
+      <c r="N56" s="108"/>
+    </row>
+    <row r="57" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A57" s="116"/>
+      <c r="B57" s="119"/>
+      <c r="C57" s="103"/>
       <c r="D57" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="E57" s="113"/>
-      <c r="F57" s="115"/>
-      <c r="G57" s="107"/>
-      <c r="H57" s="102"/>
-      <c r="I57" s="107"/>
-      <c r="J57" s="102"/>
-      <c r="K57" s="107"/>
-      <c r="L57" s="107"/>
-      <c r="M57" s="107"/>
-    </row>
-    <row r="58" spans="1:13" ht="30">
-      <c r="A58" s="110"/>
-      <c r="B58" s="112"/>
-      <c r="C58" s="114"/>
-      <c r="D58" s="44" t="s">
+      <c r="E57" s="103"/>
+      <c r="F57" s="106"/>
+      <c r="G57" s="108"/>
+      <c r="H57" s="94"/>
+      <c r="I57" s="108"/>
+      <c r="J57" s="94"/>
+      <c r="K57" s="108"/>
+      <c r="L57" s="108"/>
+      <c r="M57" s="108"/>
+      <c r="N57" s="108"/>
+    </row>
+    <row r="58" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A58" s="117"/>
+      <c r="B58" s="120"/>
+      <c r="C58" s="104"/>
+      <c r="D58" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="E58" s="114"/>
-      <c r="F58" s="116"/>
-      <c r="G58" s="108"/>
-      <c r="H58" s="103">
-        <v>4</v>
-      </c>
-      <c r="I58" s="108"/>
-      <c r="J58" s="103">
-        <v>3</v>
-      </c>
-      <c r="K58" s="108"/>
-      <c r="L58" s="108"/>
-      <c r="M58" s="108"/>
-    </row>
-    <row r="59" spans="1:13" ht="18">
-      <c r="A59" s="75"/>
-      <c r="B59" s="76"/>
-      <c r="C59" s="77"/>
-      <c r="D59" s="77"/>
-      <c r="E59" s="77"/>
-      <c r="F59" s="78">
+      <c r="E58" s="104"/>
+      <c r="F58" s="107"/>
+      <c r="G58" s="109"/>
+      <c r="H58" s="95">
+        <v>4</v>
+      </c>
+      <c r="I58" s="109"/>
+      <c r="J58" s="95">
+        <v>3</v>
+      </c>
+      <c r="K58" s="109"/>
+      <c r="L58" s="109"/>
+      <c r="M58" s="109"/>
+      <c r="N58" s="109"/>
+    </row>
+    <row r="59" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A59" s="67"/>
+      <c r="B59" s="68"/>
+      <c r="C59" s="69"/>
+      <c r="D59" s="69"/>
+      <c r="E59" s="69"/>
+      <c r="F59" s="70">
         <v>30</v>
       </c>
-      <c r="G59" s="79">
+      <c r="G59" s="71">
         <f>G55 * F59 / 100</f>
         <v>1.2</v>
       </c>
-      <c r="H59" s="79">
+      <c r="H59" s="71">
         <f>H58 * F59 / 100</f>
         <v>1.2</v>
       </c>
-      <c r="I59" s="79">
+      <c r="I59" s="71">
         <f>I55 * F59 / 100</f>
         <v>0.9</v>
       </c>
-      <c r="J59" s="79">
+      <c r="J59" s="71">
         <f>J58 * F59 / 100</f>
         <v>0.9</v>
       </c>
-      <c r="K59" s="79">
+      <c r="K59" s="71">
         <f>K55 * F59 / 100</f>
         <v>0.9</v>
       </c>
-      <c r="L59" s="79">
+      <c r="L59" s="71">
         <f>L55 * F59 / 100</f>
         <v>1.5</v>
       </c>
-      <c r="M59" s="80">
+      <c r="M59" s="72">
         <f>M55 * F59 / 100</f>
         <v>0.6</v>
       </c>
-    </row>
-    <row r="60" spans="1:13">
-      <c r="A60" s="35"/>
+      <c r="N59" s="72">
+        <f>N55 * F59 / 100</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A60" s="31"/>
       <c r="B60" s="19"/>
       <c r="C60" s="11"/>
       <c r="D60" s="11"/>
@@ -3672,67 +3823,56 @@
       <c r="L60" s="11"/>
       <c r="M60" s="13"/>
     </row>
-    <row r="61" spans="1:13" ht="20">
-      <c r="A61" s="124" t="s">
+    <row r="61" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A61" s="110" t="s">
         <v>89</v>
       </c>
-      <c r="B61" s="125"/>
-      <c r="C61" s="125"/>
-      <c r="D61" s="125"/>
-      <c r="E61" s="125"/>
-      <c r="F61" s="81">
+      <c r="B61" s="111"/>
+      <c r="C61" s="111"/>
+      <c r="D61" s="111"/>
+      <c r="E61" s="111"/>
+      <c r="F61" s="73">
         <f>SUM(F59,F54,F43,F39,F25,F23)</f>
         <v>100</v>
       </c>
-      <c r="G61" s="82">
+      <c r="G61" s="74">
         <f>ROUNDUP(SUM(G59,G54,G43,G39,G25,G23), 2)</f>
         <v>4.0999999999999996</v>
       </c>
-      <c r="H61" s="82">
+      <c r="H61" s="74">
         <f>ROUNDUP(SUM(H59,H54,H43,H39,H25,H23), 2)</f>
         <v>4.18</v>
       </c>
-      <c r="I61" s="82">
-        <f t="shared" ref="I61:M61" si="2">ROUNDUP(SUM(I59,I54,I43,I39,I25,I23), 2)</f>
+      <c r="I61" s="74">
+        <f t="shared" ref="I61:N61" si="2">ROUNDUP(SUM(I59,I54,I43,I39,I25,I23), 2)</f>
         <v>3.4699999999999998</v>
       </c>
-      <c r="J61" s="82">
+      <c r="J61" s="74">
         <f t="shared" si="2"/>
         <v>3.75</v>
       </c>
-      <c r="K61" s="82">
+      <c r="K61" s="74">
         <f t="shared" si="2"/>
         <v>3.23</v>
       </c>
-      <c r="L61" s="82">
+      <c r="L61" s="74">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="M61" s="82">
+      <c r="M61" s="74">
         <f t="shared" si="2"/>
         <v>2.5399999999999996</v>
       </c>
+      <c r="N61" s="74">
+        <f t="shared" si="2"/>
+        <v>3.3699999999999997</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="E55:E58"/>
-    <mergeCell ref="F55:F58"/>
-    <mergeCell ref="I30:I35"/>
-    <mergeCell ref="A61:E61"/>
-    <mergeCell ref="G55:G58"/>
-    <mergeCell ref="B3:B22"/>
-    <mergeCell ref="B30:B37"/>
-    <mergeCell ref="A55:A58"/>
-    <mergeCell ref="B55:B58"/>
-    <mergeCell ref="C55:C58"/>
-    <mergeCell ref="M55:M58"/>
-    <mergeCell ref="I46:I53"/>
-    <mergeCell ref="K46:K53"/>
-    <mergeCell ref="L46:L53"/>
-    <mergeCell ref="M46:M53"/>
-    <mergeCell ref="K55:K58"/>
-    <mergeCell ref="L55:L58"/>
-    <mergeCell ref="I55:I58"/>
+  <mergeCells count="35">
+    <mergeCell ref="N30:N35"/>
+    <mergeCell ref="N46:N53"/>
+    <mergeCell ref="N55:N58"/>
     <mergeCell ref="K30:K35"/>
     <mergeCell ref="L30:L35"/>
     <mergeCell ref="M30:M35"/>
@@ -3747,6 +3887,24 @@
     <mergeCell ref="E30:E35"/>
     <mergeCell ref="F30:F35"/>
     <mergeCell ref="J30:J35"/>
+    <mergeCell ref="M55:M58"/>
+    <mergeCell ref="I46:I53"/>
+    <mergeCell ref="K46:K53"/>
+    <mergeCell ref="L46:L53"/>
+    <mergeCell ref="M46:M53"/>
+    <mergeCell ref="K55:K58"/>
+    <mergeCell ref="L55:L58"/>
+    <mergeCell ref="I55:I58"/>
+    <mergeCell ref="B3:B22"/>
+    <mergeCell ref="B30:B37"/>
+    <mergeCell ref="A55:A58"/>
+    <mergeCell ref="B55:B58"/>
+    <mergeCell ref="C55:C58"/>
+    <mergeCell ref="E55:E58"/>
+    <mergeCell ref="F55:F58"/>
+    <mergeCell ref="I30:I35"/>
+    <mergeCell ref="A61:E61"/>
+    <mergeCell ref="G55:G58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3762,73 +3920,75 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:E16"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5" style="37" customWidth="1"/>
-    <col min="2" max="2" width="21.1640625" style="20" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="35.6640625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="25.1640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" style="33" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="35.7109375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" style="3" customWidth="1"/>
-    <col min="9" max="9" width="17.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.83203125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="13.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" style="3" customWidth="1"/>
-    <col min="13" max="13" width="17.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.83203125" style="2"/>
-    <col min="15" max="16384" width="10.83203125" style="3"/>
+    <col min="13" max="13" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" style="2"/>
+    <col min="15" max="16384" width="10.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="20">
-      <c r="A1" s="89" t="s">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+      <c r="A1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="90" t="s">
+      <c r="B1" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="91" t="s">
+      <c r="C1" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="92" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="91" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="91" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="93" t="s">
+      <c r="D1" s="84" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="83" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="83" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="94" t="s">
+      <c r="H1" s="86" t="s">
         <v>102</v>
       </c>
-      <c r="I1" s="94" t="s">
+      <c r="I1" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="94" t="s">
+      <c r="J1" s="86" t="s">
         <v>101</v>
       </c>
-      <c r="K1" s="94" t="s">
+      <c r="K1" s="86" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="94" t="s">
+      <c r="L1" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="95" t="s">
+      <c r="M1" s="87" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="30"/>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="35"/>
+      <c r="N1" s="87" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="31"/>
       <c r="B2" s="19"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
@@ -3841,117 +4001,123 @@
       <c r="K2" s="11"/>
       <c r="L2" s="11"/>
       <c r="M2" s="13"/>
-      <c r="N2" s="69"/>
-    </row>
-    <row r="3" spans="1:14" ht="45" customHeight="1">
-      <c r="A3" s="109">
+      <c r="N2" s="13"/>
+    </row>
+    <row r="3" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="116">
         <v>1</v>
       </c>
-      <c r="B3" s="118" t="s">
+      <c r="B3" s="113" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="62"/>
-      <c r="D3" s="128" t="s">
+      <c r="C3" s="55"/>
+      <c r="D3" s="100" t="s">
         <v>91</v>
       </c>
-      <c r="E3" s="97"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="65">
-        <v>5</v>
-      </c>
-      <c r="H3" s="104">
-        <v>5</v>
-      </c>
-      <c r="I3" s="65">
-        <v>4</v>
-      </c>
-      <c r="J3" s="104">
-        <v>5</v>
-      </c>
-      <c r="K3" s="65">
-        <v>3</v>
-      </c>
-      <c r="L3" s="65">
-        <v>4</v>
-      </c>
-      <c r="M3" s="63">
-        <v>5</v>
-      </c>
-      <c r="N3" s="58"/>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="109"/>
-      <c r="B4" s="118"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="58">
+        <v>5</v>
+      </c>
+      <c r="H3" s="96">
+        <v>5</v>
+      </c>
+      <c r="I3" s="58">
+        <v>4</v>
+      </c>
+      <c r="J3" s="96">
+        <v>5</v>
+      </c>
+      <c r="K3" s="58">
+        <v>3</v>
+      </c>
+      <c r="L3" s="58">
+        <v>4</v>
+      </c>
+      <c r="M3" s="56">
+        <v>5</v>
+      </c>
+      <c r="N3" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="116"/>
+      <c r="B4" s="113"/>
       <c r="C4" s="8"/>
-      <c r="D4" s="128" t="s">
+      <c r="D4" s="100" t="s">
         <v>92</v>
       </c>
       <c r="E4" s="15"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="65">
-        <v>3</v>
-      </c>
-      <c r="H4" s="104">
-        <v>3</v>
-      </c>
-      <c r="I4" s="65">
+      <c r="F4" s="57"/>
+      <c r="G4" s="58">
+        <v>3</v>
+      </c>
+      <c r="H4" s="96">
+        <v>3</v>
+      </c>
+      <c r="I4" s="58">
         <v>1</v>
       </c>
-      <c r="J4" s="104">
-        <v>4</v>
-      </c>
-      <c r="K4" s="65">
-        <v>4</v>
-      </c>
-      <c r="L4" s="65">
+      <c r="J4" s="96">
+        <v>4</v>
+      </c>
+      <c r="K4" s="58">
+        <v>4</v>
+      </c>
+      <c r="L4" s="58">
         <v>1</v>
       </c>
-      <c r="M4" s="63">
-        <v>5</v>
-      </c>
-      <c r="N4" s="58"/>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="109"/>
-      <c r="B5" s="118"/>
+      <c r="M4" s="56">
+        <v>5</v>
+      </c>
+      <c r="N4" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="116"/>
+      <c r="B5" s="113"/>
       <c r="C5" s="8"/>
-      <c r="D5" s="128" t="s">
+      <c r="D5" s="100" t="s">
         <v>93</v>
       </c>
       <c r="E5" s="15"/>
-      <c r="F5" s="64"/>
-      <c r="G5" s="56">
-        <v>4</v>
-      </c>
-      <c r="H5" s="105">
-        <v>4</v>
-      </c>
-      <c r="I5" s="56">
-        <v>4</v>
-      </c>
-      <c r="J5" s="105">
-        <v>4</v>
-      </c>
-      <c r="K5" s="56">
-        <v>3</v>
-      </c>
-      <c r="L5" s="56">
-        <v>3</v>
-      </c>
-      <c r="M5" s="56">
+      <c r="F5" s="57"/>
+      <c r="G5" s="50">
+        <v>4</v>
+      </c>
+      <c r="H5" s="97">
+        <v>4</v>
+      </c>
+      <c r="I5" s="50">
+        <v>4</v>
+      </c>
+      <c r="J5" s="97">
+        <v>4</v>
+      </c>
+      <c r="K5" s="50">
+        <v>3</v>
+      </c>
+      <c r="L5" s="50">
+        <v>3</v>
+      </c>
+      <c r="M5" s="50">
         <v>2</v>
       </c>
-      <c r="N5" s="58"/>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="109"/>
-      <c r="B6" s="118"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="100"/>
-      <c r="E6" s="97"/>
-      <c r="F6" s="64"/>
+      <c r="N5" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="116"/>
+      <c r="B6" s="113"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="92"/>
+      <c r="E6" s="89"/>
+      <c r="F6" s="57"/>
       <c r="G6" s="21">
-        <f t="shared" ref="G6:M6" si="0">AVERAGE(G4:G5)</f>
+        <f t="shared" ref="G6:N6" si="0">AVERAGE(G4:G5)</f>
         <v>3.5</v>
       </c>
       <c r="H6" s="21">
@@ -3978,22 +4144,25 @@
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="N6" s="58"/>
-    </row>
-    <row r="7" spans="1:14" s="52" customFormat="1" ht="18">
-      <c r="A7" s="47"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="50">
+      <c r="N6" s="22">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="47" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="43"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="46">
         <v>50</v>
       </c>
-      <c r="G7" s="99">
+      <c r="G7" s="91">
         <f>G6 * F7 / 100</f>
         <v>1.75</v>
       </c>
-      <c r="H7" s="99">
+      <c r="H7" s="91">
         <f>H6 * F7 / 100</f>
         <v>1.75</v>
       </c>
@@ -4017,120 +4186,129 @@
         <f>M6 * F7 / 100</f>
         <v>1.75</v>
       </c>
-      <c r="N7" s="51"/>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8" s="109">
+      <c r="N7" s="27">
+        <f>N6 * F7 / 100</f>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="116">
         <v>2</v>
       </c>
-      <c r="B8" s="118" t="s">
+      <c r="B8" s="113" t="s">
         <v>94</v>
       </c>
-      <c r="C8" s="62"/>
-      <c r="D8" s="129" t="s">
+      <c r="C8" s="55"/>
+      <c r="D8" s="101" t="s">
         <v>95</v>
       </c>
-      <c r="E8" s="46"/>
-      <c r="F8" s="64"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="57"/>
       <c r="G8" s="13">
         <v>3</v>
       </c>
-      <c r="H8" s="104">
-        <v>4</v>
-      </c>
-      <c r="I8" s="65">
+      <c r="H8" s="96">
+        <v>4</v>
+      </c>
+      <c r="I8" s="58">
         <v>1</v>
       </c>
-      <c r="J8" s="104">
-        <v>4</v>
-      </c>
-      <c r="K8" s="65">
+      <c r="J8" s="96">
+        <v>4</v>
+      </c>
+      <c r="K8" s="58">
         <v>2</v>
       </c>
-      <c r="L8" s="65">
-        <v>3</v>
-      </c>
-      <c r="M8" s="63">
-        <v>5</v>
-      </c>
-      <c r="N8" s="58"/>
-    </row>
-    <row r="9" spans="1:14" s="4" customFormat="1" ht="45">
-      <c r="A9" s="109"/>
-      <c r="B9" s="118"/>
+      <c r="L8" s="58">
+        <v>3</v>
+      </c>
+      <c r="M8" s="56">
+        <v>5</v>
+      </c>
+      <c r="N8" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="4" customFormat="1" ht="47.25" x14ac:dyDescent="0.3">
+      <c r="A9" s="116"/>
+      <c r="B9" s="113"/>
       <c r="C9" s="8"/>
-      <c r="D9" s="98" t="s">
+      <c r="D9" s="90" t="s">
         <v>96</v>
       </c>
-      <c r="E9" s="46"/>
-      <c r="F9" s="64"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="57"/>
       <c r="G9" s="13">
         <v>3</v>
       </c>
-      <c r="H9" s="104">
-        <v>4</v>
-      </c>
-      <c r="I9" s="65">
-        <v>3</v>
-      </c>
-      <c r="J9" s="104">
-        <v>4</v>
-      </c>
-      <c r="K9" s="65">
-        <v>4</v>
-      </c>
-      <c r="L9" s="65">
+      <c r="H9" s="96">
+        <v>4</v>
+      </c>
+      <c r="I9" s="58">
+        <v>3</v>
+      </c>
+      <c r="J9" s="96">
+        <v>4</v>
+      </c>
+      <c r="K9" s="58">
+        <v>4</v>
+      </c>
+      <c r="L9" s="58">
         <v>2</v>
       </c>
-      <c r="M9" s="63">
-        <v>5</v>
-      </c>
-      <c r="N9" s="31"/>
-    </row>
-    <row r="10" spans="1:14" ht="30">
-      <c r="A10" s="109"/>
-      <c r="B10" s="118"/>
+      <c r="M9" s="56">
+        <v>5</v>
+      </c>
+      <c r="N9" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="116"/>
+      <c r="B10" s="113"/>
       <c r="C10" s="8"/>
-      <c r="D10" s="101" t="s">
+      <c r="D10" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="E10" s="46"/>
-      <c r="F10" s="64"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="57"/>
       <c r="G10" s="13">
         <v>4</v>
       </c>
-      <c r="H10" s="106">
-        <v>4</v>
-      </c>
-      <c r="I10" s="56">
+      <c r="H10" s="98">
+        <v>4</v>
+      </c>
+      <c r="I10" s="50">
         <v>1</v>
       </c>
-      <c r="J10" s="105">
+      <c r="J10" s="97">
         <v>2</v>
       </c>
-      <c r="K10" s="56">
-        <v>5</v>
-      </c>
-      <c r="L10" s="56">
-        <v>3</v>
-      </c>
-      <c r="M10" s="56">
-        <v>5</v>
-      </c>
-      <c r="N10" s="58"/>
-    </row>
-    <row r="11" spans="1:14" s="5" customFormat="1">
-      <c r="A11" s="109"/>
-      <c r="B11" s="118"/>
-      <c r="C11" s="62"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="45">
+      <c r="K10" s="50">
+        <v>5</v>
+      </c>
+      <c r="L10" s="50">
+        <v>3</v>
+      </c>
+      <c r="M10" s="50">
+        <v>5</v>
+      </c>
+      <c r="N10" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="116"/>
+      <c r="B11" s="113"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="41">
         <f>AVERAGE(G9:G10)</f>
         <v>3.5</v>
       </c>
-      <c r="H11" s="45">
+      <c r="H11" s="41">
         <f>AVERAGE(H9:H10)</f>
         <v>4</v>
       </c>
@@ -4154,22 +4332,25 @@
         <f>AVERAGE(M9:M10)</f>
         <v>5</v>
       </c>
-      <c r="N11" s="32"/>
-    </row>
-    <row r="12" spans="1:14" s="54" customFormat="1" ht="18">
-      <c r="A12" s="47"/>
-      <c r="B12" s="48"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="50">
+      <c r="N11" s="22">
+        <f>AVERAGE(N9:N10)</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="48" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="43"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="46">
         <v>30</v>
       </c>
-      <c r="G12" s="99">
+      <c r="G12" s="91">
         <f>G11 * F12 / 100</f>
         <v>1.05</v>
       </c>
-      <c r="H12" s="99">
+      <c r="H12" s="91">
         <f>H11 * F12 / 100</f>
         <v>1.2</v>
       </c>
@@ -4193,19 +4374,22 @@
         <f>M11 * F12 / 100</f>
         <v>1.5</v>
       </c>
-      <c r="N12" s="53"/>
-    </row>
-    <row r="13" spans="1:14" s="4" customFormat="1" ht="18">
-      <c r="A13" s="60">
-        <v>3</v>
-      </c>
-      <c r="B13" s="66" t="s">
+      <c r="N12" s="27">
+        <f>N11 * F12 / 100</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="53">
+        <v>3</v>
+      </c>
+      <c r="B13" s="59" t="s">
         <v>98</v>
       </c>
-      <c r="C13" s="63"/>
-      <c r="D13" s="63"/>
-      <c r="E13" s="63"/>
-      <c r="F13" s="63"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="56"/>
       <c r="G13">
         <v>5</v>
       </c>
@@ -4223,15 +4407,17 @@
       <c r="M13">
         <v>5</v>
       </c>
-      <c r="N13" s="58"/>
-    </row>
-    <row r="14" spans="1:14" s="54" customFormat="1" ht="18">
-      <c r="A14" s="47"/>
-      <c r="B14" s="48"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="50">
+      <c r="N13" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="48" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="43"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="46">
         <v>20</v>
       </c>
       <c r="G14" s="26">
@@ -4260,37 +4446,40 @@
         <f>M13 * F14 / 100</f>
         <v>1</v>
       </c>
-      <c r="N14" s="51"/>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="A15" s="36"/>
+      <c r="N14" s="27">
+        <f>N13 * F14 / 100</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="32"/>
       <c r="B15" s="18"/>
       <c r="C15" s="8"/>
-      <c r="D15" s="63"/>
+      <c r="D15" s="56"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
-      <c r="G15" s="57"/>
-      <c r="H15" s="104"/>
-      <c r="I15" s="65"/>
-      <c r="J15" s="104"/>
-      <c r="K15" s="65"/>
-      <c r="L15" s="65"/>
-      <c r="M15" s="63"/>
-      <c r="N15" s="58"/>
-    </row>
-    <row r="16" spans="1:14" ht="20">
-      <c r="A16" s="126" t="s">
+      <c r="G15" s="51"/>
+      <c r="H15" s="96"/>
+      <c r="I15" s="58"/>
+      <c r="J15" s="96"/>
+      <c r="K15" s="58"/>
+      <c r="L15" s="58"/>
+      <c r="M15" s="56"/>
+      <c r="N15" s="13"/>
+    </row>
+    <row r="16" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A16" s="121" t="s">
         <v>89</v>
       </c>
-      <c r="B16" s="127"/>
-      <c r="C16" s="127"/>
-      <c r="D16" s="127"/>
-      <c r="E16" s="127"/>
+      <c r="B16" s="122"/>
+      <c r="C16" s="122"/>
+      <c r="D16" s="122"/>
+      <c r="E16" s="122"/>
       <c r="F16" s="28">
         <v>100</v>
       </c>
       <c r="G16" s="29">
-        <f t="shared" ref="G16:M16" si="1">ROUNDUP(SUM(G7,G12,G14), 2)</f>
+        <f t="shared" ref="G16:N16" si="1">ROUNDUP(SUM(G7,G12,G14), 2)</f>
         <v>3.8</v>
       </c>
       <c r="H16" s="29">
@@ -4317,9 +4506,12 @@
         <f t="shared" si="1"/>
         <v>4.25</v>
       </c>
-      <c r="N16" s="33"/>
-    </row>
-    <row r="20" spans="4:4">
+      <c r="N16" s="29">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D20" s="7" t="s">
         <v>103</v>
       </c>
@@ -4346,149 +4538,157 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20">
-      <c r="A1" s="42"/>
-      <c r="B1" s="39" t="s">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="38"/>
+      <c r="B1" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-    </row>
-    <row r="2" spans="1:5" ht="20">
-      <c r="A2" s="40" t="s">
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+    </row>
+    <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="41">
+      <c r="B2" s="37">
         <f>Adoption!G16</f>
         <v>3.8</v>
       </c>
-      <c r="C2" s="41">
+      <c r="C2" s="37">
         <f>Capabilities!G61</f>
         <v>4.0999999999999996</v>
       </c>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-    </row>
-    <row r="3" spans="1:5" ht="20">
-      <c r="A3" s="40" t="s">
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+    </row>
+    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A3" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="41">
+      <c r="B3" s="37">
         <v>3.95</v>
       </c>
-      <c r="C3" s="41">
+      <c r="C3" s="37">
         <v>4.18</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-    </row>
-    <row r="4" spans="1:5" ht="20">
-      <c r="A4" s="40" t="s">
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+    </row>
+    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A4" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="41">
+      <c r="B4" s="37">
         <f>Adoption!I16</f>
         <v>2.85</v>
       </c>
-      <c r="C4" s="41">
+      <c r="C4" s="37">
         <f>Capabilities!I61</f>
         <v>3.4699999999999998</v>
       </c>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-    </row>
-    <row r="5" spans="1:5" ht="20">
-      <c r="A5" s="40" t="s">
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+    </row>
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A5" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="B5" s="41">
-        <v>4</v>
-      </c>
-      <c r="C5" s="41">
+      <c r="B5" s="37">
+        <v>4</v>
+      </c>
+      <c r="C5" s="37">
         <v>3.75</v>
       </c>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-    </row>
-    <row r="6" spans="1:5" ht="20">
-      <c r="A6" s="40" t="s">
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+    </row>
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A6" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="55">
+      <c r="B6" s="49">
         <f>Adoption!K16</f>
         <v>4.0999999999999996</v>
       </c>
-      <c r="C6" s="41">
+      <c r="C6" s="37">
         <f>Capabilities!K61</f>
         <v>3.23</v>
       </c>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-    </row>
-    <row r="7" spans="1:5" ht="20">
-      <c r="A7" s="40" t="s">
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+    </row>
+    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A7" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="55">
+      <c r="B7" s="49">
         <f>Adoption!L16</f>
         <v>1.95</v>
       </c>
-      <c r="C7" s="41">
+      <c r="C7" s="37">
         <f>Capabilities!L61</f>
         <v>4</v>
       </c>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-    </row>
-    <row r="8" spans="1:5" ht="20">
-      <c r="A8" s="40" t="s">
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+    </row>
+    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A8" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="55">
+      <c r="B8" s="49">
         <f>Adoption!M16</f>
         <v>4.25</v>
       </c>
-      <c r="C8" s="41">
+      <c r="C8" s="37">
         <f>Capabilities!M61</f>
         <v>2.5399999999999996</v>
       </c>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="38"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="38"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="38"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+    </row>
+    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A9" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" s="49">
+        <f>[1]Adoption!N16</f>
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="C9" s="37">
+        <f>[1]Capabilities!N61</f>
+        <v>3.3699999999999997</v>
+      </c>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="34"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="34"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Updated document after review
</commit_message>
<xml_diff>
--- a/TechWatchJSFrameworkComparison.xlsx
+++ b/TechWatchJSFrameworkComparison.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,16 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14175" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14175" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Capabilities" sheetId="1" r:id="rId1"/>
     <sheet name="Adoption" sheetId="7" r:id="rId2"/>
     <sheet name="Adoption Vs Capabilities" sheetId="2" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -350,7 +347,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -466,6 +463,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -922,7 +926,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1215,6 +1219,51 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1231,12 +1280,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1244,33 +1287,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1612,11 +1628,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="295179456"/>
-        <c:axId val="295181024"/>
+        <c:axId val="269271440"/>
+        <c:axId val="269271048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="295179456"/>
+        <c:axId val="269271440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1626,12 +1642,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="295181024"/>
+        <c:crossAx val="269271048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="295181024"/>
+        <c:axId val="269271048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1642,7 +1658,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="295179456"/>
+        <c:crossAx val="269271440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1684,7 +1700,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1705,35 +1721,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Capabilities"/>
-      <sheetName val="Adoption"/>
-      <sheetName val="Adoption Vs Capabilities"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="61">
-          <cell r="N61">
-            <v>3.3699999999999997</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1">
-        <row r="16">
-          <cell r="N16">
-            <v>4.1500000000000004</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2033,10 +2020,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N61"/>
+  <dimension ref="A1:N445"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
@@ -2122,7 +2109,7 @@
       <c r="A3" s="52">
         <v>1</v>
       </c>
-      <c r="B3" s="113" t="s">
+      <c r="B3" s="109" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="55" t="s">
@@ -2145,7 +2132,7 @@
     </row>
     <row r="4" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="52"/>
-      <c r="B4" s="113"/>
+      <c r="B4" s="109"/>
       <c r="C4" s="8"/>
       <c r="D4" s="14" t="s">
         <v>15</v>
@@ -2181,7 +2168,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="52"/>
-      <c r="B5" s="113"/>
+      <c r="B5" s="109"/>
       <c r="C5" s="8"/>
       <c r="D5" s="14" t="s">
         <v>17</v>
@@ -2217,7 +2204,7 @@
     </row>
     <row r="6" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="52"/>
-      <c r="B6" s="113"/>
+      <c r="B6" s="109"/>
       <c r="C6" s="8"/>
       <c r="D6" s="14" t="s">
         <v>19</v>
@@ -2253,7 +2240,7 @@
     </row>
     <row r="7" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="52"/>
-      <c r="B7" s="113"/>
+      <c r="B7" s="109"/>
       <c r="C7" s="8"/>
       <c r="D7" s="14" t="s">
         <v>21</v>
@@ -2289,7 +2276,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="52"/>
-      <c r="B8" s="113"/>
+      <c r="B8" s="109"/>
       <c r="C8" s="8"/>
       <c r="D8" s="14" t="s">
         <v>23</v>
@@ -2323,7 +2310,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="52"/>
-      <c r="B9" s="113"/>
+      <c r="B9" s="109"/>
       <c r="C9" s="8"/>
       <c r="D9" s="14" t="s">
         <v>24</v>
@@ -2352,12 +2339,12 @@
         <v>5</v>
       </c>
       <c r="N9" s="99">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="52"/>
-      <c r="B10" s="113"/>
+      <c r="B10" s="109"/>
       <c r="C10" s="8"/>
       <c r="D10" s="14" t="s">
         <v>25</v>
@@ -2393,7 +2380,7 @@
     </row>
     <row r="11" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="52"/>
-      <c r="B11" s="113"/>
+      <c r="B11" s="109"/>
       <c r="C11" s="8"/>
       <c r="D11" s="14" t="s">
         <v>27</v>
@@ -2424,12 +2411,12 @@
         <v>3</v>
       </c>
       <c r="N11" s="99">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="52"/>
-      <c r="B12" s="113"/>
+      <c r="B12" s="109"/>
       <c r="C12" s="8"/>
       <c r="D12" s="14" t="s">
         <v>29</v>
@@ -2458,12 +2445,12 @@
         <v>3</v>
       </c>
       <c r="N12" s="99">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="52"/>
-      <c r="B13" s="113"/>
+      <c r="B13" s="109"/>
       <c r="C13" s="8"/>
       <c r="D13" s="14" t="s">
         <v>30</v>
@@ -2491,13 +2478,13 @@
       <c r="M13" s="56">
         <v>1</v>
       </c>
-      <c r="N13" s="99">
-        <v>3</v>
+      <c r="N13" s="102">
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="52"/>
-      <c r="B14" s="113"/>
+      <c r="B14" s="109"/>
       <c r="C14" s="8"/>
       <c r="D14" s="14" t="s">
         <v>31</v>
@@ -2526,12 +2513,12 @@
         <v>1</v>
       </c>
       <c r="N14" s="99">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="52"/>
-      <c r="B15" s="113"/>
+      <c r="B15" s="109"/>
       <c r="C15" s="8"/>
       <c r="D15" s="14" t="s">
         <v>32</v>
@@ -2559,13 +2546,13 @@
       <c r="M15" s="56">
         <v>3</v>
       </c>
-      <c r="N15" s="99">
+      <c r="N15" s="102">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="52"/>
-      <c r="B16" s="113"/>
+      <c r="B16" s="109"/>
       <c r="C16" s="8"/>
       <c r="D16" s="14" t="s">
         <v>33</v>
@@ -2599,7 +2586,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="52"/>
-      <c r="B17" s="113"/>
+      <c r="B17" s="109"/>
       <c r="C17" s="8"/>
       <c r="D17" s="14" t="s">
         <v>34</v>
@@ -2627,12 +2614,12 @@
         <v>2</v>
       </c>
       <c r="N17" s="99">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="52"/>
-      <c r="B18" s="113"/>
+      <c r="B18" s="109"/>
       <c r="C18" s="8"/>
       <c r="D18" s="14" t="s">
         <v>35</v>
@@ -2666,7 +2653,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="52"/>
-      <c r="B19" s="113"/>
+      <c r="B19" s="109"/>
       <c r="C19" s="8"/>
       <c r="D19" s="14" t="s">
         <v>36</v>
@@ -2700,7 +2687,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="52"/>
-      <c r="B20" s="113"/>
+      <c r="B20" s="109"/>
       <c r="C20" s="8"/>
       <c r="D20" s="14" t="s">
         <v>37</v>
@@ -2734,7 +2721,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="52"/>
-      <c r="B21" s="113"/>
+      <c r="B21" s="109"/>
       <c r="C21" s="8"/>
       <c r="D21" s="14" t="s">
         <v>38</v>
@@ -2762,13 +2749,13 @@
       <c r="M21" s="56">
         <v>1</v>
       </c>
-      <c r="N21" s="99">
-        <v>3</v>
+      <c r="N21" s="103">
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="53"/>
-      <c r="B22" s="114"/>
+      <c r="B22" s="110"/>
       <c r="C22" s="56"/>
       <c r="D22" s="14"/>
       <c r="E22" s="16"/>
@@ -2803,7 +2790,7 @@
       </c>
       <c r="N22" s="21">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>4.4444444444444446</v>
       </c>
     </row>
     <row r="23" spans="1:14" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
@@ -2845,7 +2832,7 @@
       </c>
       <c r="N23" s="27">
         <f>N22 * F23 / 100</f>
-        <v>1.2</v>
+        <v>1.3333333333333335</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
@@ -3017,136 +3004,136 @@
       <c r="N29" s="99"/>
     </row>
     <row r="30" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A30" s="116">
-        <v>5</v>
-      </c>
-      <c r="B30" s="113" t="s">
+      <c r="A30" s="112">
+        <v>5</v>
+      </c>
+      <c r="B30" s="109" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="103" t="s">
+      <c r="C30" s="118" t="s">
         <v>50</v>
       </c>
       <c r="D30" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="E30" s="103" t="s">
+      <c r="E30" s="118" t="s">
         <v>52</v>
       </c>
-      <c r="F30" s="106"/>
-      <c r="G30" s="108">
+      <c r="F30" s="121"/>
+      <c r="G30" s="104">
         <v>4</v>
       </c>
       <c r="H30" s="94"/>
-      <c r="I30" s="108">
+      <c r="I30" s="104">
         <v>2</v>
       </c>
-      <c r="J30" s="108">
+      <c r="J30" s="104">
         <v>0</v>
       </c>
-      <c r="K30" s="108">
-        <v>3</v>
-      </c>
-      <c r="L30" s="108">
-        <v>4</v>
-      </c>
-      <c r="M30" s="108">
-        <v>3</v>
-      </c>
-      <c r="N30" s="108">
+      <c r="K30" s="104">
+        <v>3</v>
+      </c>
+      <c r="L30" s="104">
+        <v>4</v>
+      </c>
+      <c r="M30" s="104">
+        <v>3</v>
+      </c>
+      <c r="N30" s="104">
         <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="116"/>
-      <c r="B31" s="113"/>
-      <c r="C31" s="103"/>
+      <c r="A31" s="112"/>
+      <c r="B31" s="109"/>
+      <c r="C31" s="118"/>
       <c r="D31" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E31" s="103"/>
-      <c r="F31" s="106"/>
-      <c r="G31" s="108"/>
+      <c r="E31" s="118"/>
+      <c r="F31" s="121"/>
+      <c r="G31" s="104"/>
       <c r="H31" s="94"/>
-      <c r="I31" s="108"/>
-      <c r="J31" s="108"/>
-      <c r="K31" s="108"/>
-      <c r="L31" s="108"/>
-      <c r="M31" s="108"/>
-      <c r="N31" s="108"/>
+      <c r="I31" s="104"/>
+      <c r="J31" s="104"/>
+      <c r="K31" s="104"/>
+      <c r="L31" s="104"/>
+      <c r="M31" s="104"/>
+      <c r="N31" s="104"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="116"/>
-      <c r="B32" s="113"/>
-      <c r="C32" s="103"/>
+      <c r="A32" s="112"/>
+      <c r="B32" s="109"/>
+      <c r="C32" s="118"/>
       <c r="D32" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E32" s="103"/>
-      <c r="F32" s="106"/>
-      <c r="G32" s="108"/>
+      <c r="E32" s="118"/>
+      <c r="F32" s="121"/>
+      <c r="G32" s="104"/>
       <c r="H32" s="94"/>
-      <c r="I32" s="108"/>
-      <c r="J32" s="108"/>
-      <c r="K32" s="108"/>
-      <c r="L32" s="108"/>
-      <c r="M32" s="108"/>
-      <c r="N32" s="108"/>
+      <c r="I32" s="104"/>
+      <c r="J32" s="104"/>
+      <c r="K32" s="104"/>
+      <c r="L32" s="104"/>
+      <c r="M32" s="104"/>
+      <c r="N32" s="104"/>
     </row>
     <row r="33" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="116"/>
-      <c r="B33" s="113"/>
-      <c r="C33" s="103"/>
+      <c r="A33" s="112"/>
+      <c r="B33" s="109"/>
+      <c r="C33" s="118"/>
       <c r="D33" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E33" s="103"/>
-      <c r="F33" s="106"/>
-      <c r="G33" s="108"/>
+      <c r="E33" s="118"/>
+      <c r="F33" s="121"/>
+      <c r="G33" s="104"/>
       <c r="H33" s="94"/>
-      <c r="I33" s="108"/>
-      <c r="J33" s="108"/>
-      <c r="K33" s="108"/>
-      <c r="L33" s="108"/>
-      <c r="M33" s="108"/>
-      <c r="N33" s="108"/>
+      <c r="I33" s="104"/>
+      <c r="J33" s="104"/>
+      <c r="K33" s="104"/>
+      <c r="L33" s="104"/>
+      <c r="M33" s="104"/>
+      <c r="N33" s="104"/>
     </row>
     <row r="34" spans="1:14" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="116"/>
-      <c r="B34" s="113"/>
-      <c r="C34" s="103"/>
+      <c r="A34" s="112"/>
+      <c r="B34" s="109"/>
+      <c r="C34" s="118"/>
       <c r="D34" s="9"/>
-      <c r="E34" s="103"/>
-      <c r="F34" s="106"/>
-      <c r="G34" s="108"/>
+      <c r="E34" s="118"/>
+      <c r="F34" s="121"/>
+      <c r="G34" s="104"/>
       <c r="H34" s="94"/>
-      <c r="I34" s="108"/>
-      <c r="J34" s="108"/>
-      <c r="K34" s="108"/>
-      <c r="L34" s="108"/>
-      <c r="M34" s="108"/>
-      <c r="N34" s="108"/>
+      <c r="I34" s="104"/>
+      <c r="J34" s="104"/>
+      <c r="K34" s="104"/>
+      <c r="L34" s="104"/>
+      <c r="M34" s="104"/>
+      <c r="N34" s="104"/>
     </row>
     <row r="35" spans="1:14" ht="63" x14ac:dyDescent="0.25">
-      <c r="A35" s="116"/>
-      <c r="B35" s="113"/>
-      <c r="C35" s="103"/>
+      <c r="A35" s="112"/>
+      <c r="B35" s="109"/>
+      <c r="C35" s="118"/>
       <c r="D35" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="E35" s="104"/>
-      <c r="F35" s="107"/>
-      <c r="G35" s="109"/>
+      <c r="E35" s="119"/>
+      <c r="F35" s="122"/>
+      <c r="G35" s="105"/>
       <c r="H35" s="95"/>
-      <c r="I35" s="109"/>
-      <c r="J35" s="109"/>
-      <c r="K35" s="109"/>
-      <c r="L35" s="109"/>
-      <c r="M35" s="109"/>
-      <c r="N35" s="109"/>
+      <c r="I35" s="105"/>
+      <c r="J35" s="105"/>
+      <c r="K35" s="105"/>
+      <c r="L35" s="105"/>
+      <c r="M35" s="105"/>
+      <c r="N35" s="105"/>
     </row>
     <row r="36" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A36" s="52"/>
-      <c r="B36" s="113"/>
+      <c r="B36" s="109"/>
       <c r="C36" s="8"/>
       <c r="D36" s="12" t="s">
         <v>57</v>
@@ -3180,7 +3167,7 @@
     </row>
     <row r="37" spans="1:14" ht="63" x14ac:dyDescent="0.25">
       <c r="A37" s="53"/>
-      <c r="B37" s="114"/>
+      <c r="B37" s="110"/>
       <c r="C37" s="56"/>
       <c r="D37" s="40" t="s">
         <v>58</v>
@@ -3461,13 +3448,13 @@
       <c r="M45" s="13"/>
     </row>
     <row r="46" spans="1:14" s="4" customFormat="1" ht="95.25" x14ac:dyDescent="0.3">
-      <c r="A46" s="116">
+      <c r="A46" s="112">
         <v>9</v>
       </c>
-      <c r="B46" s="119" t="s">
+      <c r="B46" s="115" t="s">
         <v>71</v>
       </c>
-      <c r="C46" s="103" t="s">
+      <c r="C46" s="118" t="s">
         <v>72</v>
       </c>
       <c r="D46" s="60" t="s">
@@ -3476,157 +3463,157 @@
       <c r="E46" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="F46" s="106"/>
-      <c r="G46" s="108">
+      <c r="F46" s="121"/>
+      <c r="G46" s="104">
         <v>4</v>
       </c>
       <c r="H46" s="94"/>
-      <c r="I46" s="108">
+      <c r="I46" s="104">
         <v>5</v>
       </c>
       <c r="J46" s="94"/>
-      <c r="K46" s="108">
+      <c r="K46" s="104">
         <v>2</v>
       </c>
-      <c r="L46" s="108">
-        <v>3</v>
-      </c>
-      <c r="M46" s="108">
-        <v>4</v>
-      </c>
-      <c r="N46" s="108">
+      <c r="L46" s="104">
+        <v>3</v>
+      </c>
+      <c r="M46" s="104">
+        <v>4</v>
+      </c>
+      <c r="N46" s="106">
         <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="157.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="116"/>
-      <c r="B47" s="119"/>
-      <c r="C47" s="103"/>
+      <c r="A47" s="112"/>
+      <c r="B47" s="115"/>
+      <c r="C47" s="118"/>
       <c r="D47" s="9" t="s">
         <v>75</v>
       </c>
       <c r="E47" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="F47" s="106"/>
-      <c r="G47" s="108"/>
+      <c r="F47" s="121"/>
+      <c r="G47" s="104"/>
       <c r="H47" s="94"/>
-      <c r="I47" s="108"/>
+      <c r="I47" s="104"/>
       <c r="J47" s="94"/>
-      <c r="K47" s="108"/>
-      <c r="L47" s="108"/>
-      <c r="M47" s="108"/>
-      <c r="N47" s="108"/>
+      <c r="K47" s="104"/>
+      <c r="L47" s="104"/>
+      <c r="M47" s="104"/>
+      <c r="N47" s="106"/>
     </row>
     <row r="48" spans="1:14" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A48" s="116"/>
-      <c r="B48" s="119"/>
-      <c r="C48" s="103"/>
+      <c r="A48" s="112"/>
+      <c r="B48" s="115"/>
+      <c r="C48" s="118"/>
       <c r="D48" s="9" t="s">
         <v>77</v>
       </c>
       <c r="E48" s="17"/>
-      <c r="F48" s="106"/>
-      <c r="G48" s="108"/>
+      <c r="F48" s="121"/>
+      <c r="G48" s="104"/>
       <c r="H48" s="94"/>
-      <c r="I48" s="108"/>
+      <c r="I48" s="104"/>
       <c r="J48" s="94"/>
-      <c r="K48" s="108"/>
-      <c r="L48" s="108"/>
-      <c r="M48" s="108"/>
-      <c r="N48" s="108"/>
+      <c r="K48" s="104"/>
+      <c r="L48" s="104"/>
+      <c r="M48" s="104"/>
+      <c r="N48" s="106"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="116"/>
-      <c r="B49" s="119"/>
-      <c r="C49" s="103"/>
+      <c r="A49" s="112"/>
+      <c r="B49" s="115"/>
+      <c r="C49" s="118"/>
       <c r="D49" s="10"/>
       <c r="E49" s="17"/>
-      <c r="F49" s="106"/>
-      <c r="G49" s="108"/>
+      <c r="F49" s="121"/>
+      <c r="G49" s="104"/>
       <c r="H49" s="94"/>
-      <c r="I49" s="108"/>
+      <c r="I49" s="104"/>
       <c r="J49" s="94"/>
-      <c r="K49" s="108"/>
-      <c r="L49" s="108"/>
-      <c r="M49" s="108"/>
-      <c r="N49" s="108"/>
+      <c r="K49" s="104"/>
+      <c r="L49" s="104"/>
+      <c r="M49" s="104"/>
+      <c r="N49" s="106"/>
     </row>
     <row r="50" spans="1:14" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A50" s="116"/>
-      <c r="B50" s="119"/>
-      <c r="C50" s="103"/>
+      <c r="A50" s="112"/>
+      <c r="B50" s="115"/>
+      <c r="C50" s="118"/>
       <c r="D50" s="9" t="s">
         <v>78</v>
       </c>
       <c r="E50" s="17"/>
-      <c r="F50" s="106"/>
-      <c r="G50" s="108"/>
+      <c r="F50" s="121"/>
+      <c r="G50" s="104"/>
       <c r="H50" s="94"/>
-      <c r="I50" s="108"/>
+      <c r="I50" s="104"/>
       <c r="J50" s="94"/>
-      <c r="K50" s="108"/>
-      <c r="L50" s="108"/>
-      <c r="M50" s="108"/>
-      <c r="N50" s="108"/>
+      <c r="K50" s="104"/>
+      <c r="L50" s="104"/>
+      <c r="M50" s="104"/>
+      <c r="N50" s="106"/>
     </row>
     <row r="51" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="116"/>
-      <c r="B51" s="119"/>
-      <c r="C51" s="103"/>
+      <c r="A51" s="112"/>
+      <c r="B51" s="115"/>
+      <c r="C51" s="118"/>
       <c r="D51" s="9" t="s">
         <v>79</v>
       </c>
       <c r="E51" s="17"/>
-      <c r="F51" s="106"/>
-      <c r="G51" s="108"/>
+      <c r="F51" s="121"/>
+      <c r="G51" s="104"/>
       <c r="H51" s="94"/>
-      <c r="I51" s="108"/>
+      <c r="I51" s="104"/>
       <c r="J51" s="94"/>
-      <c r="K51" s="108"/>
-      <c r="L51" s="108"/>
-      <c r="M51" s="108"/>
-      <c r="N51" s="108"/>
+      <c r="K51" s="104"/>
+      <c r="L51" s="104"/>
+      <c r="M51" s="104"/>
+      <c r="N51" s="106"/>
     </row>
     <row r="52" spans="1:14" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A52" s="116"/>
-      <c r="B52" s="119"/>
-      <c r="C52" s="103"/>
+      <c r="A52" s="112"/>
+      <c r="B52" s="115"/>
+      <c r="C52" s="118"/>
       <c r="D52" s="9" t="s">
         <v>80</v>
       </c>
       <c r="E52" s="17"/>
-      <c r="F52" s="106"/>
-      <c r="G52" s="108"/>
+      <c r="F52" s="121"/>
+      <c r="G52" s="104"/>
       <c r="H52" s="94"/>
-      <c r="I52" s="108"/>
+      <c r="I52" s="104"/>
       <c r="J52" s="94"/>
-      <c r="K52" s="108"/>
-      <c r="L52" s="108"/>
-      <c r="M52" s="108"/>
-      <c r="N52" s="108"/>
+      <c r="K52" s="104"/>
+      <c r="L52" s="104"/>
+      <c r="M52" s="104"/>
+      <c r="N52" s="106"/>
     </row>
     <row r="53" spans="1:14" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="117"/>
-      <c r="B53" s="120"/>
-      <c r="C53" s="104"/>
+      <c r="A53" s="113"/>
+      <c r="B53" s="116"/>
+      <c r="C53" s="119"/>
       <c r="D53" s="60" t="s">
         <v>81</v>
       </c>
       <c r="E53" s="17"/>
-      <c r="F53" s="107"/>
-      <c r="G53" s="109"/>
+      <c r="F53" s="122"/>
+      <c r="G53" s="105"/>
       <c r="H53" s="95">
         <v>4</v>
       </c>
-      <c r="I53" s="109"/>
+      <c r="I53" s="105"/>
       <c r="J53" s="95">
         <v>5</v>
       </c>
-      <c r="K53" s="109"/>
-      <c r="L53" s="109"/>
-      <c r="M53" s="109"/>
-      <c r="N53" s="109"/>
+      <c r="K53" s="105"/>
+      <c r="L53" s="105"/>
+      <c r="M53" s="105"/>
+      <c r="N53" s="107"/>
     </row>
     <row r="54" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A54" s="43"/>
@@ -3671,100 +3658,100 @@
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" s="115">
+      <c r="A55" s="111">
         <v>10</v>
       </c>
-      <c r="B55" s="118" t="s">
+      <c r="B55" s="114" t="s">
         <v>82</v>
       </c>
-      <c r="C55" s="102" t="s">
+      <c r="C55" s="117" t="s">
         <v>83</v>
       </c>
       <c r="D55" s="60" t="s">
         <v>84</v>
       </c>
-      <c r="E55" s="102" t="s">
+      <c r="E55" s="117" t="s">
         <v>85</v>
       </c>
-      <c r="F55" s="105"/>
-      <c r="G55" s="112">
+      <c r="F55" s="120"/>
+      <c r="G55" s="108">
         <v>4</v>
       </c>
       <c r="H55" s="97"/>
-      <c r="I55" s="112">
+      <c r="I55" s="108">
         <v>3</v>
       </c>
       <c r="J55" s="97"/>
-      <c r="K55" s="112">
-        <v>3</v>
-      </c>
-      <c r="L55" s="112">
-        <v>5</v>
-      </c>
-      <c r="M55" s="112">
+      <c r="K55" s="108">
+        <v>3</v>
+      </c>
+      <c r="L55" s="108">
+        <v>5</v>
+      </c>
+      <c r="M55" s="108">
         <v>2</v>
       </c>
-      <c r="N55" s="112">
+      <c r="N55" s="108">
         <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" s="116"/>
-      <c r="B56" s="119"/>
-      <c r="C56" s="103"/>
+      <c r="A56" s="112"/>
+      <c r="B56" s="115"/>
+      <c r="C56" s="118"/>
       <c r="D56" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="E56" s="103"/>
-      <c r="F56" s="106"/>
-      <c r="G56" s="108"/>
+      <c r="E56" s="118"/>
+      <c r="F56" s="121"/>
+      <c r="G56" s="104"/>
       <c r="H56" s="94"/>
-      <c r="I56" s="108"/>
+      <c r="I56" s="104"/>
       <c r="J56" s="94"/>
-      <c r="K56" s="108"/>
-      <c r="L56" s="108"/>
-      <c r="M56" s="108"/>
-      <c r="N56" s="108"/>
+      <c r="K56" s="104"/>
+      <c r="L56" s="104"/>
+      <c r="M56" s="104"/>
+      <c r="N56" s="104"/>
     </row>
     <row r="57" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A57" s="116"/>
-      <c r="B57" s="119"/>
-      <c r="C57" s="103"/>
+      <c r="A57" s="112"/>
+      <c r="B57" s="115"/>
+      <c r="C57" s="118"/>
       <c r="D57" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="E57" s="103"/>
-      <c r="F57" s="106"/>
-      <c r="G57" s="108"/>
+      <c r="E57" s="118"/>
+      <c r="F57" s="121"/>
+      <c r="G57" s="104"/>
       <c r="H57" s="94"/>
-      <c r="I57" s="108"/>
+      <c r="I57" s="104"/>
       <c r="J57" s="94"/>
-      <c r="K57" s="108"/>
-      <c r="L57" s="108"/>
-      <c r="M57" s="108"/>
-      <c r="N57" s="108"/>
+      <c r="K57" s="104"/>
+      <c r="L57" s="104"/>
+      <c r="M57" s="104"/>
+      <c r="N57" s="104"/>
     </row>
     <row r="58" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A58" s="117"/>
-      <c r="B58" s="120"/>
-      <c r="C58" s="104"/>
+      <c r="A58" s="113"/>
+      <c r="B58" s="116"/>
+      <c r="C58" s="119"/>
       <c r="D58" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="E58" s="104"/>
-      <c r="F58" s="107"/>
-      <c r="G58" s="109"/>
+      <c r="E58" s="119"/>
+      <c r="F58" s="122"/>
+      <c r="G58" s="105"/>
       <c r="H58" s="95">
         <v>4</v>
       </c>
-      <c r="I58" s="109"/>
+      <c r="I58" s="105"/>
       <c r="J58" s="95">
         <v>3</v>
       </c>
-      <c r="K58" s="109"/>
-      <c r="L58" s="109"/>
-      <c r="M58" s="109"/>
-      <c r="N58" s="109"/>
+      <c r="K58" s="105"/>
+      <c r="L58" s="105"/>
+      <c r="M58" s="105"/>
+      <c r="N58" s="105"/>
     </row>
     <row r="59" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A59" s="67"/>
@@ -3824,13 +3811,13 @@
       <c r="M60" s="13"/>
     </row>
     <row r="61" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A61" s="110" t="s">
+      <c r="A61" s="123" t="s">
         <v>89</v>
       </c>
-      <c r="B61" s="111"/>
-      <c r="C61" s="111"/>
-      <c r="D61" s="111"/>
-      <c r="E61" s="111"/>
+      <c r="B61" s="124"/>
+      <c r="C61" s="124"/>
+      <c r="D61" s="124"/>
+      <c r="E61" s="124"/>
       <c r="F61" s="73">
         <f>SUM(F59,F54,F43,F39,F25,F23)</f>
         <v>100</v>
@@ -3844,7 +3831,7 @@
         <v>4.18</v>
       </c>
       <c r="I61" s="74">
-        <f t="shared" ref="I61:N61" si="2">ROUNDUP(SUM(I59,I54,I43,I39,I25,I23), 2)</f>
+        <f t="shared" ref="I61:M61" si="2">ROUNDUP(SUM(I59,I54,I43,I39,I25,I23), 2)</f>
         <v>3.4699999999999998</v>
       </c>
       <c r="J61" s="74">
@@ -3864,28 +3851,1184 @@
         <v>2.5399999999999996</v>
       </c>
       <c r="N61" s="74">
-        <f t="shared" si="2"/>
-        <v>3.3699999999999997</v>
-      </c>
+        <f>ROUNDUP(SUM(N59,N54,N43,N39,N25,N23), 2)</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N62" s="3"/>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N63" s="3"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N64" s="3"/>
+    </row>
+    <row r="65" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N65" s="3"/>
+    </row>
+    <row r="66" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N66" s="3"/>
+    </row>
+    <row r="67" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N67" s="3"/>
+    </row>
+    <row r="68" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N68" s="3"/>
+    </row>
+    <row r="69" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N69" s="3"/>
+    </row>
+    <row r="70" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N70" s="3"/>
+    </row>
+    <row r="71" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N71" s="3"/>
+    </row>
+    <row r="72" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N72" s="3"/>
+    </row>
+    <row r="73" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N73" s="3"/>
+    </row>
+    <row r="74" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N74" s="3"/>
+    </row>
+    <row r="75" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N75" s="3"/>
+    </row>
+    <row r="76" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N76" s="3"/>
+    </row>
+    <row r="77" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N77" s="3"/>
+    </row>
+    <row r="78" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N78" s="3"/>
+    </row>
+    <row r="79" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N79" s="3"/>
+    </row>
+    <row r="80" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N80" s="3"/>
+    </row>
+    <row r="81" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N81" s="3"/>
+    </row>
+    <row r="82" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N82" s="3"/>
+    </row>
+    <row r="83" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N83" s="3"/>
+    </row>
+    <row r="84" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N84" s="3"/>
+    </row>
+    <row r="85" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N85" s="3"/>
+    </row>
+    <row r="86" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N86" s="3"/>
+    </row>
+    <row r="87" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N87" s="3"/>
+    </row>
+    <row r="88" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N88" s="3"/>
+    </row>
+    <row r="89" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N89" s="3"/>
+    </row>
+    <row r="90" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N90" s="3"/>
+    </row>
+    <row r="91" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N91" s="3"/>
+    </row>
+    <row r="92" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N92" s="3"/>
+    </row>
+    <row r="93" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N93" s="3"/>
+    </row>
+    <row r="94" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N94" s="3"/>
+    </row>
+    <row r="95" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N95" s="3"/>
+    </row>
+    <row r="96" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N96" s="3"/>
+    </row>
+    <row r="97" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N97" s="3"/>
+    </row>
+    <row r="98" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N98" s="3"/>
+    </row>
+    <row r="99" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N99" s="3"/>
+    </row>
+    <row r="100" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N100" s="3"/>
+    </row>
+    <row r="101" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N101" s="3"/>
+    </row>
+    <row r="102" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N102" s="3"/>
+    </row>
+    <row r="103" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N103" s="3"/>
+    </row>
+    <row r="104" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N104" s="3"/>
+    </row>
+    <row r="105" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N105" s="3"/>
+    </row>
+    <row r="106" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N106" s="3"/>
+    </row>
+    <row r="107" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N107" s="3"/>
+    </row>
+    <row r="108" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N108" s="3"/>
+    </row>
+    <row r="109" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N109" s="3"/>
+    </row>
+    <row r="110" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N110" s="3"/>
+    </row>
+    <row r="111" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N111" s="3"/>
+    </row>
+    <row r="112" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N112" s="3"/>
+    </row>
+    <row r="113" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N113" s="3"/>
+    </row>
+    <row r="114" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N114" s="3"/>
+    </row>
+    <row r="115" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N115" s="3"/>
+    </row>
+    <row r="116" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N116" s="3"/>
+    </row>
+    <row r="117" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N117" s="3"/>
+    </row>
+    <row r="118" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N118" s="3"/>
+    </row>
+    <row r="119" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N119" s="3"/>
+    </row>
+    <row r="120" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N120" s="3"/>
+    </row>
+    <row r="121" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N121" s="3"/>
+    </row>
+    <row r="122" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N122" s="3"/>
+    </row>
+    <row r="123" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N123" s="3"/>
+    </row>
+    <row r="124" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N124" s="3"/>
+    </row>
+    <row r="125" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N125" s="3"/>
+    </row>
+    <row r="126" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N126" s="3"/>
+    </row>
+    <row r="127" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N127" s="3"/>
+    </row>
+    <row r="128" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N128" s="3"/>
+    </row>
+    <row r="129" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N129" s="3"/>
+    </row>
+    <row r="130" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N130" s="3"/>
+    </row>
+    <row r="131" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N131" s="3"/>
+    </row>
+    <row r="132" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N132" s="3"/>
+    </row>
+    <row r="133" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N133" s="3"/>
+    </row>
+    <row r="134" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N134" s="3"/>
+    </row>
+    <row r="135" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N135" s="3"/>
+    </row>
+    <row r="136" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N136" s="3"/>
+    </row>
+    <row r="137" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N137" s="3"/>
+    </row>
+    <row r="138" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N138" s="3"/>
+    </row>
+    <row r="139" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N139" s="3"/>
+    </row>
+    <row r="140" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N140" s="3"/>
+    </row>
+    <row r="141" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N141" s="3"/>
+    </row>
+    <row r="142" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N142" s="3"/>
+    </row>
+    <row r="143" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N143" s="3"/>
+    </row>
+    <row r="144" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N144" s="3"/>
+    </row>
+    <row r="145" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N145" s="3"/>
+    </row>
+    <row r="146" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N146" s="3"/>
+    </row>
+    <row r="147" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N147" s="3"/>
+    </row>
+    <row r="148" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N148" s="3"/>
+    </row>
+    <row r="149" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N149" s="3"/>
+    </row>
+    <row r="150" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N150" s="3"/>
+    </row>
+    <row r="151" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N151" s="3"/>
+    </row>
+    <row r="152" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N152" s="3"/>
+    </row>
+    <row r="153" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N153" s="3"/>
+    </row>
+    <row r="154" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N154" s="3"/>
+    </row>
+    <row r="155" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N155" s="3"/>
+    </row>
+    <row r="156" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N156" s="3"/>
+    </row>
+    <row r="157" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N157" s="3"/>
+    </row>
+    <row r="158" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N158" s="3"/>
+    </row>
+    <row r="159" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N159" s="3"/>
+    </row>
+    <row r="160" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N160" s="3"/>
+    </row>
+    <row r="161" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N161" s="3"/>
+    </row>
+    <row r="162" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N162" s="3"/>
+    </row>
+    <row r="163" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N163" s="3"/>
+    </row>
+    <row r="164" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N164" s="3"/>
+    </row>
+    <row r="165" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N165" s="3"/>
+    </row>
+    <row r="166" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N166" s="3"/>
+    </row>
+    <row r="167" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N167" s="3"/>
+    </row>
+    <row r="168" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N168" s="3"/>
+    </row>
+    <row r="169" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N169" s="3"/>
+    </row>
+    <row r="170" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N170" s="3"/>
+    </row>
+    <row r="171" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N171" s="3"/>
+    </row>
+    <row r="172" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N172" s="3"/>
+    </row>
+    <row r="173" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N173" s="3"/>
+    </row>
+    <row r="174" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N174" s="3"/>
+    </row>
+    <row r="175" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N175" s="3"/>
+    </row>
+    <row r="176" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N176" s="3"/>
+    </row>
+    <row r="177" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N177" s="3"/>
+    </row>
+    <row r="178" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N178" s="3"/>
+    </row>
+    <row r="179" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N179" s="3"/>
+    </row>
+    <row r="180" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N180" s="3"/>
+    </row>
+    <row r="181" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N181" s="3"/>
+    </row>
+    <row r="182" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N182" s="3"/>
+    </row>
+    <row r="183" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N183" s="3"/>
+    </row>
+    <row r="184" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N184" s="3"/>
+    </row>
+    <row r="185" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N185" s="3"/>
+    </row>
+    <row r="186" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N186" s="3"/>
+    </row>
+    <row r="187" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N187" s="3"/>
+    </row>
+    <row r="188" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N188" s="3"/>
+    </row>
+    <row r="189" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N189" s="3"/>
+    </row>
+    <row r="190" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N190" s="3"/>
+    </row>
+    <row r="191" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N191" s="3"/>
+    </row>
+    <row r="192" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N192" s="3"/>
+    </row>
+    <row r="193" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N193" s="3"/>
+    </row>
+    <row r="194" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N194" s="3"/>
+    </row>
+    <row r="195" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N195" s="3"/>
+    </row>
+    <row r="196" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N196" s="3"/>
+    </row>
+    <row r="197" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N197" s="3"/>
+    </row>
+    <row r="198" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N198" s="3"/>
+    </row>
+    <row r="199" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N199" s="3"/>
+    </row>
+    <row r="200" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N200" s="3"/>
+    </row>
+    <row r="201" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N201" s="3"/>
+    </row>
+    <row r="202" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N202" s="3"/>
+    </row>
+    <row r="203" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N203" s="3"/>
+    </row>
+    <row r="204" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N204" s="3"/>
+    </row>
+    <row r="205" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N205" s="3"/>
+    </row>
+    <row r="206" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N206" s="3"/>
+    </row>
+    <row r="207" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N207" s="3"/>
+    </row>
+    <row r="208" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N208" s="3"/>
+    </row>
+    <row r="209" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N209" s="3"/>
+    </row>
+    <row r="210" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N210" s="3"/>
+    </row>
+    <row r="211" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N211" s="3"/>
+    </row>
+    <row r="212" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N212" s="3"/>
+    </row>
+    <row r="213" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N213" s="3"/>
+    </row>
+    <row r="214" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N214" s="3"/>
+    </row>
+    <row r="215" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N215" s="3"/>
+    </row>
+    <row r="216" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N216" s="3"/>
+    </row>
+    <row r="217" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N217" s="3"/>
+    </row>
+    <row r="218" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N218" s="3"/>
+    </row>
+    <row r="219" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N219" s="3"/>
+    </row>
+    <row r="220" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N220" s="3"/>
+    </row>
+    <row r="221" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N221" s="3"/>
+    </row>
+    <row r="222" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N222" s="3"/>
+    </row>
+    <row r="223" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N223" s="3"/>
+    </row>
+    <row r="224" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N224" s="3"/>
+    </row>
+    <row r="225" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N225" s="3"/>
+    </row>
+    <row r="226" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N226" s="3"/>
+    </row>
+    <row r="227" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N227" s="3"/>
+    </row>
+    <row r="228" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N228" s="3"/>
+    </row>
+    <row r="229" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N229" s="3"/>
+    </row>
+    <row r="230" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N230" s="3"/>
+    </row>
+    <row r="231" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N231" s="3"/>
+    </row>
+    <row r="232" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N232" s="3"/>
+    </row>
+    <row r="233" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N233" s="3"/>
+    </row>
+    <row r="234" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N234" s="3"/>
+    </row>
+    <row r="235" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N235" s="3"/>
+    </row>
+    <row r="236" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N236" s="3"/>
+    </row>
+    <row r="237" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N237" s="3"/>
+    </row>
+    <row r="238" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N238" s="3"/>
+    </row>
+    <row r="239" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N239" s="3"/>
+    </row>
+    <row r="240" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N240" s="3"/>
+    </row>
+    <row r="241" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N241" s="3"/>
+    </row>
+    <row r="242" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N242" s="3"/>
+    </row>
+    <row r="243" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N243" s="3"/>
+    </row>
+    <row r="244" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N244" s="3"/>
+    </row>
+    <row r="245" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N245" s="3"/>
+    </row>
+    <row r="246" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N246" s="3"/>
+    </row>
+    <row r="247" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N247" s="3"/>
+    </row>
+    <row r="248" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N248" s="3"/>
+    </row>
+    <row r="249" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N249" s="3"/>
+    </row>
+    <row r="250" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N250" s="3"/>
+    </row>
+    <row r="251" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N251" s="3"/>
+    </row>
+    <row r="252" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N252" s="3"/>
+    </row>
+    <row r="253" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N253" s="3"/>
+    </row>
+    <row r="254" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N254" s="3"/>
+    </row>
+    <row r="255" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N255" s="3"/>
+    </row>
+    <row r="256" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N256" s="3"/>
+    </row>
+    <row r="257" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N257" s="3"/>
+    </row>
+    <row r="258" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N258" s="3"/>
+    </row>
+    <row r="259" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N259" s="3"/>
+    </row>
+    <row r="260" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N260" s="3"/>
+    </row>
+    <row r="261" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N261" s="3"/>
+    </row>
+    <row r="262" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N262" s="3"/>
+    </row>
+    <row r="263" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N263" s="3"/>
+    </row>
+    <row r="264" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N264" s="3"/>
+    </row>
+    <row r="265" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N265" s="3"/>
+    </row>
+    <row r="266" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N266" s="3"/>
+    </row>
+    <row r="267" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N267" s="3"/>
+    </row>
+    <row r="268" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N268" s="3"/>
+    </row>
+    <row r="269" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N269" s="3"/>
+    </row>
+    <row r="270" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N270" s="3"/>
+    </row>
+    <row r="271" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N271" s="3"/>
+    </row>
+    <row r="272" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N272" s="3"/>
+    </row>
+    <row r="273" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N273" s="3"/>
+    </row>
+    <row r="274" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N274" s="3"/>
+    </row>
+    <row r="275" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N275" s="3"/>
+    </row>
+    <row r="276" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N276" s="3"/>
+    </row>
+    <row r="277" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N277" s="3"/>
+    </row>
+    <row r="278" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N278" s="3"/>
+    </row>
+    <row r="279" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N279" s="3"/>
+    </row>
+    <row r="280" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N280" s="3"/>
+    </row>
+    <row r="281" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N281" s="3"/>
+    </row>
+    <row r="282" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N282" s="3"/>
+    </row>
+    <row r="283" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N283" s="3"/>
+    </row>
+    <row r="284" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N284" s="3"/>
+    </row>
+    <row r="285" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N285" s="3"/>
+    </row>
+    <row r="286" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N286" s="3"/>
+    </row>
+    <row r="287" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N287" s="3"/>
+    </row>
+    <row r="288" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N288" s="3"/>
+    </row>
+    <row r="289" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N289" s="3"/>
+    </row>
+    <row r="290" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N290" s="3"/>
+    </row>
+    <row r="291" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N291" s="3"/>
+    </row>
+    <row r="292" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N292" s="3"/>
+    </row>
+    <row r="293" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N293" s="3"/>
+    </row>
+    <row r="294" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N294" s="3"/>
+    </row>
+    <row r="295" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N295" s="3"/>
+    </row>
+    <row r="296" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N296" s="3"/>
+    </row>
+    <row r="297" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N297" s="3"/>
+    </row>
+    <row r="298" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N298" s="3"/>
+    </row>
+    <row r="299" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N299" s="3"/>
+    </row>
+    <row r="300" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N300" s="3"/>
+    </row>
+    <row r="301" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N301" s="3"/>
+    </row>
+    <row r="302" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N302" s="3"/>
+    </row>
+    <row r="303" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N303" s="3"/>
+    </row>
+    <row r="304" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N304" s="3"/>
+    </row>
+    <row r="305" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N305" s="3"/>
+    </row>
+    <row r="306" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N306" s="3"/>
+    </row>
+    <row r="307" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N307" s="3"/>
+    </row>
+    <row r="308" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N308" s="3"/>
+    </row>
+    <row r="309" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N309" s="3"/>
+    </row>
+    <row r="310" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N310" s="3"/>
+    </row>
+    <row r="311" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N311" s="3"/>
+    </row>
+    <row r="312" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N312" s="3"/>
+    </row>
+    <row r="313" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N313" s="3"/>
+    </row>
+    <row r="314" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N314" s="3"/>
+    </row>
+    <row r="315" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N315" s="3"/>
+    </row>
+    <row r="316" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N316" s="3"/>
+    </row>
+    <row r="317" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N317" s="3"/>
+    </row>
+    <row r="318" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N318" s="3"/>
+    </row>
+    <row r="319" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N319" s="3"/>
+    </row>
+    <row r="320" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N320" s="3"/>
+    </row>
+    <row r="321" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N321" s="3"/>
+    </row>
+    <row r="322" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N322" s="3"/>
+    </row>
+    <row r="323" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N323" s="3"/>
+    </row>
+    <row r="324" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N324" s="3"/>
+    </row>
+    <row r="325" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N325" s="3"/>
+    </row>
+    <row r="326" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N326" s="3"/>
+    </row>
+    <row r="327" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N327" s="3"/>
+    </row>
+    <row r="328" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N328" s="3"/>
+    </row>
+    <row r="329" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N329" s="3"/>
+    </row>
+    <row r="330" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N330" s="3"/>
+    </row>
+    <row r="331" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N331" s="3"/>
+    </row>
+    <row r="332" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N332" s="3"/>
+    </row>
+    <row r="333" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N333" s="3"/>
+    </row>
+    <row r="334" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N334" s="3"/>
+    </row>
+    <row r="335" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N335" s="3"/>
+    </row>
+    <row r="336" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N336" s="3"/>
+    </row>
+    <row r="337" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N337" s="3"/>
+    </row>
+    <row r="338" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N338" s="3"/>
+    </row>
+    <row r="339" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N339" s="3"/>
+    </row>
+    <row r="340" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N340" s="3"/>
+    </row>
+    <row r="341" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N341" s="3"/>
+    </row>
+    <row r="342" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N342" s="3"/>
+    </row>
+    <row r="343" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N343" s="3"/>
+    </row>
+    <row r="344" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N344" s="3"/>
+    </row>
+    <row r="345" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N345" s="3"/>
+    </row>
+    <row r="346" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N346" s="3"/>
+    </row>
+    <row r="347" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N347" s="3"/>
+    </row>
+    <row r="348" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N348" s="3"/>
+    </row>
+    <row r="349" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N349" s="3"/>
+    </row>
+    <row r="350" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N350" s="3"/>
+    </row>
+    <row r="351" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N351" s="3"/>
+    </row>
+    <row r="352" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N352" s="3"/>
+    </row>
+    <row r="353" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N353" s="3"/>
+    </row>
+    <row r="354" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N354" s="3"/>
+    </row>
+    <row r="355" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N355" s="3"/>
+    </row>
+    <row r="356" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N356" s="3"/>
+    </row>
+    <row r="357" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N357" s="3"/>
+    </row>
+    <row r="358" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N358" s="3"/>
+    </row>
+    <row r="359" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N359" s="3"/>
+    </row>
+    <row r="360" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N360" s="3"/>
+    </row>
+    <row r="361" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N361" s="3"/>
+    </row>
+    <row r="362" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N362" s="3"/>
+    </row>
+    <row r="363" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N363" s="3"/>
+    </row>
+    <row r="364" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N364" s="3"/>
+    </row>
+    <row r="365" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N365" s="3"/>
+    </row>
+    <row r="366" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N366" s="3"/>
+    </row>
+    <row r="367" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N367" s="3"/>
+    </row>
+    <row r="368" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N368" s="3"/>
+    </row>
+    <row r="369" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N369" s="3"/>
+    </row>
+    <row r="370" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N370" s="3"/>
+    </row>
+    <row r="371" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N371" s="3"/>
+    </row>
+    <row r="372" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N372" s="3"/>
+    </row>
+    <row r="373" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N373" s="3"/>
+    </row>
+    <row r="374" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N374" s="3"/>
+    </row>
+    <row r="375" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N375" s="3"/>
+    </row>
+    <row r="376" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N376" s="3"/>
+    </row>
+    <row r="377" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N377" s="3"/>
+    </row>
+    <row r="378" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N378" s="3"/>
+    </row>
+    <row r="379" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N379" s="3"/>
+    </row>
+    <row r="380" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N380" s="3"/>
+    </row>
+    <row r="381" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N381" s="3"/>
+    </row>
+    <row r="382" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N382" s="3"/>
+    </row>
+    <row r="383" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N383" s="3"/>
+    </row>
+    <row r="384" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N384" s="3"/>
+    </row>
+    <row r="385" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N385" s="3"/>
+    </row>
+    <row r="386" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N386" s="3"/>
+    </row>
+    <row r="387" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N387" s="3"/>
+    </row>
+    <row r="388" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N388" s="3"/>
+    </row>
+    <row r="389" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N389" s="3"/>
+    </row>
+    <row r="390" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N390" s="3"/>
+    </row>
+    <row r="391" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N391" s="3"/>
+    </row>
+    <row r="392" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N392" s="3"/>
+    </row>
+    <row r="393" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N393" s="3"/>
+    </row>
+    <row r="394" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N394" s="3"/>
+    </row>
+    <row r="395" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N395" s="3"/>
+    </row>
+    <row r="396" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N396" s="3"/>
+    </row>
+    <row r="397" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N397" s="3"/>
+    </row>
+    <row r="398" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N398" s="3"/>
+    </row>
+    <row r="399" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N399" s="3"/>
+    </row>
+    <row r="400" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N400" s="3"/>
+    </row>
+    <row r="401" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N401" s="3"/>
+    </row>
+    <row r="402" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N402" s="3"/>
+    </row>
+    <row r="403" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N403" s="3"/>
+    </row>
+    <row r="404" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N404" s="3"/>
+    </row>
+    <row r="405" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N405" s="3"/>
+    </row>
+    <row r="406" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N406" s="3"/>
+    </row>
+    <row r="407" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N407" s="3"/>
+    </row>
+    <row r="408" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N408" s="3"/>
+    </row>
+    <row r="409" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N409" s="3"/>
+    </row>
+    <row r="410" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N410" s="3"/>
+    </row>
+    <row r="411" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N411" s="3"/>
+    </row>
+    <row r="412" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N412" s="3"/>
+    </row>
+    <row r="413" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N413" s="3"/>
+    </row>
+    <row r="414" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N414" s="3"/>
+    </row>
+    <row r="415" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N415" s="3"/>
+    </row>
+    <row r="416" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N416" s="3"/>
+    </row>
+    <row r="417" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N417" s="3"/>
+    </row>
+    <row r="418" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N418" s="3"/>
+    </row>
+    <row r="419" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N419" s="3"/>
+    </row>
+    <row r="420" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N420" s="3"/>
+    </row>
+    <row r="421" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N421" s="3"/>
+    </row>
+    <row r="422" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N422" s="3"/>
+    </row>
+    <row r="423" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N423" s="3"/>
+    </row>
+    <row r="424" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N424" s="3"/>
+    </row>
+    <row r="425" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N425" s="3"/>
+    </row>
+    <row r="426" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N426" s="3"/>
+    </row>
+    <row r="427" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N427" s="3"/>
+    </row>
+    <row r="428" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N428" s="3"/>
+    </row>
+    <row r="429" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N429" s="3"/>
+    </row>
+    <row r="430" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N430" s="3"/>
+    </row>
+    <row r="431" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N431" s="3"/>
+    </row>
+    <row r="432" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N432" s="3"/>
+    </row>
+    <row r="433" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N433" s="3"/>
+    </row>
+    <row r="434" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N434" s="3"/>
+    </row>
+    <row r="435" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N435" s="3"/>
+    </row>
+    <row r="436" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N436" s="3"/>
+    </row>
+    <row r="437" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N437" s="3"/>
+    </row>
+    <row r="438" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N438" s="3"/>
+    </row>
+    <row r="439" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N439" s="3"/>
+    </row>
+    <row r="440" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N440" s="3"/>
+    </row>
+    <row r="441" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N441" s="3"/>
+    </row>
+    <row r="442" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N442" s="3"/>
+    </row>
+    <row r="443" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N443" s="3"/>
+    </row>
+    <row r="444" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N444" s="3"/>
+    </row>
+    <row r="445" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N445" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="N30:N35"/>
-    <mergeCell ref="N46:N53"/>
-    <mergeCell ref="N55:N58"/>
-    <mergeCell ref="K30:K35"/>
-    <mergeCell ref="L30:L35"/>
-    <mergeCell ref="M30:M35"/>
+    <mergeCell ref="E55:E58"/>
+    <mergeCell ref="F55:F58"/>
+    <mergeCell ref="I30:I35"/>
+    <mergeCell ref="A61:E61"/>
+    <mergeCell ref="G55:G58"/>
+    <mergeCell ref="G30:G35"/>
+    <mergeCell ref="E30:E35"/>
+    <mergeCell ref="F30:F35"/>
+    <mergeCell ref="F46:F53"/>
+    <mergeCell ref="G46:G53"/>
+    <mergeCell ref="B3:B22"/>
+    <mergeCell ref="B30:B37"/>
+    <mergeCell ref="A55:A58"/>
+    <mergeCell ref="B55:B58"/>
+    <mergeCell ref="C55:C58"/>
+    <mergeCell ref="A30:A35"/>
+    <mergeCell ref="C30:C35"/>
     <mergeCell ref="A46:A53"/>
     <mergeCell ref="B46:B53"/>
     <mergeCell ref="C46:C53"/>
-    <mergeCell ref="F46:F53"/>
-    <mergeCell ref="G46:G53"/>
-    <mergeCell ref="G30:G35"/>
-    <mergeCell ref="A30:A35"/>
-    <mergeCell ref="C30:C35"/>
-    <mergeCell ref="E30:E35"/>
-    <mergeCell ref="F30:F35"/>
     <mergeCell ref="J30:J35"/>
     <mergeCell ref="M55:M58"/>
     <mergeCell ref="I46:I53"/>
@@ -3895,19 +5038,15 @@
     <mergeCell ref="K55:K58"/>
     <mergeCell ref="L55:L58"/>
     <mergeCell ref="I55:I58"/>
-    <mergeCell ref="B3:B22"/>
-    <mergeCell ref="B30:B37"/>
-    <mergeCell ref="A55:A58"/>
-    <mergeCell ref="B55:B58"/>
-    <mergeCell ref="C55:C58"/>
-    <mergeCell ref="E55:E58"/>
-    <mergeCell ref="F55:F58"/>
-    <mergeCell ref="I30:I35"/>
-    <mergeCell ref="A61:E61"/>
-    <mergeCell ref="G55:G58"/>
+    <mergeCell ref="N30:N35"/>
+    <mergeCell ref="N46:N53"/>
+    <mergeCell ref="N55:N58"/>
+    <mergeCell ref="K30:K35"/>
+    <mergeCell ref="L30:L35"/>
+    <mergeCell ref="M30:M35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3920,8 +5059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4004,10 +5143,10 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="116">
+      <c r="A3" s="112">
         <v>1</v>
       </c>
-      <c r="B3" s="113" t="s">
+      <c r="B3" s="109" t="s">
         <v>90</v>
       </c>
       <c r="C3" s="55"/>
@@ -4042,8 +5181,8 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="116"/>
-      <c r="B4" s="113"/>
+      <c r="A4" s="112"/>
+      <c r="B4" s="109"/>
       <c r="C4" s="8"/>
       <c r="D4" s="100" t="s">
         <v>92</v>
@@ -4076,8 +5215,8 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="116"/>
-      <c r="B5" s="113"/>
+      <c r="A5" s="112"/>
+      <c r="B5" s="109"/>
       <c r="C5" s="8"/>
       <c r="D5" s="100" t="s">
         <v>93</v>
@@ -4110,8 +5249,8 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="116"/>
-      <c r="B6" s="113"/>
+      <c r="A6" s="112"/>
+      <c r="B6" s="109"/>
       <c r="C6" s="55"/>
       <c r="D6" s="92"/>
       <c r="E6" s="89"/>
@@ -4192,10 +5331,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="116">
+      <c r="A8" s="112">
         <v>2</v>
       </c>
-      <c r="B8" s="113" t="s">
+      <c r="B8" s="109" t="s">
         <v>94</v>
       </c>
       <c r="C8" s="55"/>
@@ -4230,8 +5369,8 @@
       </c>
     </row>
     <row r="9" spans="1:14" s="4" customFormat="1" ht="47.25" x14ac:dyDescent="0.3">
-      <c r="A9" s="116"/>
-      <c r="B9" s="113"/>
+      <c r="A9" s="112"/>
+      <c r="B9" s="109"/>
       <c r="C9" s="8"/>
       <c r="D9" s="90" t="s">
         <v>96</v>
@@ -4264,8 +5403,8 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="116"/>
-      <c r="B10" s="113"/>
+      <c r="A10" s="112"/>
+      <c r="B10" s="109"/>
       <c r="C10" s="8"/>
       <c r="D10" s="93" t="s">
         <v>97</v>
@@ -4298,8 +5437,8 @@
       </c>
     </row>
     <row r="11" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="116"/>
-      <c r="B11" s="113"/>
+      <c r="A11" s="112"/>
+      <c r="B11" s="109"/>
       <c r="C11" s="55"/>
       <c r="D11" s="50"/>
       <c r="E11" s="42"/>
@@ -4468,13 +5607,13 @@
       <c r="N15" s="13"/>
     </row>
     <row r="16" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A16" s="121" t="s">
+      <c r="A16" s="125" t="s">
         <v>89</v>
       </c>
-      <c r="B16" s="122"/>
-      <c r="C16" s="122"/>
-      <c r="D16" s="122"/>
-      <c r="E16" s="122"/>
+      <c r="B16" s="126"/>
+      <c r="C16" s="126"/>
+      <c r="D16" s="126"/>
+      <c r="E16" s="126"/>
       <c r="F16" s="28">
         <v>100</v>
       </c>
@@ -4538,8 +5677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4666,12 +5805,12 @@
         <v>104</v>
       </c>
       <c r="B9" s="49">
-        <f>[1]Adoption!N16</f>
-        <v>4.1500000000000004</v>
+        <f>Adoption!N16</f>
+        <v>4</v>
       </c>
       <c r="C9" s="37">
-        <f>[1]Capabilities!N61</f>
-        <v>3.3699999999999997</v>
+        <f>Capabilities!N61</f>
+        <v>3.5</v>
       </c>
       <c r="D9" s="34"/>
       <c r="E9" s="34"/>

</xml_diff>

<commit_message>
updated score as per new code change
</commit_message>
<xml_diff>
--- a/TechWatchJSFrameworkComparison.xlsx
+++ b/TechWatchJSFrameworkComparison.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14175" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14175" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Capabilities" sheetId="1" r:id="rId1"/>
@@ -1628,11 +1628,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="269271440"/>
-        <c:axId val="269271048"/>
+        <c:axId val="259617616"/>
+        <c:axId val="259618792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="269271440"/>
+        <c:axId val="259617616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1642,12 +1642,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="269271048"/>
+        <c:crossAx val="259618792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="269271048"/>
+        <c:axId val="259618792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1658,7 +1658,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="269271440"/>
+        <c:crossAx val="259617616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2023,8 +2023,8 @@
   <dimension ref="A1:N445"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N21" sqref="N21"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N38" sqref="N38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3150,7 +3150,7 @@
         <v>2</v>
       </c>
       <c r="J36" s="96">
-        <v>2.2000000000000002</v>
+        <v>2.8</v>
       </c>
       <c r="K36" s="58">
         <v>5</v>
@@ -3162,7 +3162,7 @@
         <v>5</v>
       </c>
       <c r="N36" s="99">
-        <v>2.5</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="63" x14ac:dyDescent="0.25">
@@ -3220,7 +3220,7 @@
       </c>
       <c r="J38" s="21">
         <f t="shared" si="1"/>
-        <v>3.1</v>
+        <v>3.4</v>
       </c>
       <c r="K38" s="21">
         <f t="shared" si="1"/>
@@ -3236,7 +3236,7 @@
       </c>
       <c r="N38" s="22">
         <f t="shared" si="1"/>
-        <v>3.25</v>
+        <v>4.45</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
@@ -3262,7 +3262,7 @@
       </c>
       <c r="J39" s="26">
         <f>J38 * F39 / 100</f>
-        <v>0.77500000000000002</v>
+        <v>0.85</v>
       </c>
       <c r="K39" s="26">
         <f>K38 * F39 / 100</f>
@@ -3278,7 +3278,7 @@
       </c>
       <c r="N39" s="27">
         <f>N38 * F39 / 100</f>
-        <v>0.8125</v>
+        <v>1.1125</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="110.25" x14ac:dyDescent="0.25">
@@ -3692,7 +3692,7 @@
         <v>2</v>
       </c>
       <c r="N55" s="108">
-        <v>2</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
@@ -3746,7 +3746,7 @@
       </c>
       <c r="I58" s="105"/>
       <c r="J58" s="95">
-        <v>3</v>
+        <v>4.2</v>
       </c>
       <c r="K58" s="105"/>
       <c r="L58" s="105"/>
@@ -3776,7 +3776,7 @@
       </c>
       <c r="J59" s="71">
         <f>J58 * F59 / 100</f>
-        <v>0.9</v>
+        <v>1.26</v>
       </c>
       <c r="K59" s="71">
         <f>K55 * F59 / 100</f>
@@ -3792,7 +3792,7 @@
       </c>
       <c r="N59" s="72">
         <f>N55 * F59 / 100</f>
-        <v>0.6</v>
+        <v>1.44</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
@@ -3836,7 +3836,7 @@
       </c>
       <c r="J61" s="74">
         <f t="shared" si="2"/>
-        <v>3.75</v>
+        <v>4.18</v>
       </c>
       <c r="K61" s="74">
         <f t="shared" si="2"/>
@@ -3852,7 +3852,7 @@
       </c>
       <c r="N61" s="74">
         <f>ROUNDUP(SUM(N59,N54,N43,N39,N25,N23), 2)</f>
-        <v>3.5</v>
+        <v>4.6399999999999997</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
@@ -5059,7 +5059,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -5677,8 +5677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5810,7 +5810,7 @@
       </c>
       <c r="C9" s="37">
         <f>Capabilities!N61</f>
-        <v>3.5</v>
+        <v>4.6399999999999997</v>
       </c>
       <c r="D9" s="34"/>
       <c r="E9" s="34"/>

</xml_diff>

<commit_message>
updated document as per new stat
</commit_message>
<xml_diff>
--- a/TechWatchJSFrameworkComparison.xlsx
+++ b/TechWatchJSFrameworkComparison.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14175" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14175"/>
   </bookViews>
   <sheets>
     <sheet name="Capabilities" sheetId="1" r:id="rId1"/>
@@ -926,7 +926,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1225,20 +1225,47 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1264,29 +1291,11 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1628,11 +1637,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="259617616"/>
-        <c:axId val="259618792"/>
+        <c:axId val="247550096"/>
+        <c:axId val="247556368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="259617616"/>
+        <c:axId val="247550096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1642,12 +1651,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="259618792"/>
+        <c:crossAx val="247556368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="259618792"/>
+        <c:axId val="247556368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1658,14 +1667,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="259617616"/>
+        <c:crossAx val="247550096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1700,7 +1708,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2022,9 +2030,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N445"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N38" sqref="N38"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M69" sqref="M69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2109,7 +2117,7 @@
       <c r="A3" s="52">
         <v>1</v>
       </c>
-      <c r="B3" s="109" t="s">
+      <c r="B3" s="118" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="55" t="s">
@@ -2132,7 +2140,7 @@
     </row>
     <row r="4" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="52"/>
-      <c r="B4" s="109"/>
+      <c r="B4" s="118"/>
       <c r="C4" s="8"/>
       <c r="D4" s="14" t="s">
         <v>15</v>
@@ -2168,7 +2176,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="52"/>
-      <c r="B5" s="109"/>
+      <c r="B5" s="118"/>
       <c r="C5" s="8"/>
       <c r="D5" s="14" t="s">
         <v>17</v>
@@ -2204,7 +2212,7 @@
     </row>
     <row r="6" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="52"/>
-      <c r="B6" s="109"/>
+      <c r="B6" s="118"/>
       <c r="C6" s="8"/>
       <c r="D6" s="14" t="s">
         <v>19</v>
@@ -2240,7 +2248,7 @@
     </row>
     <row r="7" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="52"/>
-      <c r="B7" s="109"/>
+      <c r="B7" s="118"/>
       <c r="C7" s="8"/>
       <c r="D7" s="14" t="s">
         <v>21</v>
@@ -2276,7 +2284,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="52"/>
-      <c r="B8" s="109"/>
+      <c r="B8" s="118"/>
       <c r="C8" s="8"/>
       <c r="D8" s="14" t="s">
         <v>23</v>
@@ -2310,7 +2318,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="52"/>
-      <c r="B9" s="109"/>
+      <c r="B9" s="118"/>
       <c r="C9" s="8"/>
       <c r="D9" s="14" t="s">
         <v>24</v>
@@ -2344,7 +2352,7 @@
     </row>
     <row r="10" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="52"/>
-      <c r="B10" s="109"/>
+      <c r="B10" s="118"/>
       <c r="C10" s="8"/>
       <c r="D10" s="14" t="s">
         <v>25</v>
@@ -2380,7 +2388,7 @@
     </row>
     <row r="11" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="52"/>
-      <c r="B11" s="109"/>
+      <c r="B11" s="118"/>
       <c r="C11" s="8"/>
       <c r="D11" s="14" t="s">
         <v>27</v>
@@ -2416,7 +2424,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="52"/>
-      <c r="B12" s="109"/>
+      <c r="B12" s="118"/>
       <c r="C12" s="8"/>
       <c r="D12" s="14" t="s">
         <v>29</v>
@@ -2445,12 +2453,12 @@
         <v>3</v>
       </c>
       <c r="N12" s="99">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="52"/>
-      <c r="B13" s="109"/>
+      <c r="B13" s="118"/>
       <c r="C13" s="8"/>
       <c r="D13" s="14" t="s">
         <v>30</v>
@@ -2484,7 +2492,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="52"/>
-      <c r="B14" s="109"/>
+      <c r="B14" s="118"/>
       <c r="C14" s="8"/>
       <c r="D14" s="14" t="s">
         <v>31</v>
@@ -2518,7 +2526,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="52"/>
-      <c r="B15" s="109"/>
+      <c r="B15" s="118"/>
       <c r="C15" s="8"/>
       <c r="D15" s="14" t="s">
         <v>32</v>
@@ -2552,7 +2560,7 @@
     </row>
     <row r="16" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="52"/>
-      <c r="B16" s="109"/>
+      <c r="B16" s="118"/>
       <c r="C16" s="8"/>
       <c r="D16" s="14" t="s">
         <v>33</v>
@@ -2586,7 +2594,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="52"/>
-      <c r="B17" s="109"/>
+      <c r="B17" s="118"/>
       <c r="C17" s="8"/>
       <c r="D17" s="14" t="s">
         <v>34</v>
@@ -2614,12 +2622,12 @@
         <v>2</v>
       </c>
       <c r="N17" s="99">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="52"/>
-      <c r="B18" s="109"/>
+      <c r="B18" s="118"/>
       <c r="C18" s="8"/>
       <c r="D18" s="14" t="s">
         <v>35</v>
@@ -2648,12 +2656,12 @@
         <v>3</v>
       </c>
       <c r="N18" s="99">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="52"/>
-      <c r="B19" s="109"/>
+      <c r="B19" s="118"/>
       <c r="C19" s="8"/>
       <c r="D19" s="14" t="s">
         <v>36</v>
@@ -2687,7 +2695,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="52"/>
-      <c r="B20" s="109"/>
+      <c r="B20" s="118"/>
       <c r="C20" s="8"/>
       <c r="D20" s="14" t="s">
         <v>37</v>
@@ -2716,12 +2724,12 @@
         <v>3</v>
       </c>
       <c r="N20" s="99">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="52"/>
-      <c r="B21" s="109"/>
+      <c r="B21" s="118"/>
       <c r="C21" s="8"/>
       <c r="D21" s="14" t="s">
         <v>38</v>
@@ -2755,7 +2763,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="53"/>
-      <c r="B22" s="110"/>
+      <c r="B22" s="119"/>
       <c r="C22" s="56"/>
       <c r="D22" s="14"/>
       <c r="E22" s="16"/>
@@ -2790,7 +2798,7 @@
       </c>
       <c r="N22" s="21">
         <f t="shared" si="0"/>
-        <v>4.4444444444444446</v>
+        <v>4.333333333333333</v>
       </c>
     </row>
     <row r="23" spans="1:14" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
@@ -2832,7 +2840,7 @@
       </c>
       <c r="N23" s="27">
         <f>N22 * F23 / 100</f>
-        <v>1.3333333333333335</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
@@ -3004,136 +3012,138 @@
       <c r="N29" s="99"/>
     </row>
     <row r="30" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A30" s="112">
-        <v>5</v>
-      </c>
-      <c r="B30" s="109" t="s">
+      <c r="A30" s="121">
+        <v>5</v>
+      </c>
+      <c r="B30" s="118" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="118" t="s">
+      <c r="C30" s="105" t="s">
         <v>50</v>
       </c>
       <c r="D30" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="E30" s="118" t="s">
+      <c r="E30" s="105" t="s">
         <v>52</v>
       </c>
-      <c r="F30" s="121"/>
-      <c r="G30" s="104">
-        <v>4</v>
-      </c>
-      <c r="H30" s="94"/>
-      <c r="I30" s="104">
+      <c r="F30" s="108"/>
+      <c r="G30" s="110">
+        <v>4</v>
+      </c>
+      <c r="H30" s="115">
+        <v>4</v>
+      </c>
+      <c r="I30" s="110">
         <v>2</v>
       </c>
-      <c r="J30" s="104">
+      <c r="J30" s="110">
         <v>0</v>
       </c>
-      <c r="K30" s="104">
-        <v>3</v>
-      </c>
-      <c r="L30" s="104">
-        <v>4</v>
-      </c>
-      <c r="M30" s="104">
-        <v>3</v>
-      </c>
-      <c r="N30" s="104">
-        <v>2</v>
+      <c r="K30" s="110">
+        <v>3</v>
+      </c>
+      <c r="L30" s="110">
+        <v>4</v>
+      </c>
+      <c r="M30" s="110">
+        <v>3</v>
+      </c>
+      <c r="N30" s="110">
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="112"/>
-      <c r="B31" s="109"/>
-      <c r="C31" s="118"/>
+      <c r="A31" s="121"/>
+      <c r="B31" s="118"/>
+      <c r="C31" s="105"/>
       <c r="D31" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E31" s="118"/>
-      <c r="F31" s="121"/>
-      <c r="G31" s="104"/>
-      <c r="H31" s="94"/>
-      <c r="I31" s="104"/>
-      <c r="J31" s="104"/>
-      <c r="K31" s="104"/>
-      <c r="L31" s="104"/>
-      <c r="M31" s="104"/>
-      <c r="N31" s="104"/>
+      <c r="E31" s="105"/>
+      <c r="F31" s="108"/>
+      <c r="G31" s="110"/>
+      <c r="H31" s="116"/>
+      <c r="I31" s="110"/>
+      <c r="J31" s="110"/>
+      <c r="K31" s="110"/>
+      <c r="L31" s="110"/>
+      <c r="M31" s="110"/>
+      <c r="N31" s="110"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="112"/>
-      <c r="B32" s="109"/>
-      <c r="C32" s="118"/>
+      <c r="A32" s="121"/>
+      <c r="B32" s="118"/>
+      <c r="C32" s="105"/>
       <c r="D32" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E32" s="118"/>
-      <c r="F32" s="121"/>
-      <c r="G32" s="104"/>
-      <c r="H32" s="94"/>
-      <c r="I32" s="104"/>
-      <c r="J32" s="104"/>
-      <c r="K32" s="104"/>
-      <c r="L32" s="104"/>
-      <c r="M32" s="104"/>
-      <c r="N32" s="104"/>
+      <c r="E32" s="105"/>
+      <c r="F32" s="108"/>
+      <c r="G32" s="110"/>
+      <c r="H32" s="116"/>
+      <c r="I32" s="110"/>
+      <c r="J32" s="110"/>
+      <c r="K32" s="110"/>
+      <c r="L32" s="110"/>
+      <c r="M32" s="110"/>
+      <c r="N32" s="110"/>
     </row>
     <row r="33" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="112"/>
-      <c r="B33" s="109"/>
-      <c r="C33" s="118"/>
+      <c r="A33" s="121"/>
+      <c r="B33" s="118"/>
+      <c r="C33" s="105"/>
       <c r="D33" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E33" s="118"/>
-      <c r="F33" s="121"/>
-      <c r="G33" s="104"/>
-      <c r="H33" s="94"/>
-      <c r="I33" s="104"/>
-      <c r="J33" s="104"/>
-      <c r="K33" s="104"/>
-      <c r="L33" s="104"/>
-      <c r="M33" s="104"/>
-      <c r="N33" s="104"/>
+      <c r="E33" s="105"/>
+      <c r="F33" s="108"/>
+      <c r="G33" s="110"/>
+      <c r="H33" s="116"/>
+      <c r="I33" s="110"/>
+      <c r="J33" s="110"/>
+      <c r="K33" s="110"/>
+      <c r="L33" s="110"/>
+      <c r="M33" s="110"/>
+      <c r="N33" s="110"/>
     </row>
     <row r="34" spans="1:14" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="112"/>
-      <c r="B34" s="109"/>
-      <c r="C34" s="118"/>
+      <c r="A34" s="121"/>
+      <c r="B34" s="118"/>
+      <c r="C34" s="105"/>
       <c r="D34" s="9"/>
-      <c r="E34" s="118"/>
-      <c r="F34" s="121"/>
-      <c r="G34" s="104"/>
-      <c r="H34" s="94"/>
-      <c r="I34" s="104"/>
-      <c r="J34" s="104"/>
-      <c r="K34" s="104"/>
-      <c r="L34" s="104"/>
-      <c r="M34" s="104"/>
-      <c r="N34" s="104"/>
+      <c r="E34" s="105"/>
+      <c r="F34" s="108"/>
+      <c r="G34" s="110"/>
+      <c r="H34" s="116"/>
+      <c r="I34" s="110"/>
+      <c r="J34" s="110"/>
+      <c r="K34" s="110"/>
+      <c r="L34" s="110"/>
+      <c r="M34" s="110"/>
+      <c r="N34" s="110"/>
     </row>
     <row r="35" spans="1:14" ht="63" x14ac:dyDescent="0.25">
-      <c r="A35" s="112"/>
-      <c r="B35" s="109"/>
-      <c r="C35" s="118"/>
+      <c r="A35" s="121"/>
+      <c r="B35" s="118"/>
+      <c r="C35" s="105"/>
       <c r="D35" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="E35" s="119"/>
-      <c r="F35" s="122"/>
-      <c r="G35" s="105"/>
-      <c r="H35" s="95"/>
-      <c r="I35" s="105"/>
-      <c r="J35" s="105"/>
-      <c r="K35" s="105"/>
-      <c r="L35" s="105"/>
-      <c r="M35" s="105"/>
-      <c r="N35" s="105"/>
+      <c r="E35" s="106"/>
+      <c r="F35" s="109"/>
+      <c r="G35" s="111"/>
+      <c r="H35" s="117"/>
+      <c r="I35" s="111"/>
+      <c r="J35" s="111"/>
+      <c r="K35" s="111"/>
+      <c r="L35" s="111"/>
+      <c r="M35" s="111"/>
+      <c r="N35" s="111"/>
     </row>
     <row r="36" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A36" s="52"/>
-      <c r="B36" s="109"/>
+      <c r="B36" s="118"/>
       <c r="C36" s="8"/>
       <c r="D36" s="12" t="s">
         <v>57</v>
@@ -3162,12 +3172,12 @@
         <v>5</v>
       </c>
       <c r="N36" s="99">
-        <v>4.9000000000000004</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="63" x14ac:dyDescent="0.25">
       <c r="A37" s="53"/>
-      <c r="B37" s="110"/>
+      <c r="B37" s="119"/>
       <c r="C37" s="56"/>
       <c r="D37" s="40" t="s">
         <v>58</v>
@@ -3236,7 +3246,7 @@
       </c>
       <c r="N38" s="22">
         <f t="shared" si="1"/>
-        <v>4.45</v>
+        <v>4.25</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
@@ -3278,7 +3288,7 @@
       </c>
       <c r="N39" s="27">
         <f>N38 * F39 / 100</f>
-        <v>1.1125</v>
+        <v>1.0625</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="110.25" x14ac:dyDescent="0.25">
@@ -3361,7 +3371,7 @@
         <v>1</v>
       </c>
       <c r="N42" s="99">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
@@ -3403,7 +3413,7 @@
       </c>
       <c r="N43" s="27">
         <f>N42 * F43 / 100</f>
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="44" spans="1:14" s="4" customFormat="1" ht="95.25" x14ac:dyDescent="0.3">
@@ -3448,13 +3458,13 @@
       <c r="M45" s="13"/>
     </row>
     <row r="46" spans="1:14" s="4" customFormat="1" ht="95.25" x14ac:dyDescent="0.3">
-      <c r="A46" s="112">
+      <c r="A46" s="121">
         <v>9</v>
       </c>
-      <c r="B46" s="115" t="s">
+      <c r="B46" s="124" t="s">
         <v>71</v>
       </c>
-      <c r="C46" s="118" t="s">
+      <c r="C46" s="105" t="s">
         <v>72</v>
       </c>
       <c r="D46" s="60" t="s">
@@ -3463,157 +3473,157 @@
       <c r="E46" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="F46" s="121"/>
-      <c r="G46" s="104">
-        <v>4</v>
-      </c>
-      <c r="H46" s="94"/>
-      <c r="I46" s="104">
-        <v>5</v>
-      </c>
-      <c r="J46" s="94"/>
-      <c r="K46" s="104">
+      <c r="F46" s="108"/>
+      <c r="G46" s="110">
+        <v>4</v>
+      </c>
+      <c r="H46" s="115">
+        <v>4</v>
+      </c>
+      <c r="I46" s="110">
+        <v>5</v>
+      </c>
+      <c r="J46" s="114">
+        <v>5</v>
+      </c>
+      <c r="K46" s="110">
         <v>2</v>
       </c>
-      <c r="L46" s="104">
-        <v>3</v>
-      </c>
-      <c r="M46" s="104">
-        <v>4</v>
-      </c>
-      <c r="N46" s="106">
+      <c r="L46" s="110">
+        <v>3</v>
+      </c>
+      <c r="M46" s="110">
+        <v>4</v>
+      </c>
+      <c r="N46" s="126">
         <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="157.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="112"/>
-      <c r="B47" s="115"/>
-      <c r="C47" s="118"/>
+      <c r="A47" s="121"/>
+      <c r="B47" s="124"/>
+      <c r="C47" s="105"/>
       <c r="D47" s="9" t="s">
         <v>75</v>
       </c>
       <c r="E47" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="F47" s="121"/>
-      <c r="G47" s="104"/>
-      <c r="H47" s="94"/>
-      <c r="I47" s="104"/>
-      <c r="J47" s="94"/>
-      <c r="K47" s="104"/>
-      <c r="L47" s="104"/>
-      <c r="M47" s="104"/>
-      <c r="N47" s="106"/>
+      <c r="F47" s="108"/>
+      <c r="G47" s="110"/>
+      <c r="H47" s="116"/>
+      <c r="I47" s="110"/>
+      <c r="J47" s="110"/>
+      <c r="K47" s="110"/>
+      <c r="L47" s="110"/>
+      <c r="M47" s="110"/>
+      <c r="N47" s="126"/>
     </row>
     <row r="48" spans="1:14" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A48" s="112"/>
-      <c r="B48" s="115"/>
-      <c r="C48" s="118"/>
+      <c r="A48" s="121"/>
+      <c r="B48" s="124"/>
+      <c r="C48" s="105"/>
       <c r="D48" s="9" t="s">
         <v>77</v>
       </c>
       <c r="E48" s="17"/>
-      <c r="F48" s="121"/>
-      <c r="G48" s="104"/>
-      <c r="H48" s="94"/>
-      <c r="I48" s="104"/>
-      <c r="J48" s="94"/>
-      <c r="K48" s="104"/>
-      <c r="L48" s="104"/>
-      <c r="M48" s="104"/>
-      <c r="N48" s="106"/>
+      <c r="F48" s="108"/>
+      <c r="G48" s="110"/>
+      <c r="H48" s="116"/>
+      <c r="I48" s="110"/>
+      <c r="J48" s="110"/>
+      <c r="K48" s="110"/>
+      <c r="L48" s="110"/>
+      <c r="M48" s="110"/>
+      <c r="N48" s="126"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="112"/>
-      <c r="B49" s="115"/>
-      <c r="C49" s="118"/>
+      <c r="A49" s="121"/>
+      <c r="B49" s="124"/>
+      <c r="C49" s="105"/>
       <c r="D49" s="10"/>
       <c r="E49" s="17"/>
-      <c r="F49" s="121"/>
-      <c r="G49" s="104"/>
-      <c r="H49" s="94"/>
-      <c r="I49" s="104"/>
-      <c r="J49" s="94"/>
-      <c r="K49" s="104"/>
-      <c r="L49" s="104"/>
-      <c r="M49" s="104"/>
-      <c r="N49" s="106"/>
+      <c r="F49" s="108"/>
+      <c r="G49" s="110"/>
+      <c r="H49" s="116"/>
+      <c r="I49" s="110"/>
+      <c r="J49" s="110"/>
+      <c r="K49" s="110"/>
+      <c r="L49" s="110"/>
+      <c r="M49" s="110"/>
+      <c r="N49" s="126"/>
     </row>
     <row r="50" spans="1:14" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A50" s="112"/>
-      <c r="B50" s="115"/>
-      <c r="C50" s="118"/>
+      <c r="A50" s="121"/>
+      <c r="B50" s="124"/>
+      <c r="C50" s="105"/>
       <c r="D50" s="9" t="s">
         <v>78</v>
       </c>
       <c r="E50" s="17"/>
-      <c r="F50" s="121"/>
-      <c r="G50" s="104"/>
-      <c r="H50" s="94"/>
-      <c r="I50" s="104"/>
-      <c r="J50" s="94"/>
-      <c r="K50" s="104"/>
-      <c r="L50" s="104"/>
-      <c r="M50" s="104"/>
-      <c r="N50" s="106"/>
+      <c r="F50" s="108"/>
+      <c r="G50" s="110"/>
+      <c r="H50" s="116"/>
+      <c r="I50" s="110"/>
+      <c r="J50" s="110"/>
+      <c r="K50" s="110"/>
+      <c r="L50" s="110"/>
+      <c r="M50" s="110"/>
+      <c r="N50" s="126"/>
     </row>
     <row r="51" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="112"/>
-      <c r="B51" s="115"/>
-      <c r="C51" s="118"/>
+      <c r="A51" s="121"/>
+      <c r="B51" s="124"/>
+      <c r="C51" s="105"/>
       <c r="D51" s="9" t="s">
         <v>79</v>
       </c>
       <c r="E51" s="17"/>
-      <c r="F51" s="121"/>
-      <c r="G51" s="104"/>
-      <c r="H51" s="94"/>
-      <c r="I51" s="104"/>
-      <c r="J51" s="94"/>
-      <c r="K51" s="104"/>
-      <c r="L51" s="104"/>
-      <c r="M51" s="104"/>
-      <c r="N51" s="106"/>
+      <c r="F51" s="108"/>
+      <c r="G51" s="110"/>
+      <c r="H51" s="116"/>
+      <c r="I51" s="110"/>
+      <c r="J51" s="110"/>
+      <c r="K51" s="110"/>
+      <c r="L51" s="110"/>
+      <c r="M51" s="110"/>
+      <c r="N51" s="126"/>
     </row>
     <row r="52" spans="1:14" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A52" s="112"/>
-      <c r="B52" s="115"/>
-      <c r="C52" s="118"/>
+      <c r="A52" s="121"/>
+      <c r="B52" s="124"/>
+      <c r="C52" s="105"/>
       <c r="D52" s="9" t="s">
         <v>80</v>
       </c>
       <c r="E52" s="17"/>
-      <c r="F52" s="121"/>
-      <c r="G52" s="104"/>
-      <c r="H52" s="94"/>
-      <c r="I52" s="104"/>
-      <c r="J52" s="94"/>
-      <c r="K52" s="104"/>
-      <c r="L52" s="104"/>
-      <c r="M52" s="104"/>
-      <c r="N52" s="106"/>
+      <c r="F52" s="108"/>
+      <c r="G52" s="110"/>
+      <c r="H52" s="116"/>
+      <c r="I52" s="110"/>
+      <c r="J52" s="110"/>
+      <c r="K52" s="110"/>
+      <c r="L52" s="110"/>
+      <c r="M52" s="110"/>
+      <c r="N52" s="126"/>
     </row>
     <row r="53" spans="1:14" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="113"/>
-      <c r="B53" s="116"/>
-      <c r="C53" s="119"/>
+      <c r="A53" s="122"/>
+      <c r="B53" s="125"/>
+      <c r="C53" s="106"/>
       <c r="D53" s="60" t="s">
         <v>81</v>
       </c>
       <c r="E53" s="17"/>
-      <c r="F53" s="122"/>
-      <c r="G53" s="105"/>
-      <c r="H53" s="95">
-        <v>4</v>
-      </c>
-      <c r="I53" s="105"/>
-      <c r="J53" s="95">
-        <v>5</v>
-      </c>
-      <c r="K53" s="105"/>
-      <c r="L53" s="105"/>
-      <c r="M53" s="105"/>
-      <c r="N53" s="107"/>
+      <c r="F53" s="109"/>
+      <c r="G53" s="111"/>
+      <c r="H53" s="117"/>
+      <c r="I53" s="111"/>
+      <c r="J53" s="111"/>
+      <c r="K53" s="111"/>
+      <c r="L53" s="111"/>
+      <c r="M53" s="111"/>
+      <c r="N53" s="127"/>
     </row>
     <row r="54" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A54" s="43"/>
@@ -3629,7 +3639,7 @@
         <v>0.2</v>
       </c>
       <c r="H54" s="26">
-        <f>H53 * F54 / 100</f>
+        <f>H46 * F54 / 100</f>
         <v>0.2</v>
       </c>
       <c r="I54" s="26">
@@ -3637,7 +3647,7 @@
         <v>0.25</v>
       </c>
       <c r="J54" s="26">
-        <f>J53 * F54 / 100</f>
+        <f>J46 * F54 / 100</f>
         <v>0.25</v>
       </c>
       <c r="K54" s="26">
@@ -3658,100 +3668,100 @@
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" s="111">
+      <c r="A55" s="120">
         <v>10</v>
       </c>
-      <c r="B55" s="114" t="s">
+      <c r="B55" s="123" t="s">
         <v>82</v>
       </c>
-      <c r="C55" s="117" t="s">
+      <c r="C55" s="104" t="s">
         <v>83</v>
       </c>
       <c r="D55" s="60" t="s">
         <v>84</v>
       </c>
-      <c r="E55" s="117" t="s">
+      <c r="E55" s="104" t="s">
         <v>85</v>
       </c>
-      <c r="F55" s="120"/>
-      <c r="G55" s="108">
-        <v>4</v>
-      </c>
-      <c r="H55" s="97"/>
-      <c r="I55" s="108">
+      <c r="F55" s="107"/>
+      <c r="G55" s="114">
+        <v>4</v>
+      </c>
+      <c r="H55" s="114">
+        <v>4</v>
+      </c>
+      <c r="I55" s="114">
         <v>3</v>
       </c>
       <c r="J55" s="97"/>
-      <c r="K55" s="108">
-        <v>3</v>
-      </c>
-      <c r="L55" s="108">
-        <v>5</v>
-      </c>
-      <c r="M55" s="108">
+      <c r="K55" s="114">
+        <v>3</v>
+      </c>
+      <c r="L55" s="114">
+        <v>5</v>
+      </c>
+      <c r="M55" s="114">
         <v>2</v>
       </c>
-      <c r="N55" s="108">
-        <v>4.8</v>
+      <c r="N55" s="114">
+        <v>4.5</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" s="112"/>
-      <c r="B56" s="115"/>
-      <c r="C56" s="118"/>
+      <c r="A56" s="121"/>
+      <c r="B56" s="124"/>
+      <c r="C56" s="105"/>
       <c r="D56" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="E56" s="118"/>
-      <c r="F56" s="121"/>
-      <c r="G56" s="104"/>
-      <c r="H56" s="94"/>
-      <c r="I56" s="104"/>
+      <c r="E56" s="105"/>
+      <c r="F56" s="108"/>
+      <c r="G56" s="110"/>
+      <c r="H56" s="110"/>
+      <c r="I56" s="110"/>
       <c r="J56" s="94"/>
-      <c r="K56" s="104"/>
-      <c r="L56" s="104"/>
-      <c r="M56" s="104"/>
-      <c r="N56" s="104"/>
+      <c r="K56" s="110"/>
+      <c r="L56" s="110"/>
+      <c r="M56" s="110"/>
+      <c r="N56" s="110"/>
     </row>
     <row r="57" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A57" s="112"/>
-      <c r="B57" s="115"/>
-      <c r="C57" s="118"/>
+      <c r="A57" s="121"/>
+      <c r="B57" s="124"/>
+      <c r="C57" s="105"/>
       <c r="D57" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="E57" s="118"/>
-      <c r="F57" s="121"/>
-      <c r="G57" s="104"/>
-      <c r="H57" s="94"/>
-      <c r="I57" s="104"/>
+      <c r="E57" s="105"/>
+      <c r="F57" s="108"/>
+      <c r="G57" s="110"/>
+      <c r="H57" s="110"/>
+      <c r="I57" s="110"/>
       <c r="J57" s="94"/>
-      <c r="K57" s="104"/>
-      <c r="L57" s="104"/>
-      <c r="M57" s="104"/>
-      <c r="N57" s="104"/>
+      <c r="K57" s="110"/>
+      <c r="L57" s="110"/>
+      <c r="M57" s="110"/>
+      <c r="N57" s="110"/>
     </row>
     <row r="58" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A58" s="113"/>
-      <c r="B58" s="116"/>
-      <c r="C58" s="119"/>
+      <c r="A58" s="122"/>
+      <c r="B58" s="125"/>
+      <c r="C58" s="106"/>
       <c r="D58" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="E58" s="119"/>
-      <c r="F58" s="122"/>
-      <c r="G58" s="105"/>
-      <c r="H58" s="95">
-        <v>4</v>
-      </c>
-      <c r="I58" s="105"/>
+      <c r="E58" s="106"/>
+      <c r="F58" s="109"/>
+      <c r="G58" s="111"/>
+      <c r="H58" s="111"/>
+      <c r="I58" s="111"/>
       <c r="J58" s="95">
         <v>4.2</v>
       </c>
-      <c r="K58" s="105"/>
-      <c r="L58" s="105"/>
-      <c r="M58" s="105"/>
-      <c r="N58" s="105"/>
+      <c r="K58" s="111"/>
+      <c r="L58" s="111"/>
+      <c r="M58" s="111"/>
+      <c r="N58" s="111"/>
     </row>
     <row r="59" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A59" s="67"/>
@@ -3767,7 +3777,7 @@
         <v>1.2</v>
       </c>
       <c r="H59" s="71">
-        <f>H58 * F59 / 100</f>
+        <f>H55 * F59 / 100</f>
         <v>1.2</v>
       </c>
       <c r="I59" s="71">
@@ -3792,7 +3802,7 @@
       </c>
       <c r="N59" s="72">
         <f>N55 * F59 / 100</f>
-        <v>1.44</v>
+        <v>1.35</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
@@ -3811,13 +3821,13 @@
       <c r="M60" s="13"/>
     </row>
     <row r="61" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A61" s="123" t="s">
+      <c r="A61" s="112" t="s">
         <v>89</v>
       </c>
-      <c r="B61" s="124"/>
-      <c r="C61" s="124"/>
-      <c r="D61" s="124"/>
-      <c r="E61" s="124"/>
+      <c r="B61" s="113"/>
+      <c r="C61" s="113"/>
+      <c r="D61" s="113"/>
+      <c r="E61" s="113"/>
       <c r="F61" s="73">
         <f>SUM(F59,F54,F43,F39,F25,F23)</f>
         <v>100</v>
@@ -3852,7 +3862,7 @@
       </c>
       <c r="N61" s="74">
         <f>ROUNDUP(SUM(N59,N54,N43,N39,N25,N23), 2)</f>
-        <v>4.6399999999999997</v>
+        <v>4.42</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
@@ -5008,7 +5018,33 @@
       <c r="N445" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
+  <mergeCells count="39">
+    <mergeCell ref="N30:N35"/>
+    <mergeCell ref="N46:N53"/>
+    <mergeCell ref="N55:N58"/>
+    <mergeCell ref="K30:K35"/>
+    <mergeCell ref="L30:L35"/>
+    <mergeCell ref="M30:M35"/>
+    <mergeCell ref="J30:J35"/>
+    <mergeCell ref="M55:M58"/>
+    <mergeCell ref="I46:I53"/>
+    <mergeCell ref="K46:K53"/>
+    <mergeCell ref="L46:L53"/>
+    <mergeCell ref="M46:M53"/>
+    <mergeCell ref="K55:K58"/>
+    <mergeCell ref="L55:L58"/>
+    <mergeCell ref="I55:I58"/>
+    <mergeCell ref="J46:J53"/>
+    <mergeCell ref="B3:B22"/>
+    <mergeCell ref="B30:B37"/>
+    <mergeCell ref="A55:A58"/>
+    <mergeCell ref="B55:B58"/>
+    <mergeCell ref="C55:C58"/>
+    <mergeCell ref="A30:A35"/>
+    <mergeCell ref="C30:C35"/>
+    <mergeCell ref="A46:A53"/>
+    <mergeCell ref="B46:B53"/>
+    <mergeCell ref="C46:C53"/>
     <mergeCell ref="E55:E58"/>
     <mergeCell ref="F55:F58"/>
     <mergeCell ref="I30:I35"/>
@@ -5019,31 +5055,9 @@
     <mergeCell ref="F30:F35"/>
     <mergeCell ref="F46:F53"/>
     <mergeCell ref="G46:G53"/>
-    <mergeCell ref="B3:B22"/>
-    <mergeCell ref="B30:B37"/>
-    <mergeCell ref="A55:A58"/>
-    <mergeCell ref="B55:B58"/>
-    <mergeCell ref="C55:C58"/>
-    <mergeCell ref="A30:A35"/>
-    <mergeCell ref="C30:C35"/>
-    <mergeCell ref="A46:A53"/>
-    <mergeCell ref="B46:B53"/>
-    <mergeCell ref="C46:C53"/>
-    <mergeCell ref="J30:J35"/>
-    <mergeCell ref="M55:M58"/>
-    <mergeCell ref="I46:I53"/>
-    <mergeCell ref="K46:K53"/>
-    <mergeCell ref="L46:L53"/>
-    <mergeCell ref="M46:M53"/>
-    <mergeCell ref="K55:K58"/>
-    <mergeCell ref="L55:L58"/>
-    <mergeCell ref="I55:I58"/>
-    <mergeCell ref="N30:N35"/>
-    <mergeCell ref="N46:N53"/>
-    <mergeCell ref="N55:N58"/>
-    <mergeCell ref="K30:K35"/>
-    <mergeCell ref="L30:L35"/>
-    <mergeCell ref="M30:M35"/>
+    <mergeCell ref="H30:H35"/>
+    <mergeCell ref="H46:H53"/>
+    <mergeCell ref="H55:H58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
@@ -5060,7 +5074,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5078,7 +5092,7 @@
     <col min="11" max="11" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" style="3" customWidth="1"/>
     <col min="13" max="13" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" style="2"/>
+    <col min="14" max="14" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="10.85546875" style="3"/>
   </cols>
   <sheetData>
@@ -5143,10 +5157,10 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="112">
+      <c r="A3" s="121">
         <v>1</v>
       </c>
-      <c r="B3" s="109" t="s">
+      <c r="B3" s="118" t="s">
         <v>90</v>
       </c>
       <c r="C3" s="55"/>
@@ -5181,8 +5195,8 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="112"/>
-      <c r="B4" s="109"/>
+      <c r="A4" s="121"/>
+      <c r="B4" s="118"/>
       <c r="C4" s="8"/>
       <c r="D4" s="100" t="s">
         <v>92</v>
@@ -5215,8 +5229,8 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="112"/>
-      <c r="B5" s="109"/>
+      <c r="A5" s="121"/>
+      <c r="B5" s="118"/>
       <c r="C5" s="8"/>
       <c r="D5" s="100" t="s">
         <v>93</v>
@@ -5249,8 +5263,8 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="112"/>
-      <c r="B6" s="109"/>
+      <c r="A6" s="121"/>
+      <c r="B6" s="118"/>
       <c r="C6" s="55"/>
       <c r="D6" s="92"/>
       <c r="E6" s="89"/>
@@ -5331,10 +5345,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="112">
+      <c r="A8" s="121">
         <v>2</v>
       </c>
-      <c r="B8" s="109" t="s">
+      <c r="B8" s="118" t="s">
         <v>94</v>
       </c>
       <c r="C8" s="55"/>
@@ -5369,8 +5383,8 @@
       </c>
     </row>
     <row r="9" spans="1:14" s="4" customFormat="1" ht="47.25" x14ac:dyDescent="0.3">
-      <c r="A9" s="112"/>
-      <c r="B9" s="109"/>
+      <c r="A9" s="121"/>
+      <c r="B9" s="118"/>
       <c r="C9" s="8"/>
       <c r="D9" s="90" t="s">
         <v>96</v>
@@ -5399,12 +5413,12 @@
         <v>5</v>
       </c>
       <c r="N9" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="112"/>
-      <c r="B10" s="109"/>
+      <c r="A10" s="121"/>
+      <c r="B10" s="118"/>
       <c r="C10" s="8"/>
       <c r="D10" s="93" t="s">
         <v>97</v>
@@ -5433,12 +5447,12 @@
         <v>5</v>
       </c>
       <c r="N10" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="112"/>
-      <c r="B11" s="109"/>
+      <c r="A11" s="121"/>
+      <c r="B11" s="118"/>
       <c r="C11" s="55"/>
       <c r="D11" s="50"/>
       <c r="E11" s="42"/>
@@ -5472,8 +5486,8 @@
         <v>5</v>
       </c>
       <c r="N11" s="22">
-        <f>AVERAGE(N9:N10)</f>
-        <v>2.5</v>
+        <f>AVERAGE(N8:N10)</f>
+        <v>1.6666666666666667</v>
       </c>
     </row>
     <row r="12" spans="1:14" s="48" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
@@ -5515,7 +5529,7 @@
       </c>
       <c r="N12" s="27">
         <f>N11 * F12 / 100</f>
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="1:14" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
@@ -5607,13 +5621,13 @@
       <c r="N15" s="13"/>
     </row>
     <row r="16" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A16" s="125" t="s">
+      <c r="A16" s="128" t="s">
         <v>89</v>
       </c>
-      <c r="B16" s="126"/>
-      <c r="C16" s="126"/>
-      <c r="D16" s="126"/>
-      <c r="E16" s="126"/>
+      <c r="B16" s="129"/>
+      <c r="C16" s="129"/>
+      <c r="D16" s="129"/>
+      <c r="E16" s="129"/>
       <c r="F16" s="28">
         <v>100</v>
       </c>
@@ -5647,7 +5661,7 @@
       </c>
       <c r="N16" s="29">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="20" spans="4:4" x14ac:dyDescent="0.25">
@@ -5677,7 +5691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -5806,11 +5820,11 @@
       </c>
       <c r="B9" s="49">
         <f>Adoption!N16</f>
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="C9" s="37">
         <f>Capabilities!N61</f>
-        <v>4.6399999999999997</v>
+        <v>4.42</v>
       </c>
       <c r="D9" s="34"/>
       <c r="E9" s="34"/>

</xml_diff>

<commit_message>
rearranged techstacks and updated adoption score
</commit_message>
<xml_diff>
--- a/TechWatchJSFrameworkComparison.xlsx
+++ b/TechWatchJSFrameworkComparison.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14175"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14175" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Capabilities" sheetId="1" r:id="rId1"/>
@@ -1225,6 +1225,45 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1241,12 +1280,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1256,9 +1289,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1266,36 +1296,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1564,29 +1564,32 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>'Adoption Vs Capabilities'!$B$2:$B$8</c:f>
+              <c:f>'Adoption Vs Capabilities'!$B$2:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>3.8</c:v>
+                  <c:v>2.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>3.95</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.85</c:v>
+                <c:pt idx="4">
+                  <c:v>3.09</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.0999999999999996</c:v>
+                <c:pt idx="6">
+                  <c:v>2.25</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.95</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>4.25</c:v>
                 </c:pt>
               </c:numCache>
@@ -1594,29 +1597,32 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Adoption Vs Capabilities'!$C$2:$C$8</c:f>
+              <c:f>'Adoption Vs Capabilities'!$C$2:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>3.4699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>4.0999999999999996</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>4.18</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.4699999999999998</c:v>
+                <c:pt idx="4">
+                  <c:v>4.42</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.75</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>3.23</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>2.5399999999999996</c:v>
                 </c:pt>
               </c:numCache>
@@ -1637,11 +1643,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="247550096"/>
-        <c:axId val="247556368"/>
+        <c:axId val="262136976"/>
+        <c:axId val="262138152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="247550096"/>
+        <c:axId val="262136976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1651,12 +1657,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="247556368"/>
+        <c:crossAx val="262138152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="247556368"/>
+        <c:axId val="262138152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1667,13 +1673,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="247550096"/>
+        <c:crossAx val="262136976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1708,7 +1715,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2030,7 +2037,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N445"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M69" sqref="M69"/>
     </sheetView>
@@ -2117,7 +2124,7 @@
       <c r="A3" s="52">
         <v>1</v>
       </c>
-      <c r="B3" s="118" t="s">
+      <c r="B3" s="109" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="55" t="s">
@@ -2140,7 +2147,7 @@
     </row>
     <row r="4" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="52"/>
-      <c r="B4" s="118"/>
+      <c r="B4" s="109"/>
       <c r="C4" s="8"/>
       <c r="D4" s="14" t="s">
         <v>15</v>
@@ -2176,7 +2183,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="52"/>
-      <c r="B5" s="118"/>
+      <c r="B5" s="109"/>
       <c r="C5" s="8"/>
       <c r="D5" s="14" t="s">
         <v>17</v>
@@ -2212,7 +2219,7 @@
     </row>
     <row r="6" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="52"/>
-      <c r="B6" s="118"/>
+      <c r="B6" s="109"/>
       <c r="C6" s="8"/>
       <c r="D6" s="14" t="s">
         <v>19</v>
@@ -2248,7 +2255,7 @@
     </row>
     <row r="7" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="52"/>
-      <c r="B7" s="118"/>
+      <c r="B7" s="109"/>
       <c r="C7" s="8"/>
       <c r="D7" s="14" t="s">
         <v>21</v>
@@ -2284,7 +2291,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="52"/>
-      <c r="B8" s="118"/>
+      <c r="B8" s="109"/>
       <c r="C8" s="8"/>
       <c r="D8" s="14" t="s">
         <v>23</v>
@@ -2318,7 +2325,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="52"/>
-      <c r="B9" s="118"/>
+      <c r="B9" s="109"/>
       <c r="C9" s="8"/>
       <c r="D9" s="14" t="s">
         <v>24</v>
@@ -2352,7 +2359,7 @@
     </row>
     <row r="10" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="52"/>
-      <c r="B10" s="118"/>
+      <c r="B10" s="109"/>
       <c r="C10" s="8"/>
       <c r="D10" s="14" t="s">
         <v>25</v>
@@ -2388,7 +2395,7 @@
     </row>
     <row r="11" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="52"/>
-      <c r="B11" s="118"/>
+      <c r="B11" s="109"/>
       <c r="C11" s="8"/>
       <c r="D11" s="14" t="s">
         <v>27</v>
@@ -2424,7 +2431,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="52"/>
-      <c r="B12" s="118"/>
+      <c r="B12" s="109"/>
       <c r="C12" s="8"/>
       <c r="D12" s="14" t="s">
         <v>29</v>
@@ -2458,7 +2465,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="52"/>
-      <c r="B13" s="118"/>
+      <c r="B13" s="109"/>
       <c r="C13" s="8"/>
       <c r="D13" s="14" t="s">
         <v>30</v>
@@ -2492,7 +2499,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="52"/>
-      <c r="B14" s="118"/>
+      <c r="B14" s="109"/>
       <c r="C14" s="8"/>
       <c r="D14" s="14" t="s">
         <v>31</v>
@@ -2526,7 +2533,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="52"/>
-      <c r="B15" s="118"/>
+      <c r="B15" s="109"/>
       <c r="C15" s="8"/>
       <c r="D15" s="14" t="s">
         <v>32</v>
@@ -2560,7 +2567,7 @@
     </row>
     <row r="16" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="52"/>
-      <c r="B16" s="118"/>
+      <c r="B16" s="109"/>
       <c r="C16" s="8"/>
       <c r="D16" s="14" t="s">
         <v>33</v>
@@ -2594,7 +2601,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="52"/>
-      <c r="B17" s="118"/>
+      <c r="B17" s="109"/>
       <c r="C17" s="8"/>
       <c r="D17" s="14" t="s">
         <v>34</v>
@@ -2627,7 +2634,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="52"/>
-      <c r="B18" s="118"/>
+      <c r="B18" s="109"/>
       <c r="C18" s="8"/>
       <c r="D18" s="14" t="s">
         <v>35</v>
@@ -2661,7 +2668,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="52"/>
-      <c r="B19" s="118"/>
+      <c r="B19" s="109"/>
       <c r="C19" s="8"/>
       <c r="D19" s="14" t="s">
         <v>36</v>
@@ -2695,7 +2702,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="52"/>
-      <c r="B20" s="118"/>
+      <c r="B20" s="109"/>
       <c r="C20" s="8"/>
       <c r="D20" s="14" t="s">
         <v>37</v>
@@ -2729,7 +2736,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="52"/>
-      <c r="B21" s="118"/>
+      <c r="B21" s="109"/>
       <c r="C21" s="8"/>
       <c r="D21" s="14" t="s">
         <v>38</v>
@@ -2763,7 +2770,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="53"/>
-      <c r="B22" s="119"/>
+      <c r="B22" s="110"/>
       <c r="C22" s="56"/>
       <c r="D22" s="14"/>
       <c r="E22" s="16"/>
@@ -3012,138 +3019,138 @@
       <c r="N29" s="99"/>
     </row>
     <row r="30" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A30" s="121">
-        <v>5</v>
-      </c>
-      <c r="B30" s="118" t="s">
+      <c r="A30" s="112">
+        <v>5</v>
+      </c>
+      <c r="B30" s="109" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="105" t="s">
+      <c r="C30" s="118" t="s">
         <v>50</v>
       </c>
       <c r="D30" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="E30" s="105" t="s">
+      <c r="E30" s="118" t="s">
         <v>52</v>
       </c>
-      <c r="F30" s="108"/>
-      <c r="G30" s="110">
-        <v>4</v>
-      </c>
-      <c r="H30" s="115">
-        <v>4</v>
-      </c>
-      <c r="I30" s="110">
+      <c r="F30" s="121"/>
+      <c r="G30" s="104">
+        <v>4</v>
+      </c>
+      <c r="H30" s="125">
+        <v>4</v>
+      </c>
+      <c r="I30" s="104">
         <v>2</v>
       </c>
-      <c r="J30" s="110">
+      <c r="J30" s="104">
         <v>0</v>
       </c>
-      <c r="K30" s="110">
-        <v>3</v>
-      </c>
-      <c r="L30" s="110">
-        <v>4</v>
-      </c>
-      <c r="M30" s="110">
-        <v>3</v>
-      </c>
-      <c r="N30" s="110">
+      <c r="K30" s="104">
+        <v>3</v>
+      </c>
+      <c r="L30" s="104">
+        <v>4</v>
+      </c>
+      <c r="M30" s="104">
+        <v>3</v>
+      </c>
+      <c r="N30" s="104">
         <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="121"/>
-      <c r="B31" s="118"/>
-      <c r="C31" s="105"/>
+      <c r="A31" s="112"/>
+      <c r="B31" s="109"/>
+      <c r="C31" s="118"/>
       <c r="D31" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E31" s="105"/>
-      <c r="F31" s="108"/>
-      <c r="G31" s="110"/>
-      <c r="H31" s="116"/>
-      <c r="I31" s="110"/>
-      <c r="J31" s="110"/>
-      <c r="K31" s="110"/>
-      <c r="L31" s="110"/>
-      <c r="M31" s="110"/>
-      <c r="N31" s="110"/>
+      <c r="E31" s="118"/>
+      <c r="F31" s="121"/>
+      <c r="G31" s="104"/>
+      <c r="H31" s="126"/>
+      <c r="I31" s="104"/>
+      <c r="J31" s="104"/>
+      <c r="K31" s="104"/>
+      <c r="L31" s="104"/>
+      <c r="M31" s="104"/>
+      <c r="N31" s="104"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="121"/>
-      <c r="B32" s="118"/>
-      <c r="C32" s="105"/>
+      <c r="A32" s="112"/>
+      <c r="B32" s="109"/>
+      <c r="C32" s="118"/>
       <c r="D32" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E32" s="105"/>
-      <c r="F32" s="108"/>
-      <c r="G32" s="110"/>
-      <c r="H32" s="116"/>
-      <c r="I32" s="110"/>
-      <c r="J32" s="110"/>
-      <c r="K32" s="110"/>
-      <c r="L32" s="110"/>
-      <c r="M32" s="110"/>
-      <c r="N32" s="110"/>
+      <c r="E32" s="118"/>
+      <c r="F32" s="121"/>
+      <c r="G32" s="104"/>
+      <c r="H32" s="126"/>
+      <c r="I32" s="104"/>
+      <c r="J32" s="104"/>
+      <c r="K32" s="104"/>
+      <c r="L32" s="104"/>
+      <c r="M32" s="104"/>
+      <c r="N32" s="104"/>
     </row>
     <row r="33" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="121"/>
-      <c r="B33" s="118"/>
-      <c r="C33" s="105"/>
+      <c r="A33" s="112"/>
+      <c r="B33" s="109"/>
+      <c r="C33" s="118"/>
       <c r="D33" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E33" s="105"/>
-      <c r="F33" s="108"/>
-      <c r="G33" s="110"/>
-      <c r="H33" s="116"/>
-      <c r="I33" s="110"/>
-      <c r="J33" s="110"/>
-      <c r="K33" s="110"/>
-      <c r="L33" s="110"/>
-      <c r="M33" s="110"/>
-      <c r="N33" s="110"/>
+      <c r="E33" s="118"/>
+      <c r="F33" s="121"/>
+      <c r="G33" s="104"/>
+      <c r="H33" s="126"/>
+      <c r="I33" s="104"/>
+      <c r="J33" s="104"/>
+      <c r="K33" s="104"/>
+      <c r="L33" s="104"/>
+      <c r="M33" s="104"/>
+      <c r="N33" s="104"/>
     </row>
     <row r="34" spans="1:14" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="121"/>
-      <c r="B34" s="118"/>
-      <c r="C34" s="105"/>
+      <c r="A34" s="112"/>
+      <c r="B34" s="109"/>
+      <c r="C34" s="118"/>
       <c r="D34" s="9"/>
-      <c r="E34" s="105"/>
-      <c r="F34" s="108"/>
-      <c r="G34" s="110"/>
-      <c r="H34" s="116"/>
-      <c r="I34" s="110"/>
-      <c r="J34" s="110"/>
-      <c r="K34" s="110"/>
-      <c r="L34" s="110"/>
-      <c r="M34" s="110"/>
-      <c r="N34" s="110"/>
+      <c r="E34" s="118"/>
+      <c r="F34" s="121"/>
+      <c r="G34" s="104"/>
+      <c r="H34" s="126"/>
+      <c r="I34" s="104"/>
+      <c r="J34" s="104"/>
+      <c r="K34" s="104"/>
+      <c r="L34" s="104"/>
+      <c r="M34" s="104"/>
+      <c r="N34" s="104"/>
     </row>
     <row r="35" spans="1:14" ht="63" x14ac:dyDescent="0.25">
-      <c r="A35" s="121"/>
-      <c r="B35" s="118"/>
-      <c r="C35" s="105"/>
+      <c r="A35" s="112"/>
+      <c r="B35" s="109"/>
+      <c r="C35" s="118"/>
       <c r="D35" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="E35" s="106"/>
-      <c r="F35" s="109"/>
-      <c r="G35" s="111"/>
-      <c r="H35" s="117"/>
-      <c r="I35" s="111"/>
-      <c r="J35" s="111"/>
-      <c r="K35" s="111"/>
-      <c r="L35" s="111"/>
-      <c r="M35" s="111"/>
-      <c r="N35" s="111"/>
+      <c r="E35" s="119"/>
+      <c r="F35" s="122"/>
+      <c r="G35" s="105"/>
+      <c r="H35" s="127"/>
+      <c r="I35" s="105"/>
+      <c r="J35" s="105"/>
+      <c r="K35" s="105"/>
+      <c r="L35" s="105"/>
+      <c r="M35" s="105"/>
+      <c r="N35" s="105"/>
     </row>
     <row r="36" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A36" s="52"/>
-      <c r="B36" s="118"/>
+      <c r="B36" s="109"/>
       <c r="C36" s="8"/>
       <c r="D36" s="12" t="s">
         <v>57</v>
@@ -3177,7 +3184,7 @@
     </row>
     <row r="37" spans="1:14" ht="63" x14ac:dyDescent="0.25">
       <c r="A37" s="53"/>
-      <c r="B37" s="119"/>
+      <c r="B37" s="110"/>
       <c r="C37" s="56"/>
       <c r="D37" s="40" t="s">
         <v>58</v>
@@ -3458,13 +3465,13 @@
       <c r="M45" s="13"/>
     </row>
     <row r="46" spans="1:14" s="4" customFormat="1" ht="95.25" x14ac:dyDescent="0.3">
-      <c r="A46" s="121">
+      <c r="A46" s="112">
         <v>9</v>
       </c>
-      <c r="B46" s="124" t="s">
+      <c r="B46" s="115" t="s">
         <v>71</v>
       </c>
-      <c r="C46" s="105" t="s">
+      <c r="C46" s="118" t="s">
         <v>72</v>
       </c>
       <c r="D46" s="60" t="s">
@@ -3473,157 +3480,157 @@
       <c r="E46" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="F46" s="108"/>
-      <c r="G46" s="110">
-        <v>4</v>
-      </c>
-      <c r="H46" s="115">
-        <v>4</v>
-      </c>
-      <c r="I46" s="110">
-        <v>5</v>
-      </c>
-      <c r="J46" s="114">
-        <v>5</v>
-      </c>
-      <c r="K46" s="110">
+      <c r="F46" s="121"/>
+      <c r="G46" s="104">
+        <v>4</v>
+      </c>
+      <c r="H46" s="125">
+        <v>4</v>
+      </c>
+      <c r="I46" s="104">
+        <v>5</v>
+      </c>
+      <c r="J46" s="108">
+        <v>5</v>
+      </c>
+      <c r="K46" s="104">
         <v>2</v>
       </c>
-      <c r="L46" s="110">
-        <v>3</v>
-      </c>
-      <c r="M46" s="110">
-        <v>4</v>
-      </c>
-      <c r="N46" s="126">
+      <c r="L46" s="104">
+        <v>3</v>
+      </c>
+      <c r="M46" s="104">
+        <v>4</v>
+      </c>
+      <c r="N46" s="106">
         <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="157.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="121"/>
-      <c r="B47" s="124"/>
-      <c r="C47" s="105"/>
+      <c r="A47" s="112"/>
+      <c r="B47" s="115"/>
+      <c r="C47" s="118"/>
       <c r="D47" s="9" t="s">
         <v>75</v>
       </c>
       <c r="E47" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="F47" s="108"/>
-      <c r="G47" s="110"/>
-      <c r="H47" s="116"/>
-      <c r="I47" s="110"/>
-      <c r="J47" s="110"/>
-      <c r="K47" s="110"/>
-      <c r="L47" s="110"/>
-      <c r="M47" s="110"/>
-      <c r="N47" s="126"/>
+      <c r="F47" s="121"/>
+      <c r="G47" s="104"/>
+      <c r="H47" s="126"/>
+      <c r="I47" s="104"/>
+      <c r="J47" s="104"/>
+      <c r="K47" s="104"/>
+      <c r="L47" s="104"/>
+      <c r="M47" s="104"/>
+      <c r="N47" s="106"/>
     </row>
     <row r="48" spans="1:14" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A48" s="121"/>
-      <c r="B48" s="124"/>
-      <c r="C48" s="105"/>
+      <c r="A48" s="112"/>
+      <c r="B48" s="115"/>
+      <c r="C48" s="118"/>
       <c r="D48" s="9" t="s">
         <v>77</v>
       </c>
       <c r="E48" s="17"/>
-      <c r="F48" s="108"/>
-      <c r="G48" s="110"/>
-      <c r="H48" s="116"/>
-      <c r="I48" s="110"/>
-      <c r="J48" s="110"/>
-      <c r="K48" s="110"/>
-      <c r="L48" s="110"/>
-      <c r="M48" s="110"/>
-      <c r="N48" s="126"/>
+      <c r="F48" s="121"/>
+      <c r="G48" s="104"/>
+      <c r="H48" s="126"/>
+      <c r="I48" s="104"/>
+      <c r="J48" s="104"/>
+      <c r="K48" s="104"/>
+      <c r="L48" s="104"/>
+      <c r="M48" s="104"/>
+      <c r="N48" s="106"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="121"/>
-      <c r="B49" s="124"/>
-      <c r="C49" s="105"/>
+      <c r="A49" s="112"/>
+      <c r="B49" s="115"/>
+      <c r="C49" s="118"/>
       <c r="D49" s="10"/>
       <c r="E49" s="17"/>
-      <c r="F49" s="108"/>
-      <c r="G49" s="110"/>
-      <c r="H49" s="116"/>
-      <c r="I49" s="110"/>
-      <c r="J49" s="110"/>
-      <c r="K49" s="110"/>
-      <c r="L49" s="110"/>
-      <c r="M49" s="110"/>
-      <c r="N49" s="126"/>
+      <c r="F49" s="121"/>
+      <c r="G49" s="104"/>
+      <c r="H49" s="126"/>
+      <c r="I49" s="104"/>
+      <c r="J49" s="104"/>
+      <c r="K49" s="104"/>
+      <c r="L49" s="104"/>
+      <c r="M49" s="104"/>
+      <c r="N49" s="106"/>
     </row>
     <row r="50" spans="1:14" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A50" s="121"/>
-      <c r="B50" s="124"/>
-      <c r="C50" s="105"/>
+      <c r="A50" s="112"/>
+      <c r="B50" s="115"/>
+      <c r="C50" s="118"/>
       <c r="D50" s="9" t="s">
         <v>78</v>
       </c>
       <c r="E50" s="17"/>
-      <c r="F50" s="108"/>
-      <c r="G50" s="110"/>
-      <c r="H50" s="116"/>
-      <c r="I50" s="110"/>
-      <c r="J50" s="110"/>
-      <c r="K50" s="110"/>
-      <c r="L50" s="110"/>
-      <c r="M50" s="110"/>
-      <c r="N50" s="126"/>
+      <c r="F50" s="121"/>
+      <c r="G50" s="104"/>
+      <c r="H50" s="126"/>
+      <c r="I50" s="104"/>
+      <c r="J50" s="104"/>
+      <c r="K50" s="104"/>
+      <c r="L50" s="104"/>
+      <c r="M50" s="104"/>
+      <c r="N50" s="106"/>
     </row>
     <row r="51" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="121"/>
-      <c r="B51" s="124"/>
-      <c r="C51" s="105"/>
+      <c r="A51" s="112"/>
+      <c r="B51" s="115"/>
+      <c r="C51" s="118"/>
       <c r="D51" s="9" t="s">
         <v>79</v>
       </c>
       <c r="E51" s="17"/>
-      <c r="F51" s="108"/>
-      <c r="G51" s="110"/>
-      <c r="H51" s="116"/>
-      <c r="I51" s="110"/>
-      <c r="J51" s="110"/>
-      <c r="K51" s="110"/>
-      <c r="L51" s="110"/>
-      <c r="M51" s="110"/>
-      <c r="N51" s="126"/>
+      <c r="F51" s="121"/>
+      <c r="G51" s="104"/>
+      <c r="H51" s="126"/>
+      <c r="I51" s="104"/>
+      <c r="J51" s="104"/>
+      <c r="K51" s="104"/>
+      <c r="L51" s="104"/>
+      <c r="M51" s="104"/>
+      <c r="N51" s="106"/>
     </row>
     <row r="52" spans="1:14" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A52" s="121"/>
-      <c r="B52" s="124"/>
-      <c r="C52" s="105"/>
+      <c r="A52" s="112"/>
+      <c r="B52" s="115"/>
+      <c r="C52" s="118"/>
       <c r="D52" s="9" t="s">
         <v>80</v>
       </c>
       <c r="E52" s="17"/>
-      <c r="F52" s="108"/>
-      <c r="G52" s="110"/>
-      <c r="H52" s="116"/>
-      <c r="I52" s="110"/>
-      <c r="J52" s="110"/>
-      <c r="K52" s="110"/>
-      <c r="L52" s="110"/>
-      <c r="M52" s="110"/>
-      <c r="N52" s="126"/>
+      <c r="F52" s="121"/>
+      <c r="G52" s="104"/>
+      <c r="H52" s="126"/>
+      <c r="I52" s="104"/>
+      <c r="J52" s="104"/>
+      <c r="K52" s="104"/>
+      <c r="L52" s="104"/>
+      <c r="M52" s="104"/>
+      <c r="N52" s="106"/>
     </row>
     <row r="53" spans="1:14" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="122"/>
-      <c r="B53" s="125"/>
-      <c r="C53" s="106"/>
+      <c r="A53" s="113"/>
+      <c r="B53" s="116"/>
+      <c r="C53" s="119"/>
       <c r="D53" s="60" t="s">
         <v>81</v>
       </c>
       <c r="E53" s="17"/>
-      <c r="F53" s="109"/>
-      <c r="G53" s="111"/>
-      <c r="H53" s="117"/>
-      <c r="I53" s="111"/>
-      <c r="J53" s="111"/>
-      <c r="K53" s="111"/>
-      <c r="L53" s="111"/>
-      <c r="M53" s="111"/>
-      <c r="N53" s="127"/>
+      <c r="F53" s="122"/>
+      <c r="G53" s="105"/>
+      <c r="H53" s="127"/>
+      <c r="I53" s="105"/>
+      <c r="J53" s="105"/>
+      <c r="K53" s="105"/>
+      <c r="L53" s="105"/>
+      <c r="M53" s="105"/>
+      <c r="N53" s="107"/>
     </row>
     <row r="54" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A54" s="43"/>
@@ -3668,100 +3675,100 @@
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" s="120">
+      <c r="A55" s="111">
         <v>10</v>
       </c>
-      <c r="B55" s="123" t="s">
+      <c r="B55" s="114" t="s">
         <v>82</v>
       </c>
-      <c r="C55" s="104" t="s">
+      <c r="C55" s="117" t="s">
         <v>83</v>
       </c>
       <c r="D55" s="60" t="s">
         <v>84</v>
       </c>
-      <c r="E55" s="104" t="s">
+      <c r="E55" s="117" t="s">
         <v>85</v>
       </c>
-      <c r="F55" s="107"/>
-      <c r="G55" s="114">
-        <v>4</v>
-      </c>
-      <c r="H55" s="114">
-        <v>4</v>
-      </c>
-      <c r="I55" s="114">
+      <c r="F55" s="120"/>
+      <c r="G55" s="108">
+        <v>4</v>
+      </c>
+      <c r="H55" s="108">
+        <v>4</v>
+      </c>
+      <c r="I55" s="108">
         <v>3</v>
       </c>
       <c r="J55" s="97"/>
-      <c r="K55" s="114">
-        <v>3</v>
-      </c>
-      <c r="L55" s="114">
-        <v>5</v>
-      </c>
-      <c r="M55" s="114">
+      <c r="K55" s="108">
+        <v>3</v>
+      </c>
+      <c r="L55" s="108">
+        <v>5</v>
+      </c>
+      <c r="M55" s="108">
         <v>2</v>
       </c>
-      <c r="N55" s="114">
+      <c r="N55" s="108">
         <v>4.5</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" s="121"/>
-      <c r="B56" s="124"/>
-      <c r="C56" s="105"/>
+      <c r="A56" s="112"/>
+      <c r="B56" s="115"/>
+      <c r="C56" s="118"/>
       <c r="D56" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="E56" s="105"/>
-      <c r="F56" s="108"/>
-      <c r="G56" s="110"/>
-      <c r="H56" s="110"/>
-      <c r="I56" s="110"/>
+      <c r="E56" s="118"/>
+      <c r="F56" s="121"/>
+      <c r="G56" s="104"/>
+      <c r="H56" s="104"/>
+      <c r="I56" s="104"/>
       <c r="J56" s="94"/>
-      <c r="K56" s="110"/>
-      <c r="L56" s="110"/>
-      <c r="M56" s="110"/>
-      <c r="N56" s="110"/>
+      <c r="K56" s="104"/>
+      <c r="L56" s="104"/>
+      <c r="M56" s="104"/>
+      <c r="N56" s="104"/>
     </row>
     <row r="57" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A57" s="121"/>
-      <c r="B57" s="124"/>
-      <c r="C57" s="105"/>
+      <c r="A57" s="112"/>
+      <c r="B57" s="115"/>
+      <c r="C57" s="118"/>
       <c r="D57" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="E57" s="105"/>
-      <c r="F57" s="108"/>
-      <c r="G57" s="110"/>
-      <c r="H57" s="110"/>
-      <c r="I57" s="110"/>
+      <c r="E57" s="118"/>
+      <c r="F57" s="121"/>
+      <c r="G57" s="104"/>
+      <c r="H57" s="104"/>
+      <c r="I57" s="104"/>
       <c r="J57" s="94"/>
-      <c r="K57" s="110"/>
-      <c r="L57" s="110"/>
-      <c r="M57" s="110"/>
-      <c r="N57" s="110"/>
+      <c r="K57" s="104"/>
+      <c r="L57" s="104"/>
+      <c r="M57" s="104"/>
+      <c r="N57" s="104"/>
     </row>
     <row r="58" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A58" s="122"/>
-      <c r="B58" s="125"/>
-      <c r="C58" s="106"/>
+      <c r="A58" s="113"/>
+      <c r="B58" s="116"/>
+      <c r="C58" s="119"/>
       <c r="D58" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="E58" s="106"/>
-      <c r="F58" s="109"/>
-      <c r="G58" s="111"/>
-      <c r="H58" s="111"/>
-      <c r="I58" s="111"/>
+      <c r="E58" s="119"/>
+      <c r="F58" s="122"/>
+      <c r="G58" s="105"/>
+      <c r="H58" s="105"/>
+      <c r="I58" s="105"/>
       <c r="J58" s="95">
         <v>4.2</v>
       </c>
-      <c r="K58" s="111"/>
-      <c r="L58" s="111"/>
-      <c r="M58" s="111"/>
-      <c r="N58" s="111"/>
+      <c r="K58" s="105"/>
+      <c r="L58" s="105"/>
+      <c r="M58" s="105"/>
+      <c r="N58" s="105"/>
     </row>
     <row r="59" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A59" s="67"/>
@@ -3821,13 +3828,13 @@
       <c r="M60" s="13"/>
     </row>
     <row r="61" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A61" s="112" t="s">
+      <c r="A61" s="123" t="s">
         <v>89</v>
       </c>
-      <c r="B61" s="113"/>
-      <c r="C61" s="113"/>
-      <c r="D61" s="113"/>
-      <c r="E61" s="113"/>
+      <c r="B61" s="124"/>
+      <c r="C61" s="124"/>
+      <c r="D61" s="124"/>
+      <c r="E61" s="124"/>
       <c r="F61" s="73">
         <f>SUM(F59,F54,F43,F39,F25,F23)</f>
         <v>100</v>
@@ -5019,32 +5026,6 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="N30:N35"/>
-    <mergeCell ref="N46:N53"/>
-    <mergeCell ref="N55:N58"/>
-    <mergeCell ref="K30:K35"/>
-    <mergeCell ref="L30:L35"/>
-    <mergeCell ref="M30:M35"/>
-    <mergeCell ref="J30:J35"/>
-    <mergeCell ref="M55:M58"/>
-    <mergeCell ref="I46:I53"/>
-    <mergeCell ref="K46:K53"/>
-    <mergeCell ref="L46:L53"/>
-    <mergeCell ref="M46:M53"/>
-    <mergeCell ref="K55:K58"/>
-    <mergeCell ref="L55:L58"/>
-    <mergeCell ref="I55:I58"/>
-    <mergeCell ref="J46:J53"/>
-    <mergeCell ref="B3:B22"/>
-    <mergeCell ref="B30:B37"/>
-    <mergeCell ref="A55:A58"/>
-    <mergeCell ref="B55:B58"/>
-    <mergeCell ref="C55:C58"/>
-    <mergeCell ref="A30:A35"/>
-    <mergeCell ref="C30:C35"/>
-    <mergeCell ref="A46:A53"/>
-    <mergeCell ref="B46:B53"/>
-    <mergeCell ref="C46:C53"/>
     <mergeCell ref="E55:E58"/>
     <mergeCell ref="F55:F58"/>
     <mergeCell ref="I30:I35"/>
@@ -5058,6 +5039,32 @@
     <mergeCell ref="H30:H35"/>
     <mergeCell ref="H46:H53"/>
     <mergeCell ref="H55:H58"/>
+    <mergeCell ref="B3:B22"/>
+    <mergeCell ref="B30:B37"/>
+    <mergeCell ref="A55:A58"/>
+    <mergeCell ref="B55:B58"/>
+    <mergeCell ref="C55:C58"/>
+    <mergeCell ref="A30:A35"/>
+    <mergeCell ref="C30:C35"/>
+    <mergeCell ref="A46:A53"/>
+    <mergeCell ref="B46:B53"/>
+    <mergeCell ref="C46:C53"/>
+    <mergeCell ref="J30:J35"/>
+    <mergeCell ref="M55:M58"/>
+    <mergeCell ref="I46:I53"/>
+    <mergeCell ref="K46:K53"/>
+    <mergeCell ref="L46:L53"/>
+    <mergeCell ref="M46:M53"/>
+    <mergeCell ref="K55:K58"/>
+    <mergeCell ref="L55:L58"/>
+    <mergeCell ref="I55:I58"/>
+    <mergeCell ref="J46:J53"/>
+    <mergeCell ref="N30:N35"/>
+    <mergeCell ref="N46:N53"/>
+    <mergeCell ref="N55:N58"/>
+    <mergeCell ref="K30:K35"/>
+    <mergeCell ref="L30:L35"/>
+    <mergeCell ref="M30:M35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
@@ -5074,7 +5081,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5157,10 +5164,10 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="121">
+      <c r="A3" s="112">
         <v>1</v>
       </c>
-      <c r="B3" s="118" t="s">
+      <c r="B3" s="109" t="s">
         <v>90</v>
       </c>
       <c r="C3" s="55"/>
@@ -5195,8 +5202,8 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="121"/>
-      <c r="B4" s="118"/>
+      <c r="A4" s="112"/>
+      <c r="B4" s="109"/>
       <c r="C4" s="8"/>
       <c r="D4" s="100" t="s">
         <v>92</v>
@@ -5229,8 +5236,8 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="121"/>
-      <c r="B5" s="118"/>
+      <c r="A5" s="112"/>
+      <c r="B5" s="109"/>
       <c r="C5" s="8"/>
       <c r="D5" s="100" t="s">
         <v>93</v>
@@ -5263,8 +5270,8 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="121"/>
-      <c r="B6" s="118"/>
+      <c r="A6" s="112"/>
+      <c r="B6" s="109"/>
       <c r="C6" s="55"/>
       <c r="D6" s="92"/>
       <c r="E6" s="89"/>
@@ -5345,10 +5352,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="121">
+      <c r="A8" s="112">
         <v>2</v>
       </c>
-      <c r="B8" s="118" t="s">
+      <c r="B8" s="109" t="s">
         <v>94</v>
       </c>
       <c r="C8" s="55"/>
@@ -5383,8 +5390,8 @@
       </c>
     </row>
     <row r="9" spans="1:14" s="4" customFormat="1" ht="47.25" x14ac:dyDescent="0.3">
-      <c r="A9" s="121"/>
-      <c r="B9" s="118"/>
+      <c r="A9" s="112"/>
+      <c r="B9" s="109"/>
       <c r="C9" s="8"/>
       <c r="D9" s="90" t="s">
         <v>96</v>
@@ -5417,8 +5424,8 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="121"/>
-      <c r="B10" s="118"/>
+      <c r="A10" s="112"/>
+      <c r="B10" s="109"/>
       <c r="C10" s="8"/>
       <c r="D10" s="93" t="s">
         <v>97</v>
@@ -5451,8 +5458,8 @@
       </c>
     </row>
     <row r="11" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="121"/>
-      <c r="B11" s="118"/>
+      <c r="A11" s="112"/>
+      <c r="B11" s="109"/>
       <c r="C11" s="55"/>
       <c r="D11" s="50"/>
       <c r="E11" s="42"/>
@@ -5497,39 +5504,39 @@
       <c r="D12" s="45"/>
       <c r="E12" s="45"/>
       <c r="F12" s="46">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="G12" s="91">
         <f>G11 * F12 / 100</f>
-        <v>1.05</v>
+        <v>1.75</v>
       </c>
       <c r="H12" s="91">
         <f>H11 * F12 / 100</f>
-        <v>1.2</v>
+        <v>2</v>
       </c>
       <c r="I12" s="26">
         <f>I11 * F12 / 100</f>
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="J12" s="26">
         <f>J11 * F12 / 100</f>
-        <v>1</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="K12" s="26">
         <f>K11 * F12 / 100</f>
-        <v>1.35</v>
+        <v>2.25</v>
       </c>
       <c r="L12" s="26">
         <f>L11 * F12 / 100</f>
-        <v>0.75</v>
+        <v>1.25</v>
       </c>
       <c r="M12" s="27">
         <f>M11 * F12 / 100</f>
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="N12" s="27">
         <f>N11 * F12 / 100</f>
-        <v>0.5</v>
+        <v>0.83333333333333348</v>
       </c>
     </row>
     <row r="13" spans="1:14" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
@@ -5571,37 +5578,37 @@
       <c r="D14" s="45"/>
       <c r="E14" s="45"/>
       <c r="F14" s="46">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G14" s="26">
         <f>G13 * F14 / 100</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="26">
         <v>1</v>
       </c>
       <c r="I14" s="26">
         <f>I13 * F14 / 100</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" s="26">
         <v>1</v>
       </c>
       <c r="K14" s="26">
         <f>K13 * F14 / 100</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L14" s="26">
         <f>L13 * F14 / 100</f>
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="M14" s="27">
         <f>M13 * F14 / 100</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N14" s="27">
         <f>N13 * F14 / 100</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -5633,27 +5640,27 @@
       </c>
       <c r="G16" s="29">
         <f t="shared" ref="G16:N16" si="1">ROUNDUP(SUM(G7,G12,G14), 2)</f>
-        <v>3.8</v>
+        <v>3.5</v>
       </c>
       <c r="H16" s="29">
         <f t="shared" si="1"/>
-        <v>3.95</v>
+        <v>4.75</v>
       </c>
       <c r="I16" s="29">
         <f t="shared" si="1"/>
-        <v>2.85</v>
+        <v>2.25</v>
       </c>
       <c r="J16" s="29">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>4.67</v>
       </c>
       <c r="K16" s="29">
         <f t="shared" si="1"/>
-        <v>4.0999999999999996</v>
+        <v>4</v>
       </c>
       <c r="L16" s="29">
         <f t="shared" si="1"/>
-        <v>1.95</v>
+        <v>2.25</v>
       </c>
       <c r="M16" s="29">
         <f t="shared" si="1"/>
@@ -5661,7 +5668,7 @@
       </c>
       <c r="N16" s="29">
         <f t="shared" si="1"/>
-        <v>3.75</v>
+        <v>3.09</v>
       </c>
     </row>
     <row r="20" spans="4:4" x14ac:dyDescent="0.25">
@@ -5689,10 +5696,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5715,116 +5722,116 @@
     </row>
     <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="37">
+        <f>Adoption!I16</f>
+        <v>2.25</v>
+      </c>
+      <c r="C2" s="37">
+        <f>Capabilities!I61</f>
+        <v>3.4699999999999998</v>
+      </c>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+    </row>
+    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A3" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="37">
+        <v>4</v>
+      </c>
+      <c r="C3" s="37">
+        <v>3.75</v>
+      </c>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+    </row>
+    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A4" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="37">
+      <c r="B4" s="37">
         <f>Adoption!G16</f>
-        <v>3.8</v>
-      </c>
-      <c r="C2" s="37">
+        <v>3.5</v>
+      </c>
+      <c r="C4" s="37">
         <f>Capabilities!G61</f>
         <v>4.0999999999999996</v>
       </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-    </row>
-    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="36" t="s">
-        <v>102</v>
-      </c>
-      <c r="B3" s="37">
-        <v>3.95</v>
-      </c>
-      <c r="C3" s="37">
-        <v>4.18</v>
-      </c>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-    </row>
-    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="36" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="37">
-        <f>Adoption!I16</f>
-        <v>2.85</v>
-      </c>
-      <c r="C4" s="37">
-        <f>Capabilities!I61</f>
-        <v>3.4699999999999998</v>
-      </c>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
     </row>
     <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="36" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B5" s="37">
-        <v>4</v>
+        <v>3.95</v>
       </c>
       <c r="C5" s="37">
-        <v>3.75</v>
+        <v>4.18</v>
       </c>
       <c r="D5" s="34"/>
       <c r="E5" s="34"/>
     </row>
     <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="49">
+        <f>Adoption!N16</f>
+        <v>3.09</v>
+      </c>
+      <c r="C6" s="37">
+        <f>Capabilities!N61</f>
+        <v>4.42</v>
+      </c>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+    </row>
+    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A7" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="49">
+      <c r="B7" s="49">
         <f>Adoption!K16</f>
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="C6" s="37">
+        <v>4</v>
+      </c>
+      <c r="C7" s="37">
         <f>Capabilities!K61</f>
         <v>3.23</v>
       </c>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-    </row>
-    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A7" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="49">
-        <f>Adoption!L16</f>
-        <v>1.95</v>
-      </c>
-      <c r="C7" s="37">
-        <f>Capabilities!L61</f>
-        <v>4</v>
-      </c>
       <c r="D7" s="34"/>
       <c r="E7" s="34"/>
     </row>
     <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="49">
+        <f>Adoption!L16</f>
+        <v>2.25</v>
+      </c>
+      <c r="C8" s="37">
+        <f>Capabilities!L61</f>
+        <v>4</v>
+      </c>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+    </row>
+    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A9" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="49">
+      <c r="B9" s="49">
         <f>Adoption!M16</f>
         <v>4.25</v>
       </c>
-      <c r="C8" s="37">
+      <c r="C9" s="37">
         <f>Capabilities!M61</f>
         <v>2.5399999999999996</v>
-      </c>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-    </row>
-    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A9" s="36" t="s">
-        <v>104</v>
-      </c>
-      <c r="B9" s="49">
-        <f>Adoption!N16</f>
-        <v>3.75</v>
-      </c>
-      <c r="C9" s="37">
-        <f>Capabilities!N61</f>
-        <v>4.42</v>
       </c>
       <c r="D9" s="34"/>
       <c r="E9" s="34"/>
@@ -5835,13 +5842,6 @@
       <c r="C10" s="34"/>
       <c r="D10" s="34"/>
       <c r="E10" s="34"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>